<commit_message>
Fix follow-up log and qualitative export
Export follow-up log including all contact details
Use passphrase to decrypt encrypted qualitative data
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update RCT monitoring report
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="521">
   <si>
     <t>old</t>
   </si>
@@ -1575,6 +1575,18 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>consent-district</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>consent-facility</t>
+  </si>
+  <si>
+    <t>facility</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1699,6 +1711,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1980,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3263,80 +3278,80 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="4">
+        <v>1</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B58" s="11" t="s">
         <v>516</v>
       </c>
-      <c r="C56" s="2">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4">
-        <v>1</v>
-      </c>
-      <c r="F56" s="4">
-        <v>0</v>
-      </c>
-      <c r="G56" s="11" t="s">
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="11" t="s">
         <v>515</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C57" s="2">
-        <v>0</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0</v>
-      </c>
-      <c r="E57" s="4">
-        <v>1</v>
-      </c>
-      <c r="F57" s="3">
-        <v>0</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="2">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2">
-        <v>0</v>
-      </c>
-      <c r="E58" s="4">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
-        <v>0</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -3351,15 +3366,15 @@
         <v>0</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C60" s="2">
         <v>0</v>
@@ -3374,15 +3389,15 @@
         <v>0</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
@@ -3397,15 +3412,15 @@
         <v>0</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C62" s="2">
         <v>0</v>
@@ -3420,15 +3435,15 @@
         <v>0</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C63" s="2">
         <v>0</v>
@@ -3443,15 +3458,15 @@
         <v>0</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C64" s="2">
         <v>0</v>
@@ -3466,15 +3481,15 @@
         <v>0</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -3489,15 +3504,15 @@
         <v>0</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
@@ -3512,15 +3527,15 @@
         <v>0</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
@@ -3535,15 +3550,15 @@
         <v>0</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C68" s="2">
         <v>0</v>
@@ -3558,15 +3573,15 @@
         <v>0</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -3581,15 +3596,15 @@
         <v>0</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
@@ -3604,15 +3619,15 @@
         <v>0</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C71" s="2">
         <v>0</v>
@@ -3627,15 +3642,15 @@
         <v>0</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C72" s="2">
         <v>0</v>
@@ -3650,15 +3665,15 @@
         <v>0</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -3673,15 +3688,15 @@
         <v>0</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -3696,15 +3711,15 @@
         <v>0</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -3719,15 +3734,15 @@
         <v>0</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -3742,15 +3757,15 @@
         <v>0</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -3765,15 +3780,15 @@
         <v>0</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -3788,15 +3803,15 @@
         <v>0</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -3811,15 +3826,15 @@
         <v>0</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -3834,15 +3849,15 @@
         <v>0</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
@@ -3857,15 +3872,15 @@
         <v>0</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C82" s="2">
         <v>0</v>
@@ -3880,15 +3895,15 @@
         <v>0</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -3903,15 +3918,15 @@
         <v>0</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C84" s="2">
         <v>0</v>
@@ -3926,84 +3941,84 @@
         <v>0</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
+      <c r="E86" s="4">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B87" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="2">
-        <v>0</v>
-      </c>
-      <c r="D85" s="2">
-        <v>0</v>
-      </c>
-      <c r="E85" s="4">
-        <v>1</v>
-      </c>
-      <c r="F85" s="3">
-        <v>0</v>
-      </c>
-      <c r="G85" s="13" t="s">
+      <c r="C87" s="2">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
+      <c r="E87" s="4">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="G87" s="13" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="2">
-        <v>0</v>
-      </c>
-      <c r="D86" s="2">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2">
-        <v>1</v>
-      </c>
-      <c r="F86" s="3">
-        <v>1</v>
-      </c>
-      <c r="G86" s="17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C87" s="2">
-        <v>0</v>
-      </c>
-      <c r="D87" s="2">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-      <c r="F87" s="3">
-        <v>1</v>
-      </c>
-      <c r="G87" s="17" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C88" s="2">
         <v>0</v>
@@ -4018,15 +4033,15 @@
         <v>1</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C89" s="2">
         <v>0</v>
@@ -4041,15 +4056,15 @@
         <v>1</v>
       </c>
       <c r="G89" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C90" s="2">
         <v>0</v>
@@ -4064,15 +4079,15 @@
         <v>1</v>
       </c>
       <c r="G90" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C91" s="2">
         <v>0</v>
@@ -4087,15 +4102,15 @@
         <v>1</v>
       </c>
       <c r="G91" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C92" s="2">
         <v>0</v>
@@ -4110,15 +4125,15 @@
         <v>1</v>
       </c>
       <c r="G92" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -4133,15 +4148,15 @@
         <v>1</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -4156,15 +4171,15 @@
         <v>1</v>
       </c>
       <c r="G94" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C95" s="2">
         <v>0</v>
@@ -4179,15 +4194,15 @@
         <v>1</v>
       </c>
       <c r="G95" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C96" s="2">
         <v>0</v>
@@ -4202,15 +4217,15 @@
         <v>1</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -4225,15 +4240,15 @@
         <v>1</v>
       </c>
       <c r="G97" s="17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -4248,15 +4263,15 @@
         <v>1</v>
       </c>
       <c r="G98" s="17" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -4271,15 +4286,15 @@
         <v>1</v>
       </c>
       <c r="G99" s="17" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -4294,15 +4309,15 @@
         <v>1</v>
       </c>
       <c r="G100" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -4317,15 +4332,15 @@
         <v>1</v>
       </c>
       <c r="G101" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
@@ -4340,15 +4355,15 @@
         <v>1</v>
       </c>
       <c r="G102" s="17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -4363,15 +4378,15 @@
         <v>1</v>
       </c>
       <c r="G103" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>427</v>
-      </c>
-      <c r="B104" s="15" t="s">
-        <v>99</v>
+        <v>425</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -4386,15 +4401,15 @@
         <v>1</v>
       </c>
       <c r="G104" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="B105" s="15" t="s">
-        <v>100</v>
+        <v>426</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
@@ -4409,15 +4424,15 @@
         <v>1</v>
       </c>
       <c r="G105" s="17" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -4432,15 +4447,15 @@
         <v>1</v>
       </c>
       <c r="G106" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
@@ -4455,15 +4470,15 @@
         <v>1</v>
       </c>
       <c r="G107" s="17" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
@@ -4478,15 +4493,15 @@
         <v>1</v>
       </c>
       <c r="G108" s="17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -4501,15 +4516,15 @@
         <v>1</v>
       </c>
       <c r="G109" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -4524,15 +4539,15 @@
         <v>1</v>
       </c>
       <c r="G110" s="17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -4547,15 +4562,15 @@
         <v>1</v>
       </c>
       <c r="G111" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
@@ -4570,15 +4585,15 @@
         <v>1</v>
       </c>
       <c r="G112" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C113" s="2">
         <v>0</v>
@@ -4593,15 +4608,15 @@
         <v>1</v>
       </c>
       <c r="G113" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -4616,15 +4631,15 @@
         <v>1</v>
       </c>
       <c r="G114" s="17" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -4639,15 +4654,15 @@
         <v>1</v>
       </c>
       <c r="G115" s="17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -4662,15 +4677,15 @@
         <v>1</v>
       </c>
       <c r="G116" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
@@ -4685,15 +4700,15 @@
         <v>1</v>
       </c>
       <c r="G117" s="17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C118" s="2">
         <v>0</v>
@@ -4708,15 +4723,15 @@
         <v>1</v>
       </c>
       <c r="G118" s="17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>442</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>114</v>
+        <v>440</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="C119" s="2">
         <v>0</v>
@@ -4731,15 +4746,15 @@
         <v>1</v>
       </c>
       <c r="G119" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>443</v>
-      </c>
-      <c r="B120" s="14" t="s">
-        <v>115</v>
+        <v>441</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
@@ -4754,15 +4769,15 @@
         <v>1</v>
       </c>
       <c r="G120" s="17" t="s">
-        <v>115</v>
+        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C121" s="2">
         <v>0</v>
@@ -4777,15 +4792,15 @@
         <v>1</v>
       </c>
       <c r="G121" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C122" s="2">
         <v>0</v>
@@ -4800,15 +4815,15 @@
         <v>1</v>
       </c>
       <c r="G122" s="17" t="s">
-        <v>282</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -4823,15 +4838,15 @@
         <v>1</v>
       </c>
       <c r="G123" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -4846,15 +4861,15 @@
         <v>1</v>
       </c>
       <c r="G124" s="17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -4869,15 +4884,15 @@
         <v>1</v>
       </c>
       <c r="G125" s="17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -4892,15 +4907,15 @@
         <v>1</v>
       </c>
       <c r="G126" s="17" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -4915,15 +4930,15 @@
         <v>1</v>
       </c>
       <c r="G127" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -4938,15 +4953,15 @@
         <v>1</v>
       </c>
       <c r="G128" s="17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -4961,15 +4976,15 @@
         <v>1</v>
       </c>
       <c r="G129" s="17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>417</v>
+        <v>451</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -4984,15 +4999,15 @@
         <v>1</v>
       </c>
       <c r="G130" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C131" s="2">
         <v>0</v>
@@ -5007,15 +5022,15 @@
         <v>1</v>
       </c>
       <c r="G131" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>454</v>
+        <v>417</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C132" s="2">
         <v>0</v>
@@ -5030,15 +5045,15 @@
         <v>1</v>
       </c>
       <c r="G132" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
-        <v>455</v>
-      </c>
-      <c r="B133" s="15" t="s">
-        <v>128</v>
+        <v>453</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
@@ -5053,15 +5068,15 @@
         <v>1</v>
       </c>
       <c r="G133" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B134" s="15" t="s">
-        <v>129</v>
+        <v>454</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="C134" s="2">
         <v>0</v>
@@ -5076,15 +5091,15 @@
         <v>1</v>
       </c>
       <c r="G134" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>130</v>
+        <v>455</v>
+      </c>
+      <c r="B135" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -5099,15 +5114,15 @@
         <v>1</v>
       </c>
       <c r="G135" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>458</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>131</v>
+        <v>456</v>
+      </c>
+      <c r="B136" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -5122,15 +5137,15 @@
         <v>1</v>
       </c>
       <c r="G136" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -5145,15 +5160,15 @@
         <v>1</v>
       </c>
       <c r="G137" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5168,15 +5183,15 @@
         <v>1</v>
       </c>
       <c r="G138" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -5191,15 +5206,15 @@
         <v>1</v>
       </c>
       <c r="G139" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C140" s="2">
         <v>0</v>
@@ -5214,15 +5229,15 @@
         <v>1</v>
       </c>
       <c r="G140" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -5237,15 +5252,15 @@
         <v>1</v>
       </c>
       <c r="G141" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -5260,15 +5275,15 @@
         <v>1</v>
       </c>
       <c r="G142" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -5283,15 +5298,15 @@
         <v>1</v>
       </c>
       <c r="G143" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -5306,15 +5321,15 @@
         <v>1</v>
       </c>
       <c r="G144" s="17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -5329,15 +5344,15 @@
         <v>1</v>
       </c>
       <c r="G145" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -5352,15 +5367,15 @@
         <v>1</v>
       </c>
       <c r="G146" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -5375,15 +5390,15 @@
         <v>1</v>
       </c>
       <c r="G147" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -5398,15 +5413,15 @@
         <v>1</v>
       </c>
       <c r="G148" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -5421,15 +5436,15 @@
         <v>1</v>
       </c>
       <c r="G149" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -5444,15 +5459,15 @@
         <v>1</v>
       </c>
       <c r="G150" s="17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -5467,15 +5482,15 @@
         <v>1</v>
       </c>
       <c r="G151" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -5490,15 +5505,15 @@
         <v>1</v>
       </c>
       <c r="G152" s="17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -5513,15 +5528,15 @@
         <v>1</v>
       </c>
       <c r="G153" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -5536,15 +5551,15 @@
         <v>1</v>
       </c>
       <c r="G154" s="17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -5559,15 +5574,15 @@
         <v>1</v>
       </c>
       <c r="G155" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -5582,15 +5597,15 @@
         <v>1</v>
       </c>
       <c r="G156" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -5605,15 +5620,15 @@
         <v>1</v>
       </c>
       <c r="G157" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -5628,15 +5643,15 @@
         <v>1</v>
       </c>
       <c r="G158" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -5651,15 +5666,15 @@
         <v>1</v>
       </c>
       <c r="G159" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -5674,15 +5689,15 @@
         <v>1</v>
       </c>
       <c r="G160" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -5697,15 +5712,15 @@
         <v>1</v>
       </c>
       <c r="G161" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -5720,15 +5735,15 @@
         <v>1</v>
       </c>
       <c r="G162" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -5743,15 +5758,15 @@
         <v>1</v>
       </c>
       <c r="G163" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -5766,15 +5781,15 @@
         <v>1</v>
       </c>
       <c r="G164" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -5789,15 +5804,15 @@
         <v>1</v>
       </c>
       <c r="G165" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -5812,84 +5827,84 @@
         <v>1</v>
       </c>
       <c r="G166" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="B167" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C167" s="2">
+        <v>0</v>
+      </c>
+      <c r="D167" s="2">
+        <v>0</v>
+      </c>
+      <c r="E167" s="2">
+        <v>1</v>
+      </c>
+      <c r="F167" s="3">
+        <v>1</v>
+      </c>
+      <c r="G167" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B168" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C168" s="2">
+        <v>0</v>
+      </c>
+      <c r="D168" s="2">
+        <v>0</v>
+      </c>
+      <c r="E168" s="2">
+        <v>1</v>
+      </c>
+      <c r="F168" s="3">
+        <v>1</v>
+      </c>
+      <c r="G168" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="B167" s="14" t="s">
+      <c r="B169" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C167" s="2">
-        <v>0</v>
-      </c>
-      <c r="D167" s="2">
-        <v>0</v>
-      </c>
-      <c r="E167" s="2">
-        <v>1</v>
-      </c>
-      <c r="F167" s="3">
-        <v>1</v>
-      </c>
-      <c r="G167" s="17" t="s">
+      <c r="C169" s="2">
+        <v>0</v>
+      </c>
+      <c r="D169" s="2">
+        <v>0</v>
+      </c>
+      <c r="E169" s="2">
+        <v>1</v>
+      </c>
+      <c r="F169" s="3">
+        <v>1</v>
+      </c>
+      <c r="G169" s="17" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A168" s="18" t="s">
-        <v>490</v>
-      </c>
-      <c r="B168" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C168" s="2">
-        <v>0</v>
-      </c>
-      <c r="D168" s="2">
-        <v>0</v>
-      </c>
-      <c r="E168" s="2">
-        <v>1</v>
-      </c>
-      <c r="F168" s="3">
-        <v>1</v>
-      </c>
-      <c r="G168" s="18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A169" s="18" t="s">
-        <v>491</v>
-      </c>
-      <c r="B169" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C169" s="2">
-        <v>0</v>
-      </c>
-      <c r="D169" s="2">
-        <v>0</v>
-      </c>
-      <c r="E169" s="2">
-        <v>1</v>
-      </c>
-      <c r="F169" s="3">
-        <v>1</v>
-      </c>
-      <c r="G169" s="18" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="18" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B170" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -5904,15 +5919,15 @@
         <v>1</v>
       </c>
       <c r="G170" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -5927,15 +5942,15 @@
         <v>1</v>
       </c>
       <c r="G171" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -5950,15 +5965,15 @@
         <v>1</v>
       </c>
       <c r="G172" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="18" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B173" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -5973,15 +5988,15 @@
         <v>1</v>
       </c>
       <c r="G173" s="18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="18" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B174" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -5996,29 +6011,75 @@
         <v>1</v>
       </c>
       <c r="G174" s="18" t="s">
-        <v>214</v>
+        <v>332</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C175" s="2">
+        <v>0</v>
+      </c>
+      <c r="D175" s="2">
+        <v>0</v>
+      </c>
+      <c r="E175" s="2">
+        <v>1</v>
+      </c>
+      <c r="F175" s="3">
+        <v>1</v>
+      </c>
+      <c r="G175" s="18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C176" s="2">
+        <v>0</v>
+      </c>
+      <c r="D176" s="2">
+        <v>0</v>
+      </c>
+      <c r="E176" s="2">
+        <v>1</v>
+      </c>
+      <c r="F176" s="3">
+        <v>1</v>
+      </c>
+      <c r="G176" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" s="18" t="s">
         <v>497</v>
       </c>
-      <c r="B175" s="16" t="s">
+      <c r="B177" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C175" s="2">
-        <v>0</v>
-      </c>
-      <c r="D175" s="2">
-        <v>0</v>
-      </c>
-      <c r="E175" s="2">
-        <v>1</v>
-      </c>
-      <c r="F175" s="3">
-        <v>1</v>
-      </c>
-      <c r="G175" s="18" t="s">
+      <c r="C177" s="2">
+        <v>0</v>
+      </c>
+      <c r="D177" s="2">
+        <v>0</v>
+      </c>
+      <c r="E177" s="2">
+        <v>1</v>
+      </c>
+      <c r="F177" s="3">
+        <v>1</v>
+      </c>
+      <c r="G177" s="18" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update qual / multicountry
- Load and export problem report data
- Export deidentified data for caregiver IDIs
- Fix referral definition
- Disable groupby district (to be compatible with test Senegal and India data)
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="528">
   <si>
     <t>old</t>
   </si>
@@ -1605,6 +1605,9 @@
   </si>
   <si>
     <t>cg_eligibility</t>
+  </si>
+  <si>
+    <t>qual</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G179"/>
+  <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2026,11 +2029,11 @@
     <col min="3" max="3" width="8.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
     <col min="5" max="5" width="9.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="3"/>
-    <col min="7" max="7" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" style="3"/>
+    <col min="8" max="8" width="31.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2050,10 +2053,13 @@
         <v>172</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2072,11 +2078,14 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -2095,11 +2104,14 @@
       <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -2118,11 +2130,14 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>498</v>
       </c>
@@ -2141,11 +2156,14 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>335</v>
       </c>
@@ -2164,11 +2182,14 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>336</v>
       </c>
@@ -2187,11 +2208,14 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>499</v>
       </c>
@@ -2210,11 +2234,14 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>337</v>
       </c>
@@ -2233,11 +2260,14 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>338</v>
       </c>
@@ -2256,11 +2286,14 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>339</v>
       </c>
@@ -2279,11 +2312,14 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>507</v>
       </c>
@@ -2302,11 +2338,14 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>340</v>
       </c>
@@ -2325,11 +2364,14 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>341</v>
       </c>
@@ -2348,11 +2390,14 @@
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>342</v>
       </c>
@@ -2371,11 +2416,14 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>506</v>
       </c>
@@ -2394,11 +2442,14 @@
       <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>343</v>
       </c>
@@ -2417,11 +2468,14 @@
       <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>344</v>
       </c>
@@ -2440,11 +2494,14 @@
       <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>345</v>
       </c>
@@ -2463,11 +2520,14 @@
       <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>346</v>
       </c>
@@ -2486,11 +2546,14 @@
       <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>347</v>
       </c>
@@ -2509,11 +2572,14 @@
       <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>348</v>
       </c>
@@ -2532,11 +2598,14 @@
       <c r="F22" s="3">
         <v>1</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>349</v>
       </c>
@@ -2555,11 +2624,14 @@
       <c r="F23" s="3">
         <v>1</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>350</v>
       </c>
@@ -2578,11 +2650,14 @@
       <c r="F24" s="3">
         <v>1</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>351</v>
       </c>
@@ -2601,11 +2676,14 @@
       <c r="F25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>352</v>
       </c>
@@ -2624,11 +2702,14 @@
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>353</v>
       </c>
@@ -2647,11 +2728,14 @@
       <c r="F27" s="3">
         <v>1</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>354</v>
       </c>
@@ -2670,11 +2754,14 @@
       <c r="F28" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>355</v>
       </c>
@@ -2693,11 +2780,14 @@
       <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>356</v>
       </c>
@@ -2716,11 +2806,14 @@
       <c r="F30" s="3">
         <v>1</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>521</v>
       </c>
@@ -2739,11 +2832,14 @@
       <c r="F31" s="3">
         <v>1</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>525</v>
       </c>
@@ -2762,11 +2858,14 @@
       <c r="F32" s="3">
         <v>0</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>357</v>
       </c>
@@ -2785,11 +2884,14 @@
       <c r="F33" s="3">
         <v>1</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>358</v>
       </c>
@@ -2808,11 +2910,14 @@
       <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="10" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>359</v>
       </c>
@@ -2820,22 +2925,25 @@
         <v>47</v>
       </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
       <c r="E35" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3">
-        <v>0</v>
-      </c>
-      <c r="G35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>360</v>
       </c>
@@ -2854,11 +2962,14 @@
       <c r="F36" s="3">
         <v>1</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>361</v>
       </c>
@@ -2866,22 +2977,25 @@
         <v>49</v>
       </c>
       <c r="C37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3">
-        <v>0</v>
-      </c>
-      <c r="G37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>362</v>
       </c>
@@ -2900,11 +3014,14 @@
       <c r="F38" s="3">
         <v>1</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>363</v>
       </c>
@@ -2923,11 +3040,14 @@
       <c r="F39" s="3">
         <v>1</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>364</v>
       </c>
@@ -2946,11 +3066,14 @@
       <c r="F40" s="3">
         <v>1</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>365</v>
       </c>
@@ -2969,11 +3092,14 @@
       <c r="F41" s="3">
         <v>1</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>366</v>
       </c>
@@ -2992,11 +3118,14 @@
       <c r="F42" s="3">
         <v>1</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>367</v>
       </c>
@@ -3015,11 +3144,14 @@
       <c r="F43" s="3">
         <v>1</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>368</v>
       </c>
@@ -3038,11 +3170,14 @@
       <c r="F44" s="3">
         <v>1</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>369</v>
       </c>
@@ -3059,13 +3194,16 @@
         <v>1</v>
       </c>
       <c r="F45" s="3">
-        <v>0</v>
-      </c>
-      <c r="G45" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>370</v>
       </c>
@@ -3084,11 +3222,14 @@
       <c r="F46" s="3">
         <v>0</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>371</v>
       </c>
@@ -3107,11 +3248,14 @@
       <c r="F47" s="3">
         <v>0</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>372</v>
       </c>
@@ -3130,11 +3274,14 @@
       <c r="F48" s="3">
         <v>0</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="3">
+        <v>1</v>
+      </c>
+      <c r="H48" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>373</v>
       </c>
@@ -3153,11 +3300,14 @@
       <c r="F49" s="4">
         <v>0</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="9" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>374</v>
       </c>
@@ -3176,11 +3326,14 @@
       <c r="F50" s="4">
         <v>0</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>500</v>
       </c>
@@ -3199,11 +3352,14 @@
       <c r="F51" s="4">
         <v>0</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="9" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>501</v>
       </c>
@@ -3222,11 +3378,14 @@
       <c r="F52" s="4">
         <v>0</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="9" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>511</v>
       </c>
@@ -3245,11 +3404,14 @@
       <c r="F53" s="4">
         <v>0</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>375</v>
       </c>
@@ -3268,11 +3430,14 @@
       <c r="F54" s="4">
         <v>0</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>376</v>
       </c>
@@ -3291,11 +3456,14 @@
       <c r="F55" s="4">
         <v>0</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>377</v>
       </c>
@@ -3314,11 +3482,14 @@
       <c r="F56" s="4">
         <v>0</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="9" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>378</v>
       </c>
@@ -3337,11 +3508,14 @@
       <c r="F57" s="4">
         <v>0</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="9" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>517</v>
       </c>
@@ -3360,11 +3534,14 @@
       <c r="F58" s="4">
         <v>1</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="3">
+        <v>1</v>
+      </c>
+      <c r="H58" s="11" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>519</v>
       </c>
@@ -3383,11 +3560,14 @@
       <c r="F59" s="4">
         <v>1</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="3">
+        <v>1</v>
+      </c>
+      <c r="H59" s="11" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>514</v>
       </c>
@@ -3406,11 +3586,14 @@
       <c r="F60" s="4">
         <v>0</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>379</v>
       </c>
@@ -3429,11 +3612,14 @@
       <c r="F61" s="3">
         <v>0</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="H61" s="13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
         <v>380</v>
       </c>
@@ -3452,11 +3638,14 @@
       <c r="F62" s="3">
         <v>0</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+      <c r="H62" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>381</v>
       </c>
@@ -3475,11 +3664,14 @@
       <c r="F63" s="3">
         <v>0</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="G63" s="3">
+        <v>1</v>
+      </c>
+      <c r="H63" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
         <v>382</v>
       </c>
@@ -3498,11 +3690,14 @@
       <c r="F64" s="3">
         <v>0</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G64" s="3">
+        <v>1</v>
+      </c>
+      <c r="H64" s="13" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
         <v>383</v>
       </c>
@@ -3521,11 +3716,14 @@
       <c r="F65" s="3">
         <v>0</v>
       </c>
-      <c r="G65" s="13" t="s">
+      <c r="G65" s="3">
+        <v>1</v>
+      </c>
+      <c r="H65" s="13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
         <v>384</v>
       </c>
@@ -3544,11 +3742,14 @@
       <c r="F66" s="3">
         <v>0</v>
       </c>
-      <c r="G66" s="13" t="s">
+      <c r="G66" s="3">
+        <v>1</v>
+      </c>
+      <c r="H66" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
         <v>385</v>
       </c>
@@ -3567,11 +3768,14 @@
       <c r="F67" s="3">
         <v>0</v>
       </c>
-      <c r="G67" s="13" t="s">
+      <c r="G67" s="3">
+        <v>1</v>
+      </c>
+      <c r="H67" s="13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
         <v>386</v>
       </c>
@@ -3590,11 +3794,14 @@
       <c r="F68" s="3">
         <v>0</v>
       </c>
-      <c r="G68" s="13" t="s">
+      <c r="G68" s="3">
+        <v>1</v>
+      </c>
+      <c r="H68" s="13" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
         <v>387</v>
       </c>
@@ -3613,11 +3820,14 @@
       <c r="F69" s="3">
         <v>0</v>
       </c>
-      <c r="G69" s="13" t="s">
+      <c r="G69" s="3">
+        <v>1</v>
+      </c>
+      <c r="H69" s="13" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
         <v>388</v>
       </c>
@@ -3636,11 +3846,14 @@
       <c r="F70" s="3">
         <v>0</v>
       </c>
-      <c r="G70" s="13" t="s">
+      <c r="G70" s="3">
+        <v>1</v>
+      </c>
+      <c r="H70" s="13" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
         <v>389</v>
       </c>
@@ -3659,11 +3872,14 @@
       <c r="F71" s="3">
         <v>0</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G71" s="3">
+        <v>1</v>
+      </c>
+      <c r="H71" s="13" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
         <v>390</v>
       </c>
@@ -3682,11 +3898,14 @@
       <c r="F72" s="3">
         <v>0</v>
       </c>
-      <c r="G72" s="13" t="s">
+      <c r="G72" s="3">
+        <v>1</v>
+      </c>
+      <c r="H72" s="13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
         <v>391</v>
       </c>
@@ -3705,11 +3924,14 @@
       <c r="F73" s="3">
         <v>0</v>
       </c>
-      <c r="G73" s="13" t="s">
+      <c r="G73" s="3">
+        <v>1</v>
+      </c>
+      <c r="H73" s="13" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
         <v>392</v>
       </c>
@@ -3728,11 +3950,14 @@
       <c r="F74" s="3">
         <v>0</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="G74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="13" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
         <v>393</v>
       </c>
@@ -3751,11 +3976,14 @@
       <c r="F75" s="3">
         <v>0</v>
       </c>
-      <c r="G75" s="13" t="s">
+      <c r="G75" s="3">
+        <v>1</v>
+      </c>
+      <c r="H75" s="13" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
         <v>394</v>
       </c>
@@ -3774,11 +4002,14 @@
       <c r="F76" s="3">
         <v>0</v>
       </c>
-      <c r="G76" s="13" t="s">
+      <c r="G76" s="3">
+        <v>1</v>
+      </c>
+      <c r="H76" s="13" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
         <v>395</v>
       </c>
@@ -3797,11 +4028,14 @@
       <c r="F77" s="3">
         <v>0</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="G77" s="3">
+        <v>1</v>
+      </c>
+      <c r="H77" s="13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
         <v>396</v>
       </c>
@@ -3820,11 +4054,14 @@
       <c r="F78" s="3">
         <v>0</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="G78" s="3">
+        <v>1</v>
+      </c>
+      <c r="H78" s="13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
         <v>397</v>
       </c>
@@ -3843,11 +4080,14 @@
       <c r="F79" s="3">
         <v>0</v>
       </c>
-      <c r="G79" s="13" t="s">
+      <c r="G79" s="3">
+        <v>1</v>
+      </c>
+      <c r="H79" s="13" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>398</v>
       </c>
@@ -3866,11 +4106,14 @@
       <c r="F80" s="3">
         <v>0</v>
       </c>
-      <c r="G80" s="13" t="s">
+      <c r="G80" s="3">
+        <v>1</v>
+      </c>
+      <c r="H80" s="13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
         <v>399</v>
       </c>
@@ -3889,11 +4132,14 @@
       <c r="F81" s="3">
         <v>0</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="G81" s="3">
+        <v>1</v>
+      </c>
+      <c r="H81" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>400</v>
       </c>
@@ -3912,11 +4158,14 @@
       <c r="F82" s="3">
         <v>0</v>
       </c>
-      <c r="G82" s="13" t="s">
+      <c r="G82" s="3">
+        <v>1</v>
+      </c>
+      <c r="H82" s="13" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
         <v>401</v>
       </c>
@@ -3935,11 +4184,14 @@
       <c r="F83" s="3">
         <v>0</v>
       </c>
-      <c r="G83" s="13" t="s">
+      <c r="G83" s="3">
+        <v>1</v>
+      </c>
+      <c r="H83" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>402</v>
       </c>
@@ -3958,11 +4210,14 @@
       <c r="F84" s="3">
         <v>0</v>
       </c>
-      <c r="G84" s="13" t="s">
+      <c r="G84" s="3">
+        <v>1</v>
+      </c>
+      <c r="H84" s="13" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>403</v>
       </c>
@@ -3981,11 +4236,14 @@
       <c r="F85" s="3">
         <v>0</v>
       </c>
-      <c r="G85" s="13" t="s">
+      <c r="G85" s="3">
+        <v>1</v>
+      </c>
+      <c r="H85" s="13" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>404</v>
       </c>
@@ -4004,11 +4262,14 @@
       <c r="F86" s="3">
         <v>0</v>
       </c>
-      <c r="G86" s="13" t="s">
+      <c r="G86" s="3">
+        <v>1</v>
+      </c>
+      <c r="H86" s="13" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>405</v>
       </c>
@@ -4027,11 +4288,14 @@
       <c r="F87" s="3">
         <v>0</v>
       </c>
-      <c r="G87" s="13" t="s">
+      <c r="G87" s="3">
+        <v>1</v>
+      </c>
+      <c r="H87" s="13" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>406</v>
       </c>
@@ -4050,11 +4314,14 @@
       <c r="F88" s="3">
         <v>0</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G88" s="3">
+        <v>1</v>
+      </c>
+      <c r="H88" s="13" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>407</v>
       </c>
@@ -4073,11 +4340,14 @@
       <c r="F89" s="3">
         <v>0</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G89" s="3">
+        <v>1</v>
+      </c>
+      <c r="H89" s="13" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
         <v>408</v>
       </c>
@@ -4096,11 +4366,14 @@
       <c r="F90" s="3">
         <v>1</v>
       </c>
-      <c r="G90" s="17" t="s">
+      <c r="G90" s="3">
+        <v>1</v>
+      </c>
+      <c r="H90" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
         <v>409</v>
       </c>
@@ -4119,11 +4392,14 @@
       <c r="F91" s="3">
         <v>1</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="G91" s="3">
+        <v>0</v>
+      </c>
+      <c r="H91" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
         <v>410</v>
       </c>
@@ -4142,11 +4418,14 @@
       <c r="F92" s="3">
         <v>1</v>
       </c>
-      <c r="G92" s="17" t="s">
+      <c r="G92" s="3">
+        <v>0</v>
+      </c>
+      <c r="H92" s="17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
         <v>411</v>
       </c>
@@ -4165,11 +4444,14 @@
       <c r="F93" s="3">
         <v>1</v>
       </c>
-      <c r="G93" s="17" t="s">
+      <c r="G93" s="3">
+        <v>0</v>
+      </c>
+      <c r="H93" s="17" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
         <v>412</v>
       </c>
@@ -4188,11 +4470,14 @@
       <c r="F94" s="3">
         <v>1</v>
       </c>
-      <c r="G94" s="17" t="s">
+      <c r="G94" s="3">
+        <v>0</v>
+      </c>
+      <c r="H94" s="17" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
         <v>413</v>
       </c>
@@ -4211,11 +4496,14 @@
       <c r="F95" s="3">
         <v>1</v>
       </c>
-      <c r="G95" s="17" t="s">
+      <c r="G95" s="3">
+        <v>0</v>
+      </c>
+      <c r="H95" s="17" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
         <v>414</v>
       </c>
@@ -4234,11 +4522,14 @@
       <c r="F96" s="3">
         <v>1</v>
       </c>
-      <c r="G96" s="17" t="s">
+      <c r="G96" s="3">
+        <v>0</v>
+      </c>
+      <c r="H96" s="17" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
         <v>415</v>
       </c>
@@ -4257,11 +4548,14 @@
       <c r="F97" s="3">
         <v>1</v>
       </c>
-      <c r="G97" s="17" t="s">
+      <c r="G97" s="3">
+        <v>0</v>
+      </c>
+      <c r="H97" s="17" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
         <v>416</v>
       </c>
@@ -4280,11 +4574,14 @@
       <c r="F98" s="3">
         <v>1</v>
       </c>
-      <c r="G98" s="17" t="s">
+      <c r="G98" s="3">
+        <v>0</v>
+      </c>
+      <c r="H98" s="17" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
         <v>418</v>
       </c>
@@ -4303,11 +4600,14 @@
       <c r="F99" s="3">
         <v>1</v>
       </c>
-      <c r="G99" s="17" t="s">
+      <c r="G99" s="3">
+        <v>0</v>
+      </c>
+      <c r="H99" s="17" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>419</v>
       </c>
@@ -4326,11 +4626,14 @@
       <c r="F100" s="3">
         <v>1</v>
       </c>
-      <c r="G100" s="17" t="s">
+      <c r="G100" s="3">
+        <v>0</v>
+      </c>
+      <c r="H100" s="17" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
         <v>420</v>
       </c>
@@ -4349,11 +4652,14 @@
       <c r="F101" s="3">
         <v>1</v>
       </c>
-      <c r="G101" s="17" t="s">
+      <c r="G101" s="3">
+        <v>0</v>
+      </c>
+      <c r="H101" s="17" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
         <v>421</v>
       </c>
@@ -4372,11 +4678,14 @@
       <c r="F102" s="3">
         <v>1</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="G102" s="3">
+        <v>0</v>
+      </c>
+      <c r="H102" s="17" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
         <v>422</v>
       </c>
@@ -4395,11 +4704,14 @@
       <c r="F103" s="3">
         <v>1</v>
       </c>
-      <c r="G103" s="17" t="s">
+      <c r="G103" s="3">
+        <v>0</v>
+      </c>
+      <c r="H103" s="17" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
         <v>423</v>
       </c>
@@ -4418,11 +4730,14 @@
       <c r="F104" s="3">
         <v>1</v>
       </c>
-      <c r="G104" s="17" t="s">
+      <c r="G104" s="3">
+        <v>0</v>
+      </c>
+      <c r="H104" s="17" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
         <v>424</v>
       </c>
@@ -4441,11 +4756,14 @@
       <c r="F105" s="3">
         <v>1</v>
       </c>
-      <c r="G105" s="17" t="s">
+      <c r="G105" s="3">
+        <v>0</v>
+      </c>
+      <c r="H105" s="17" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
         <v>425</v>
       </c>
@@ -4464,11 +4782,14 @@
       <c r="F106" s="3">
         <v>1</v>
       </c>
-      <c r="G106" s="17" t="s">
+      <c r="G106" s="3">
+        <v>0</v>
+      </c>
+      <c r="H106" s="17" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>426</v>
       </c>
@@ -4487,11 +4808,14 @@
       <c r="F107" s="3">
         <v>1</v>
       </c>
-      <c r="G107" s="17" t="s">
+      <c r="G107" s="3">
+        <v>1</v>
+      </c>
+      <c r="H107" s="17" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
         <v>427</v>
       </c>
@@ -4510,11 +4834,14 @@
       <c r="F108" s="3">
         <v>1</v>
       </c>
-      <c r="G108" s="17" t="s">
+      <c r="G108" s="3">
+        <v>1</v>
+      </c>
+      <c r="H108" s="17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
         <v>428</v>
       </c>
@@ -4533,11 +4860,14 @@
       <c r="F109" s="3">
         <v>1</v>
       </c>
-      <c r="G109" s="17" t="s">
+      <c r="G109" s="3">
+        <v>1</v>
+      </c>
+      <c r="H109" s="17" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
         <v>429</v>
       </c>
@@ -4556,11 +4886,14 @@
       <c r="F110" s="3">
         <v>1</v>
       </c>
-      <c r="G110" s="17" t="s">
+      <c r="G110" s="3">
+        <v>1</v>
+      </c>
+      <c r="H110" s="17" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
         <v>430</v>
       </c>
@@ -4579,11 +4912,14 @@
       <c r="F111" s="3">
         <v>1</v>
       </c>
-      <c r="G111" s="17" t="s">
+      <c r="G111" s="3">
+        <v>1</v>
+      </c>
+      <c r="H111" s="17" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
         <v>431</v>
       </c>
@@ -4602,11 +4938,14 @@
       <c r="F112" s="3">
         <v>1</v>
       </c>
-      <c r="G112" s="17" t="s">
+      <c r="G112" s="3">
+        <v>1</v>
+      </c>
+      <c r="H112" s="17" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
         <v>432</v>
       </c>
@@ -4625,11 +4964,14 @@
       <c r="F113" s="3">
         <v>1</v>
       </c>
-      <c r="G113" s="17" t="s">
+      <c r="G113" s="3">
+        <v>1</v>
+      </c>
+      <c r="H113" s="17" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
         <v>433</v>
       </c>
@@ -4648,11 +4990,14 @@
       <c r="F114" s="3">
         <v>1</v>
       </c>
-      <c r="G114" s="17" t="s">
+      <c r="G114" s="3">
+        <v>1</v>
+      </c>
+      <c r="H114" s="17" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
         <v>434</v>
       </c>
@@ -4671,11 +5016,14 @@
       <c r="F115" s="3">
         <v>1</v>
       </c>
-      <c r="G115" s="17" t="s">
+      <c r="G115" s="3">
+        <v>1</v>
+      </c>
+      <c r="H115" s="17" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>435</v>
       </c>
@@ -4694,11 +5042,14 @@
       <c r="F116" s="3">
         <v>1</v>
       </c>
-      <c r="G116" s="17" t="s">
+      <c r="G116" s="3">
+        <v>1</v>
+      </c>
+      <c r="H116" s="17" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>436</v>
       </c>
@@ -4717,11 +5068,14 @@
       <c r="F117" s="3">
         <v>1</v>
       </c>
-      <c r="G117" s="17" t="s">
+      <c r="G117" s="3">
+        <v>1</v>
+      </c>
+      <c r="H117" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>437</v>
       </c>
@@ -4740,11 +5094,14 @@
       <c r="F118" s="3">
         <v>1</v>
       </c>
-      <c r="G118" s="17" t="s">
+      <c r="G118" s="3">
+        <v>1</v>
+      </c>
+      <c r="H118" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>438</v>
       </c>
@@ -4763,11 +5120,14 @@
       <c r="F119" s="3">
         <v>1</v>
       </c>
-      <c r="G119" s="17" t="s">
+      <c r="G119" s="3">
+        <v>1</v>
+      </c>
+      <c r="H119" s="17" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
         <v>439</v>
       </c>
@@ -4786,11 +5146,14 @@
       <c r="F120" s="3">
         <v>1</v>
       </c>
-      <c r="G120" s="17" t="s">
+      <c r="G120" s="3">
+        <v>1</v>
+      </c>
+      <c r="H120" s="17" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>440</v>
       </c>
@@ -4809,11 +5172,14 @@
       <c r="F121" s="3">
         <v>1</v>
       </c>
-      <c r="G121" s="17" t="s">
+      <c r="G121" s="3">
+        <v>1</v>
+      </c>
+      <c r="H121" s="17" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>441</v>
       </c>
@@ -4832,11 +5198,14 @@
       <c r="F122" s="3">
         <v>1</v>
       </c>
-      <c r="G122" s="17" t="s">
+      <c r="G122" s="3">
+        <v>1</v>
+      </c>
+      <c r="H122" s="17" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
         <v>442</v>
       </c>
@@ -4855,11 +5224,14 @@
       <c r="F123" s="3">
         <v>1</v>
       </c>
-      <c r="G123" s="17" t="s">
+      <c r="G123" s="3">
+        <v>1</v>
+      </c>
+      <c r="H123" s="17" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
         <v>443</v>
       </c>
@@ -4878,11 +5250,14 @@
       <c r="F124" s="3">
         <v>1</v>
       </c>
-      <c r="G124" s="17" t="s">
+      <c r="G124" s="3">
+        <v>0</v>
+      </c>
+      <c r="H124" s="17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
         <v>444</v>
       </c>
@@ -4901,11 +5276,14 @@
       <c r="F125" s="3">
         <v>1</v>
       </c>
-      <c r="G125" s="17" t="s">
+      <c r="G125" s="3">
+        <v>0</v>
+      </c>
+      <c r="H125" s="17" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>445</v>
       </c>
@@ -4924,11 +5302,14 @@
       <c r="F126" s="3">
         <v>1</v>
       </c>
-      <c r="G126" s="17" t="s">
+      <c r="G126" s="3">
+        <v>0</v>
+      </c>
+      <c r="H126" s="17" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
         <v>446</v>
       </c>
@@ -4947,11 +5328,14 @@
       <c r="F127" s="3">
         <v>1</v>
       </c>
-      <c r="G127" s="17" t="s">
+      <c r="G127" s="3">
+        <v>0</v>
+      </c>
+      <c r="H127" s="17" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>447</v>
       </c>
@@ -4970,11 +5354,14 @@
       <c r="F128" s="3">
         <v>1</v>
       </c>
-      <c r="G128" s="17" t="s">
+      <c r="G128" s="3">
+        <v>0</v>
+      </c>
+      <c r="H128" s="17" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
         <v>448</v>
       </c>
@@ -4993,11 +5380,14 @@
       <c r="F129" s="3">
         <v>1</v>
       </c>
-      <c r="G129" s="17" t="s">
+      <c r="G129" s="3">
+        <v>0</v>
+      </c>
+      <c r="H129" s="17" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
         <v>449</v>
       </c>
@@ -5016,11 +5406,14 @@
       <c r="F130" s="3">
         <v>1</v>
       </c>
-      <c r="G130" s="17" t="s">
+      <c r="G130" s="3">
+        <v>0</v>
+      </c>
+      <c r="H130" s="17" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
         <v>450</v>
       </c>
@@ -5039,11 +5432,14 @@
       <c r="F131" s="3">
         <v>1</v>
       </c>
-      <c r="G131" s="17" t="s">
+      <c r="G131" s="3">
+        <v>0</v>
+      </c>
+      <c r="H131" s="17" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
         <v>451</v>
       </c>
@@ -5062,11 +5458,14 @@
       <c r="F132" s="3">
         <v>1</v>
       </c>
-      <c r="G132" s="17" t="s">
+      <c r="G132" s="3">
+        <v>0</v>
+      </c>
+      <c r="H132" s="17" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
         <v>452</v>
       </c>
@@ -5085,11 +5484,14 @@
       <c r="F133" s="3">
         <v>1</v>
       </c>
-      <c r="G133" s="17" t="s">
+      <c r="G133" s="3">
+        <v>0</v>
+      </c>
+      <c r="H133" s="17" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
         <v>417</v>
       </c>
@@ -5108,11 +5510,14 @@
       <c r="F134" s="3">
         <v>1</v>
       </c>
-      <c r="G134" s="17" t="s">
+      <c r="G134" s="3">
+        <v>0</v>
+      </c>
+      <c r="H134" s="17" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
         <v>453</v>
       </c>
@@ -5131,11 +5536,14 @@
       <c r="F135" s="3">
         <v>1</v>
       </c>
-      <c r="G135" s="17" t="s">
+      <c r="G135" s="3">
+        <v>1</v>
+      </c>
+      <c r="H135" s="17" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
         <v>454</v>
       </c>
@@ -5154,11 +5562,14 @@
       <c r="F136" s="3">
         <v>1</v>
       </c>
-      <c r="G136" s="17" t="s">
+      <c r="G136" s="3">
+        <v>1</v>
+      </c>
+      <c r="H136" s="17" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
         <v>455</v>
       </c>
@@ -5177,11 +5588,14 @@
       <c r="F137" s="3">
         <v>1</v>
       </c>
-      <c r="G137" s="17" t="s">
+      <c r="G137" s="3">
+        <v>0</v>
+      </c>
+      <c r="H137" s="17" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="17" t="s">
         <v>456</v>
       </c>
@@ -5200,11 +5614,14 @@
       <c r="F138" s="3">
         <v>1</v>
       </c>
-      <c r="G138" s="17" t="s">
+      <c r="G138" s="3">
+        <v>0</v>
+      </c>
+      <c r="H138" s="17" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
         <v>457</v>
       </c>
@@ -5223,11 +5640,14 @@
       <c r="F139" s="3">
         <v>1</v>
       </c>
-      <c r="G139" s="17" t="s">
+      <c r="G139" s="3">
+        <v>0</v>
+      </c>
+      <c r="H139" s="17" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
         <v>458</v>
       </c>
@@ -5246,11 +5666,14 @@
       <c r="F140" s="3">
         <v>1</v>
       </c>
-      <c r="G140" s="17" t="s">
+      <c r="G140" s="3">
+        <v>0</v>
+      </c>
+      <c r="H140" s="17" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
         <v>459</v>
       </c>
@@ -5269,11 +5692,14 @@
       <c r="F141" s="3">
         <v>1</v>
       </c>
-      <c r="G141" s="17" t="s">
+      <c r="G141" s="3">
+        <v>0</v>
+      </c>
+      <c r="H141" s="17" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>460</v>
       </c>
@@ -5292,11 +5718,14 @@
       <c r="F142" s="3">
         <v>1</v>
       </c>
-      <c r="G142" s="17" t="s">
+      <c r="G142" s="3">
+        <v>0</v>
+      </c>
+      <c r="H142" s="17" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>461</v>
       </c>
@@ -5315,11 +5744,14 @@
       <c r="F143" s="3">
         <v>1</v>
       </c>
-      <c r="G143" s="17" t="s">
+      <c r="G143" s="3">
+        <v>0</v>
+      </c>
+      <c r="H143" s="17" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
         <v>462</v>
       </c>
@@ -5338,11 +5770,14 @@
       <c r="F144" s="3">
         <v>1</v>
       </c>
-      <c r="G144" s="17" t="s">
+      <c r="G144" s="3">
+        <v>0</v>
+      </c>
+      <c r="H144" s="17" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>463</v>
       </c>
@@ -5361,11 +5796,14 @@
       <c r="F145" s="3">
         <v>1</v>
       </c>
-      <c r="G145" s="17" t="s">
+      <c r="G145" s="3">
+        <v>0</v>
+      </c>
+      <c r="H145" s="17" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>464</v>
       </c>
@@ -5384,11 +5822,14 @@
       <c r="F146" s="3">
         <v>1</v>
       </c>
-      <c r="G146" s="17" t="s">
+      <c r="G146" s="3">
+        <v>0</v>
+      </c>
+      <c r="H146" s="17" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>465</v>
       </c>
@@ -5407,11 +5848,14 @@
       <c r="F147" s="3">
         <v>1</v>
       </c>
-      <c r="G147" s="17" t="s">
+      <c r="G147" s="3">
+        <v>0</v>
+      </c>
+      <c r="H147" s="17" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
         <v>466</v>
       </c>
@@ -5430,11 +5874,14 @@
       <c r="F148" s="3">
         <v>1</v>
       </c>
-      <c r="G148" s="17" t="s">
+      <c r="G148" s="3">
+        <v>0</v>
+      </c>
+      <c r="H148" s="17" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
         <v>467</v>
       </c>
@@ -5453,11 +5900,14 @@
       <c r="F149" s="3">
         <v>1</v>
       </c>
-      <c r="G149" s="17" t="s">
+      <c r="G149" s="3">
+        <v>0</v>
+      </c>
+      <c r="H149" s="17" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>468</v>
       </c>
@@ -5476,11 +5926,14 @@
       <c r="F150" s="3">
         <v>1</v>
       </c>
-      <c r="G150" s="17" t="s">
+      <c r="G150" s="3">
+        <v>0</v>
+      </c>
+      <c r="H150" s="17" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
         <v>469</v>
       </c>
@@ -5499,11 +5952,14 @@
       <c r="F151" s="3">
         <v>1</v>
       </c>
-      <c r="G151" s="17" t="s">
+      <c r="G151" s="3">
+        <v>0</v>
+      </c>
+      <c r="H151" s="17" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
         <v>470</v>
       </c>
@@ -5522,11 +5978,14 @@
       <c r="F152" s="3">
         <v>1</v>
       </c>
-      <c r="G152" s="17" t="s">
+      <c r="G152" s="3">
+        <v>0</v>
+      </c>
+      <c r="H152" s="17" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
         <v>471</v>
       </c>
@@ -5545,11 +6004,14 @@
       <c r="F153" s="3">
         <v>1</v>
       </c>
-      <c r="G153" s="17" t="s">
+      <c r="G153" s="3">
+        <v>0</v>
+      </c>
+      <c r="H153" s="17" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
         <v>472</v>
       </c>
@@ -5568,11 +6030,14 @@
       <c r="F154" s="3">
         <v>1</v>
       </c>
-      <c r="G154" s="17" t="s">
+      <c r="G154" s="3">
+        <v>0</v>
+      </c>
+      <c r="H154" s="17" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
         <v>473</v>
       </c>
@@ -5591,11 +6056,14 @@
       <c r="F155" s="3">
         <v>1</v>
       </c>
-      <c r="G155" s="17" t="s">
+      <c r="G155" s="3">
+        <v>0</v>
+      </c>
+      <c r="H155" s="17" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
         <v>474</v>
       </c>
@@ -5614,11 +6082,14 @@
       <c r="F156" s="3">
         <v>1</v>
       </c>
-      <c r="G156" s="17" t="s">
+      <c r="G156" s="3">
+        <v>0</v>
+      </c>
+      <c r="H156" s="17" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
         <v>475</v>
       </c>
@@ -5637,11 +6108,14 @@
       <c r="F157" s="3">
         <v>1</v>
       </c>
-      <c r="G157" s="17" t="s">
+      <c r="G157" s="3">
+        <v>0</v>
+      </c>
+      <c r="H157" s="17" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
         <v>476</v>
       </c>
@@ -5660,11 +6134,14 @@
       <c r="F158" s="3">
         <v>1</v>
       </c>
-      <c r="G158" s="17" t="s">
+      <c r="G158" s="3">
+        <v>0</v>
+      </c>
+      <c r="H158" s="17" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
         <v>477</v>
       </c>
@@ -5683,11 +6160,14 @@
       <c r="F159" s="3">
         <v>1</v>
       </c>
-      <c r="G159" s="17" t="s">
+      <c r="G159" s="3">
+        <v>0</v>
+      </c>
+      <c r="H159" s="17" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
         <v>478</v>
       </c>
@@ -5706,11 +6186,14 @@
       <c r="F160" s="3">
         <v>1</v>
       </c>
-      <c r="G160" s="17" t="s">
+      <c r="G160" s="3">
+        <v>0</v>
+      </c>
+      <c r="H160" s="17" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
         <v>479</v>
       </c>
@@ -5729,11 +6212,14 @@
       <c r="F161" s="3">
         <v>1</v>
       </c>
-      <c r="G161" s="17" t="s">
+      <c r="G161" s="3">
+        <v>0</v>
+      </c>
+      <c r="H161" s="17" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
         <v>480</v>
       </c>
@@ -5752,11 +6238,14 @@
       <c r="F162" s="3">
         <v>1</v>
       </c>
-      <c r="G162" s="17" t="s">
+      <c r="G162" s="3">
+        <v>0</v>
+      </c>
+      <c r="H162" s="17" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>481</v>
       </c>
@@ -5775,11 +6264,14 @@
       <c r="F163" s="3">
         <v>1</v>
       </c>
-      <c r="G163" s="17" t="s">
+      <c r="G163" s="3">
+        <v>0</v>
+      </c>
+      <c r="H163" s="17" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
         <v>482</v>
       </c>
@@ -5798,11 +6290,14 @@
       <c r="F164" s="3">
         <v>1</v>
       </c>
-      <c r="G164" s="17" t="s">
+      <c r="G164" s="3">
+        <v>0</v>
+      </c>
+      <c r="H164" s="17" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
         <v>483</v>
       </c>
@@ -5821,11 +6316,14 @@
       <c r="F165" s="3">
         <v>1</v>
       </c>
-      <c r="G165" s="17" t="s">
+      <c r="G165" s="3">
+        <v>0</v>
+      </c>
+      <c r="H165" s="17" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
         <v>484</v>
       </c>
@@ -5844,11 +6342,14 @@
       <c r="F166" s="3">
         <v>1</v>
       </c>
-      <c r="G166" s="17" t="s">
+      <c r="G166" s="3">
+        <v>0</v>
+      </c>
+      <c r="H166" s="17" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>485</v>
       </c>
@@ -5867,11 +6368,14 @@
       <c r="F167" s="3">
         <v>1</v>
       </c>
-      <c r="G167" s="17" t="s">
+      <c r="G167" s="3">
+        <v>0</v>
+      </c>
+      <c r="H167" s="17" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
         <v>486</v>
       </c>
@@ -5890,11 +6394,14 @@
       <c r="F168" s="3">
         <v>1</v>
       </c>
-      <c r="G168" s="17" t="s">
+      <c r="G168" s="3">
+        <v>0</v>
+      </c>
+      <c r="H168" s="17" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
         <v>487</v>
       </c>
@@ -5913,11 +6420,14 @@
       <c r="F169" s="3">
         <v>1</v>
       </c>
-      <c r="G169" s="17" t="s">
+      <c r="G169" s="3">
+        <v>0</v>
+      </c>
+      <c r="H169" s="17" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
         <v>488</v>
       </c>
@@ -5936,11 +6446,14 @@
       <c r="F170" s="3">
         <v>1</v>
       </c>
-      <c r="G170" s="17" t="s">
+      <c r="G170" s="3">
+        <v>0</v>
+      </c>
+      <c r="H170" s="17" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
         <v>489</v>
       </c>
@@ -5959,11 +6472,14 @@
       <c r="F171" s="3">
         <v>1</v>
       </c>
-      <c r="G171" s="17" t="s">
+      <c r="G171" s="3">
+        <v>0</v>
+      </c>
+      <c r="H171" s="17" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="18" t="s">
         <v>490</v>
       </c>
@@ -5982,11 +6498,14 @@
       <c r="F172" s="3">
         <v>1</v>
       </c>
-      <c r="G172" s="18" t="s">
+      <c r="G172" s="3">
+        <v>0</v>
+      </c>
+      <c r="H172" s="18" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="18" t="s">
         <v>491</v>
       </c>
@@ -6005,11 +6524,14 @@
       <c r="F173" s="3">
         <v>1</v>
       </c>
-      <c r="G173" s="18" t="s">
+      <c r="G173" s="3">
+        <v>0</v>
+      </c>
+      <c r="H173" s="18" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="18" t="s">
         <v>492</v>
       </c>
@@ -6028,11 +6550,14 @@
       <c r="F174" s="3">
         <v>1</v>
       </c>
-      <c r="G174" s="18" t="s">
+      <c r="G174" s="3">
+        <v>0</v>
+      </c>
+      <c r="H174" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="18" t="s">
         <v>493</v>
       </c>
@@ -6051,11 +6576,14 @@
       <c r="F175" s="3">
         <v>1</v>
       </c>
-      <c r="G175" s="18" t="s">
+      <c r="G175" s="3">
+        <v>0</v>
+      </c>
+      <c r="H175" s="18" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="18" t="s">
         <v>494</v>
       </c>
@@ -6074,11 +6602,14 @@
       <c r="F176" s="3">
         <v>1</v>
       </c>
-      <c r="G176" s="18" t="s">
+      <c r="G176" s="3">
+        <v>0</v>
+      </c>
+      <c r="H176" s="18" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="18" t="s">
         <v>495</v>
       </c>
@@ -6097,11 +6628,14 @@
       <c r="F177" s="3">
         <v>1</v>
       </c>
-      <c r="G177" s="18" t="s">
+      <c r="G177" s="3">
+        <v>0</v>
+      </c>
+      <c r="H177" s="18" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="18" t="s">
         <v>496</v>
       </c>
@@ -6120,11 +6654,14 @@
       <c r="F178" s="3">
         <v>1</v>
       </c>
-      <c r="G178" s="18" t="s">
+      <c r="G178" s="3">
+        <v>0</v>
+      </c>
+      <c r="H178" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="18" t="s">
         <v>497</v>
       </c>
@@ -6143,7 +6680,10 @@
       <c r="F179" s="3">
         <v>1</v>
       </c>
-      <c r="G179" s="18" t="s">
+      <c r="G179" s="3">
+        <v>0</v>
+      </c>
+      <c r="H179" s="18" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update PATH M&E report export
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -1683,7 +1683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1735,6 +1735,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2018,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="J128" sqref="J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2534,19 +2543,19 @@
       <c r="B20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="21">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22">
+        <v>1</v>
+      </c>
+      <c r="G20" s="22">
         <v>1</v>
       </c>
       <c r="H20" s="11" t="s">
@@ -2560,19 +2569,19 @@
       <c r="B21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="C21" s="20">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0</v>
+      </c>
+      <c r="E21" s="20">
+        <v>1</v>
+      </c>
+      <c r="F21" s="20">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22">
         <v>1</v>
       </c>
       <c r="H21" s="11" t="s">
@@ -2586,19 +2595,19 @@
       <c r="B22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="C22" s="20">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20">
+        <v>1</v>
+      </c>
+      <c r="E22" s="21">
+        <v>1</v>
+      </c>
+      <c r="F22" s="22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22">
         <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
@@ -3626,13 +3635,13 @@
       <c r="B62" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="2">
-        <v>0</v>
-      </c>
-      <c r="D62" s="2">
-        <v>0</v>
-      </c>
-      <c r="E62" s="4">
+      <c r="C62" s="20">
+        <v>0</v>
+      </c>
+      <c r="D62" s="20">
+        <v>0</v>
+      </c>
+      <c r="E62" s="21">
         <v>1</v>
       </c>
       <c r="F62" s="3">
@@ -3652,13 +3661,13 @@
       <c r="B63" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C63" s="2">
-        <v>0</v>
-      </c>
-      <c r="D63" s="2">
-        <v>0</v>
-      </c>
-      <c r="E63" s="4">
+      <c r="C63" s="20">
+        <v>0</v>
+      </c>
+      <c r="D63" s="20">
+        <v>0</v>
+      </c>
+      <c r="E63" s="20">
         <v>1</v>
       </c>
       <c r="F63" s="3">
@@ -3678,13 +3687,13 @@
       <c r="B64" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="2">
-        <v>0</v>
-      </c>
-      <c r="D64" s="2">
-        <v>0</v>
-      </c>
-      <c r="E64" s="4">
+      <c r="C64" s="20">
+        <v>0</v>
+      </c>
+      <c r="D64" s="20">
+        <v>0</v>
+      </c>
+      <c r="E64" s="21">
         <v>1</v>
       </c>
       <c r="F64" s="3">
@@ -3704,13 +3713,13 @@
       <c r="B65" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="2">
-        <v>0</v>
-      </c>
-      <c r="D65" s="2">
-        <v>0</v>
-      </c>
-      <c r="E65" s="4">
+      <c r="C65" s="20">
+        <v>0</v>
+      </c>
+      <c r="D65" s="20">
+        <v>0</v>
+      </c>
+      <c r="E65" s="21">
         <v>1</v>
       </c>
       <c r="F65" s="3">
@@ -4120,13 +4129,13 @@
       <c r="B81" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="20">
         <v>0</v>
       </c>
       <c r="D81" s="2">
         <v>0</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="21">
         <v>1</v>
       </c>
       <c r="F81" s="3">
@@ -4146,13 +4155,13 @@
       <c r="B82" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="20">
         <v>0</v>
       </c>
       <c r="D82" s="2">
         <v>0</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="20">
         <v>1</v>
       </c>
       <c r="F82" s="3">
@@ -4172,13 +4181,13 @@
       <c r="B83" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="20">
         <v>0</v>
       </c>
       <c r="D83" s="2">
         <v>0</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="21">
         <v>1</v>
       </c>
       <c r="F83" s="3">
@@ -4198,13 +4207,13 @@
       <c r="B84" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="20">
         <v>0</v>
       </c>
       <c r="D84" s="2">
         <v>0</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="21">
         <v>1</v>
       </c>
       <c r="F84" s="3">
@@ -4224,13 +4233,13 @@
       <c r="B85" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="20">
         <v>0</v>
       </c>
       <c r="D85" s="2">
         <v>0</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="20">
         <v>1</v>
       </c>
       <c r="F85" s="3">
@@ -4250,7 +4259,7 @@
       <c r="B86" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="20">
         <v>0</v>
       </c>
       <c r="D86" s="2">
@@ -4276,7 +4285,7 @@
       <c r="B87" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="20">
         <v>0</v>
       </c>
       <c r="D87" s="2">
@@ -5010,10 +5019,10 @@
       <c r="D115" s="2">
         <v>0</v>
       </c>
-      <c r="E115" s="2">
-        <v>1</v>
-      </c>
-      <c r="F115" s="3">
+      <c r="E115" s="20">
+        <v>1</v>
+      </c>
+      <c r="F115" s="22">
         <v>1</v>
       </c>
       <c r="G115" s="3">
@@ -5036,10 +5045,10 @@
       <c r="D116" s="2">
         <v>0</v>
       </c>
-      <c r="E116" s="2">
-        <v>1</v>
-      </c>
-      <c r="F116" s="3">
+      <c r="E116" s="20">
+        <v>1</v>
+      </c>
+      <c r="F116" s="22">
         <v>1</v>
       </c>
       <c r="G116" s="3">
@@ -5062,10 +5071,10 @@
       <c r="D117" s="2">
         <v>0</v>
       </c>
-      <c r="E117" s="2">
-        <v>1</v>
-      </c>
-      <c r="F117" s="3">
+      <c r="E117" s="20">
+        <v>1</v>
+      </c>
+      <c r="F117" s="22">
         <v>1</v>
       </c>
       <c r="G117" s="3">
@@ -5088,10 +5097,10 @@
       <c r="D118" s="2">
         <v>0</v>
       </c>
-      <c r="E118" s="2">
-        <v>1</v>
-      </c>
-      <c r="F118" s="3">
+      <c r="E118" s="20">
+        <v>1</v>
+      </c>
+      <c r="F118" s="20">
         <v>1</v>
       </c>
       <c r="G118" s="3">
@@ -5114,10 +5123,10 @@
       <c r="D119" s="2">
         <v>0</v>
       </c>
-      <c r="E119" s="2">
-        <v>1</v>
-      </c>
-      <c r="F119" s="3">
+      <c r="E119" s="20">
+        <v>1</v>
+      </c>
+      <c r="F119" s="22">
         <v>1</v>
       </c>
       <c r="G119" s="3">
@@ -5140,10 +5149,10 @@
       <c r="D120" s="2">
         <v>0</v>
       </c>
-      <c r="E120" s="2">
-        <v>1</v>
-      </c>
-      <c r="F120" s="3">
+      <c r="E120" s="20">
+        <v>1</v>
+      </c>
+      <c r="F120" s="22">
         <v>1</v>
       </c>
       <c r="G120" s="3">
@@ -5166,10 +5175,10 @@
       <c r="D121" s="2">
         <v>0</v>
       </c>
-      <c r="E121" s="2">
-        <v>1</v>
-      </c>
-      <c r="F121" s="3">
+      <c r="E121" s="20">
+        <v>1</v>
+      </c>
+      <c r="F121" s="22">
         <v>1</v>
       </c>
       <c r="G121" s="3">
@@ -5192,10 +5201,10 @@
       <c r="D122" s="2">
         <v>0</v>
       </c>
-      <c r="E122" s="2">
-        <v>1</v>
-      </c>
-      <c r="F122" s="3">
+      <c r="E122" s="20">
+        <v>1</v>
+      </c>
+      <c r="F122" s="20">
         <v>1</v>
       </c>
       <c r="G122" s="3">
@@ -5218,10 +5227,10 @@
       <c r="D123" s="2">
         <v>0</v>
       </c>
-      <c r="E123" s="2">
-        <v>1</v>
-      </c>
-      <c r="F123" s="3">
+      <c r="E123" s="20">
+        <v>1</v>
+      </c>
+      <c r="F123" s="22">
         <v>1</v>
       </c>
       <c r="G123" s="3">
@@ -5244,10 +5253,10 @@
       <c r="D124" s="2">
         <v>0</v>
       </c>
-      <c r="E124" s="2">
-        <v>1</v>
-      </c>
-      <c r="F124" s="3">
+      <c r="E124" s="20">
+        <v>1</v>
+      </c>
+      <c r="F124" s="22">
         <v>1</v>
       </c>
       <c r="G124" s="3">
@@ -5270,10 +5279,10 @@
       <c r="D125" s="2">
         <v>0</v>
       </c>
-      <c r="E125" s="2">
-        <v>1</v>
-      </c>
-      <c r="F125" s="3">
+      <c r="E125" s="20">
+        <v>1</v>
+      </c>
+      <c r="F125" s="22">
         <v>1</v>
       </c>
       <c r="G125" s="3">
@@ -5296,10 +5305,10 @@
       <c r="D126" s="2">
         <v>0</v>
       </c>
-      <c r="E126" s="2">
-        <v>1</v>
-      </c>
-      <c r="F126" s="3">
+      <c r="E126" s="20">
+        <v>1</v>
+      </c>
+      <c r="F126" s="22">
         <v>1</v>
       </c>
       <c r="G126" s="3">
@@ -5322,10 +5331,10 @@
       <c r="D127" s="2">
         <v>0</v>
       </c>
-      <c r="E127" s="2">
-        <v>1</v>
-      </c>
-      <c r="F127" s="3">
+      <c r="E127" s="20">
+        <v>1</v>
+      </c>
+      <c r="F127" s="22">
         <v>1</v>
       </c>
       <c r="G127" s="3">
@@ -5348,10 +5357,10 @@
       <c r="D128" s="2">
         <v>0</v>
       </c>
-      <c r="E128" s="2">
-        <v>1</v>
-      </c>
-      <c r="F128" s="3">
+      <c r="E128" s="20">
+        <v>1</v>
+      </c>
+      <c r="F128" s="20">
         <v>1</v>
       </c>
       <c r="G128" s="3">
@@ -5374,10 +5383,10 @@
       <c r="D129" s="2">
         <v>0</v>
       </c>
-      <c r="E129" s="2">
-        <v>1</v>
-      </c>
-      <c r="F129" s="3">
+      <c r="E129" s="20">
+        <v>1</v>
+      </c>
+      <c r="F129" s="22">
         <v>1</v>
       </c>
       <c r="G129" s="3">
@@ -5400,10 +5409,10 @@
       <c r="D130" s="2">
         <v>0</v>
       </c>
-      <c r="E130" s="2">
-        <v>1</v>
-      </c>
-      <c r="F130" s="3">
+      <c r="E130" s="20">
+        <v>1</v>
+      </c>
+      <c r="F130" s="22">
         <v>1</v>
       </c>
       <c r="G130" s="3">
@@ -5426,10 +5435,10 @@
       <c r="D131" s="2">
         <v>0</v>
       </c>
-      <c r="E131" s="2">
-        <v>1</v>
-      </c>
-      <c r="F131" s="3">
+      <c r="E131" s="20">
+        <v>1</v>
+      </c>
+      <c r="F131" s="22">
         <v>1</v>
       </c>
       <c r="G131" s="3">
@@ -5452,10 +5461,10 @@
       <c r="D132" s="2">
         <v>0</v>
       </c>
-      <c r="E132" s="2">
-        <v>1</v>
-      </c>
-      <c r="F132" s="3">
+      <c r="E132" s="20">
+        <v>1</v>
+      </c>
+      <c r="F132" s="22">
         <v>1</v>
       </c>
       <c r="G132" s="3">
@@ -5478,10 +5487,10 @@
       <c r="D133" s="2">
         <v>0</v>
       </c>
-      <c r="E133" s="2">
-        <v>1</v>
-      </c>
-      <c r="F133" s="3">
+      <c r="E133" s="20">
+        <v>1</v>
+      </c>
+      <c r="F133" s="22">
         <v>1</v>
       </c>
       <c r="G133" s="3">
@@ -5504,10 +5513,10 @@
       <c r="D134" s="2">
         <v>0</v>
       </c>
-      <c r="E134" s="2">
-        <v>1</v>
-      </c>
-      <c r="F134" s="3">
+      <c r="E134" s="20">
+        <v>1</v>
+      </c>
+      <c r="F134" s="22">
         <v>1</v>
       </c>
       <c r="G134" s="3">
@@ -5530,10 +5539,10 @@
       <c r="D135" s="2">
         <v>0</v>
       </c>
-      <c r="E135" s="2">
-        <v>1</v>
-      </c>
-      <c r="F135" s="3">
+      <c r="E135" s="20">
+        <v>1</v>
+      </c>
+      <c r="F135" s="22">
         <v>1</v>
       </c>
       <c r="G135" s="3">
@@ -5556,10 +5565,10 @@
       <c r="D136" s="2">
         <v>0</v>
       </c>
-      <c r="E136" s="2">
-        <v>1</v>
-      </c>
-      <c r="F136" s="3">
+      <c r="E136" s="20">
+        <v>1</v>
+      </c>
+      <c r="F136" s="22">
         <v>1</v>
       </c>
       <c r="G136" s="3">
@@ -5582,10 +5591,10 @@
       <c r="D137" s="2">
         <v>0</v>
       </c>
-      <c r="E137" s="2">
-        <v>1</v>
-      </c>
-      <c r="F137" s="3">
+      <c r="E137" s="20">
+        <v>1</v>
+      </c>
+      <c r="F137" s="22">
         <v>1</v>
       </c>
       <c r="G137" s="3">
@@ -5608,10 +5617,10 @@
       <c r="D138" s="2">
         <v>0</v>
       </c>
-      <c r="E138" s="2">
-        <v>1</v>
-      </c>
-      <c r="F138" s="3">
+      <c r="E138" s="20">
+        <v>1</v>
+      </c>
+      <c r="F138" s="22">
         <v>1</v>
       </c>
       <c r="G138" s="3">
@@ -5634,10 +5643,10 @@
       <c r="D139" s="2">
         <v>0</v>
       </c>
-      <c r="E139" s="2">
-        <v>1</v>
-      </c>
-      <c r="F139" s="3">
+      <c r="E139" s="20">
+        <v>1</v>
+      </c>
+      <c r="F139" s="22">
         <v>1</v>
       </c>
       <c r="G139" s="3">
@@ -5660,10 +5669,10 @@
       <c r="D140" s="2">
         <v>0</v>
       </c>
-      <c r="E140" s="2">
-        <v>1</v>
-      </c>
-      <c r="F140" s="3">
+      <c r="E140" s="20">
+        <v>1</v>
+      </c>
+      <c r="F140" s="20">
         <v>1</v>
       </c>
       <c r="G140" s="3">
@@ -5686,10 +5695,10 @@
       <c r="D141" s="2">
         <v>0</v>
       </c>
-      <c r="E141" s="2">
-        <v>1</v>
-      </c>
-      <c r="F141" s="3">
+      <c r="E141" s="20">
+        <v>1</v>
+      </c>
+      <c r="F141" s="22">
         <v>1</v>
       </c>
       <c r="G141" s="3">
@@ -5712,10 +5721,10 @@
       <c r="D142" s="2">
         <v>0</v>
       </c>
-      <c r="E142" s="2">
-        <v>1</v>
-      </c>
-      <c r="F142" s="3">
+      <c r="E142" s="20">
+        <v>1</v>
+      </c>
+      <c r="F142" s="22">
         <v>1</v>
       </c>
       <c r="G142" s="3">
@@ -5738,10 +5747,10 @@
       <c r="D143" s="2">
         <v>0</v>
       </c>
-      <c r="E143" s="2">
-        <v>1</v>
-      </c>
-      <c r="F143" s="3">
+      <c r="E143" s="20">
+        <v>1</v>
+      </c>
+      <c r="F143" s="22">
         <v>1</v>
       </c>
       <c r="G143" s="3">
@@ -5764,10 +5773,10 @@
       <c r="D144" s="2">
         <v>0</v>
       </c>
-      <c r="E144" s="2">
-        <v>1</v>
-      </c>
-      <c r="F144" s="3">
+      <c r="E144" s="20">
+        <v>1</v>
+      </c>
+      <c r="F144" s="22">
         <v>1</v>
       </c>
       <c r="G144" s="3">
@@ -5790,10 +5799,10 @@
       <c r="D145" s="2">
         <v>0</v>
       </c>
-      <c r="E145" s="2">
-        <v>1</v>
-      </c>
-      <c r="F145" s="3">
+      <c r="E145" s="20">
+        <v>1</v>
+      </c>
+      <c r="F145" s="22">
         <v>1</v>
       </c>
       <c r="G145" s="3">
@@ -5816,10 +5825,10 @@
       <c r="D146" s="2">
         <v>0</v>
       </c>
-      <c r="E146" s="2">
-        <v>1</v>
-      </c>
-      <c r="F146" s="3">
+      <c r="E146" s="20">
+        <v>1</v>
+      </c>
+      <c r="F146" s="22">
         <v>1</v>
       </c>
       <c r="G146" s="3">
@@ -5842,10 +5851,10 @@
       <c r="D147" s="2">
         <v>0</v>
       </c>
-      <c r="E147" s="2">
-        <v>1</v>
-      </c>
-      <c r="F147" s="3">
+      <c r="E147" s="20">
+        <v>1</v>
+      </c>
+      <c r="F147" s="22">
         <v>1</v>
       </c>
       <c r="G147" s="3">
@@ -5868,10 +5877,10 @@
       <c r="D148" s="2">
         <v>0</v>
       </c>
-      <c r="E148" s="2">
-        <v>1</v>
-      </c>
-      <c r="F148" s="3">
+      <c r="E148" s="20">
+        <v>1</v>
+      </c>
+      <c r="F148" s="22">
         <v>1</v>
       </c>
       <c r="G148" s="3">
@@ -5894,10 +5903,10 @@
       <c r="D149" s="2">
         <v>0</v>
       </c>
-      <c r="E149" s="2">
-        <v>1</v>
-      </c>
-      <c r="F149" s="3">
+      <c r="E149" s="20">
+        <v>1</v>
+      </c>
+      <c r="F149" s="22">
         <v>1</v>
       </c>
       <c r="G149" s="3">
@@ -5920,10 +5929,10 @@
       <c r="D150" s="2">
         <v>0</v>
       </c>
-      <c r="E150" s="2">
-        <v>1</v>
-      </c>
-      <c r="F150" s="3">
+      <c r="E150" s="20">
+        <v>1</v>
+      </c>
+      <c r="F150" s="22">
         <v>1</v>
       </c>
       <c r="G150" s="3">
@@ -5946,10 +5955,10 @@
       <c r="D151" s="2">
         <v>0</v>
       </c>
-      <c r="E151" s="2">
-        <v>1</v>
-      </c>
-      <c r="F151" s="3">
+      <c r="E151" s="20">
+        <v>1</v>
+      </c>
+      <c r="F151" s="22">
         <v>1</v>
       </c>
       <c r="G151" s="3">
@@ -5972,10 +5981,10 @@
       <c r="D152" s="2">
         <v>0</v>
       </c>
-      <c r="E152" s="2">
-        <v>1</v>
-      </c>
-      <c r="F152" s="3">
+      <c r="E152" s="20">
+        <v>1</v>
+      </c>
+      <c r="F152" s="22">
         <v>1</v>
       </c>
       <c r="G152" s="3">
@@ -5998,10 +6007,10 @@
       <c r="D153" s="2">
         <v>0</v>
       </c>
-      <c r="E153" s="2">
-        <v>1</v>
-      </c>
-      <c r="F153" s="3">
+      <c r="E153" s="20">
+        <v>1</v>
+      </c>
+      <c r="F153" s="22">
         <v>1</v>
       </c>
       <c r="G153" s="3">
@@ -6024,10 +6033,10 @@
       <c r="D154" s="2">
         <v>0</v>
       </c>
-      <c r="E154" s="2">
-        <v>1</v>
-      </c>
-      <c r="F154" s="3">
+      <c r="E154" s="20">
+        <v>1</v>
+      </c>
+      <c r="F154" s="22">
         <v>1</v>
       </c>
       <c r="G154" s="3">
@@ -6050,10 +6059,10 @@
       <c r="D155" s="2">
         <v>0</v>
       </c>
-      <c r="E155" s="2">
-        <v>1</v>
-      </c>
-      <c r="F155" s="3">
+      <c r="E155" s="20">
+        <v>1</v>
+      </c>
+      <c r="F155" s="22">
         <v>1</v>
       </c>
       <c r="G155" s="3">
@@ -6076,10 +6085,10 @@
       <c r="D156" s="2">
         <v>0</v>
       </c>
-      <c r="E156" s="2">
-        <v>1</v>
-      </c>
-      <c r="F156" s="3">
+      <c r="E156" s="20">
+        <v>1</v>
+      </c>
+      <c r="F156" s="22">
         <v>1</v>
       </c>
       <c r="G156" s="3">
@@ -6102,10 +6111,10 @@
       <c r="D157" s="2">
         <v>0</v>
       </c>
-      <c r="E157" s="2">
-        <v>1</v>
-      </c>
-      <c r="F157" s="3">
+      <c r="E157" s="20">
+        <v>1</v>
+      </c>
+      <c r="F157" s="22">
         <v>1</v>
       </c>
       <c r="G157" s="3">
@@ -6128,10 +6137,10 @@
       <c r="D158" s="2">
         <v>0</v>
       </c>
-      <c r="E158" s="2">
-        <v>1</v>
-      </c>
-      <c r="F158" s="3">
+      <c r="E158" s="20">
+        <v>1</v>
+      </c>
+      <c r="F158" s="22">
         <v>1</v>
       </c>
       <c r="G158" s="3">
@@ -6154,10 +6163,10 @@
       <c r="D159" s="2">
         <v>0</v>
       </c>
-      <c r="E159" s="2">
-        <v>1</v>
-      </c>
-      <c r="F159" s="3">
+      <c r="E159" s="20">
+        <v>1</v>
+      </c>
+      <c r="F159" s="22">
         <v>1</v>
       </c>
       <c r="G159" s="3">
@@ -6180,10 +6189,10 @@
       <c r="D160" s="2">
         <v>0</v>
       </c>
-      <c r="E160" s="2">
-        <v>1</v>
-      </c>
-      <c r="F160" s="3">
+      <c r="E160" s="20">
+        <v>1</v>
+      </c>
+      <c r="F160" s="22">
         <v>1</v>
       </c>
       <c r="G160" s="3">
@@ -6206,10 +6215,10 @@
       <c r="D161" s="2">
         <v>0</v>
       </c>
-      <c r="E161" s="2">
-        <v>1</v>
-      </c>
-      <c r="F161" s="3">
+      <c r="E161" s="20">
+        <v>1</v>
+      </c>
+      <c r="F161" s="22">
         <v>1</v>
       </c>
       <c r="G161" s="3">
@@ -6232,10 +6241,10 @@
       <c r="D162" s="2">
         <v>0</v>
       </c>
-      <c r="E162" s="2">
-        <v>1</v>
-      </c>
-      <c r="F162" s="3">
+      <c r="E162" s="20">
+        <v>1</v>
+      </c>
+      <c r="F162" s="20">
         <v>1</v>
       </c>
       <c r="G162" s="3">
@@ -6258,10 +6267,10 @@
       <c r="D163" s="2">
         <v>0</v>
       </c>
-      <c r="E163" s="2">
-        <v>1</v>
-      </c>
-      <c r="F163" s="3">
+      <c r="E163" s="20">
+        <v>1</v>
+      </c>
+      <c r="F163" s="22">
         <v>1</v>
       </c>
       <c r="G163" s="3">
@@ -6284,10 +6293,10 @@
       <c r="D164" s="2">
         <v>0</v>
       </c>
-      <c r="E164" s="2">
-        <v>1</v>
-      </c>
-      <c r="F164" s="3">
+      <c r="E164" s="20">
+        <v>1</v>
+      </c>
+      <c r="F164" s="22">
         <v>1</v>
       </c>
       <c r="G164" s="3">
@@ -6310,10 +6319,10 @@
       <c r="D165" s="2">
         <v>0</v>
       </c>
-      <c r="E165" s="2">
-        <v>1</v>
-      </c>
-      <c r="F165" s="3">
+      <c r="E165" s="20">
+        <v>1</v>
+      </c>
+      <c r="F165" s="22">
         <v>1</v>
       </c>
       <c r="G165" s="3">
@@ -6336,10 +6345,10 @@
       <c r="D166" s="2">
         <v>0</v>
       </c>
-      <c r="E166" s="2">
-        <v>1</v>
-      </c>
-      <c r="F166" s="3">
+      <c r="E166" s="20">
+        <v>1</v>
+      </c>
+      <c r="F166" s="22">
         <v>1</v>
       </c>
       <c r="G166" s="3">
@@ -6362,10 +6371,10 @@
       <c r="D167" s="2">
         <v>0</v>
       </c>
-      <c r="E167" s="2">
-        <v>1</v>
-      </c>
-      <c r="F167" s="3">
+      <c r="E167" s="20">
+        <v>1</v>
+      </c>
+      <c r="F167" s="22">
         <v>1</v>
       </c>
       <c r="G167" s="3">
@@ -6388,10 +6397,10 @@
       <c r="D168" s="2">
         <v>0</v>
       </c>
-      <c r="E168" s="2">
-        <v>1</v>
-      </c>
-      <c r="F168" s="3">
+      <c r="E168" s="20">
+        <v>1</v>
+      </c>
+      <c r="F168" s="22">
         <v>1</v>
       </c>
       <c r="G168" s="3">
@@ -6414,10 +6423,10 @@
       <c r="D169" s="2">
         <v>0</v>
       </c>
-      <c r="E169" s="2">
-        <v>1</v>
-      </c>
-      <c r="F169" s="3">
+      <c r="E169" s="20">
+        <v>1</v>
+      </c>
+      <c r="F169" s="22">
         <v>1</v>
       </c>
       <c r="G169" s="3">
@@ -6440,10 +6449,10 @@
       <c r="D170" s="2">
         <v>0</v>
       </c>
-      <c r="E170" s="2">
-        <v>1</v>
-      </c>
-      <c r="F170" s="3">
+      <c r="E170" s="20">
+        <v>1</v>
+      </c>
+      <c r="F170" s="22">
         <v>1</v>
       </c>
       <c r="G170" s="3">
@@ -6466,10 +6475,10 @@
       <c r="D171" s="2">
         <v>0</v>
       </c>
-      <c r="E171" s="2">
-        <v>1</v>
-      </c>
-      <c r="F171" s="3">
+      <c r="E171" s="20">
+        <v>1</v>
+      </c>
+      <c r="F171" s="22">
         <v>1</v>
       </c>
       <c r="G171" s="3">
@@ -6492,10 +6501,10 @@
       <c r="D172" s="2">
         <v>0</v>
       </c>
-      <c r="E172" s="2">
-        <v>1</v>
-      </c>
-      <c r="F172" s="3">
+      <c r="E172" s="20">
+        <v>1</v>
+      </c>
+      <c r="F172" s="22">
         <v>1</v>
       </c>
       <c r="G172" s="3">
@@ -6518,10 +6527,10 @@
       <c r="D173" s="2">
         <v>0</v>
       </c>
-      <c r="E173" s="2">
-        <v>1</v>
-      </c>
-      <c r="F173" s="3">
+      <c r="E173" s="20">
+        <v>1</v>
+      </c>
+      <c r="F173" s="22">
         <v>1</v>
       </c>
       <c r="G173" s="3">
@@ -6544,10 +6553,10 @@
       <c r="D174" s="2">
         <v>0</v>
       </c>
-      <c r="E174" s="2">
-        <v>1</v>
-      </c>
-      <c r="F174" s="3">
+      <c r="E174" s="20">
+        <v>1</v>
+      </c>
+      <c r="F174" s="22">
         <v>1</v>
       </c>
       <c r="G174" s="3">
@@ -6570,10 +6579,10 @@
       <c r="D175" s="2">
         <v>0</v>
       </c>
-      <c r="E175" s="2">
-        <v>1</v>
-      </c>
-      <c r="F175" s="3">
+      <c r="E175" s="20">
+        <v>1</v>
+      </c>
+      <c r="F175" s="22">
         <v>1</v>
       </c>
       <c r="G175" s="3">
@@ -6596,10 +6605,10 @@
       <c r="D176" s="2">
         <v>0</v>
       </c>
-      <c r="E176" s="2">
-        <v>1</v>
-      </c>
-      <c r="F176" s="3">
+      <c r="E176" s="20">
+        <v>1</v>
+      </c>
+      <c r="F176" s="22">
         <v>1</v>
       </c>
       <c r="G176" s="3">
@@ -6622,10 +6631,10 @@
       <c r="D177" s="2">
         <v>0</v>
       </c>
-      <c r="E177" s="2">
-        <v>1</v>
-      </c>
-      <c r="F177" s="3">
+      <c r="E177" s="20">
+        <v>1</v>
+      </c>
+      <c r="F177" s="22">
         <v>1</v>
       </c>
       <c r="G177" s="3">
@@ -6648,10 +6657,10 @@
       <c r="D178" s="2">
         <v>0</v>
       </c>
-      <c r="E178" s="2">
-        <v>1</v>
-      </c>
-      <c r="F178" s="3">
+      <c r="E178" s="20">
+        <v>1</v>
+      </c>
+      <c r="F178" s="22">
         <v>1</v>
       </c>
       <c r="G178" s="3">
@@ -6674,10 +6683,10 @@
       <c r="D179" s="2">
         <v>0</v>
       </c>
-      <c r="E179" s="2">
-        <v>1</v>
-      </c>
-      <c r="F179" s="3">
+      <c r="E179" s="20">
+        <v>1</v>
+      </c>
+      <c r="F179" s="20">
         <v>1</v>
       </c>
       <c r="G179" s="3">

</xml_diff>

<commit_message>
Fix breaklines in names for CSV export
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -2285,8 +2285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update quality check report
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="619">
   <si>
     <t>old</t>
   </si>
@@ -1863,6 +1863,24 @@
   </si>
   <si>
     <t>crfs-t02b-a4_a_10a</t>
+  </si>
+  <si>
+    <t>crfs-t09a2-i2_1b</t>
+  </si>
+  <si>
+    <t>ref_facility</t>
+  </si>
+  <si>
+    <t>i2_1b</t>
+  </si>
+  <si>
+    <t>crfs-t09a2-i2_1o</t>
+  </si>
+  <si>
+    <t>ref_facility_oth</t>
+  </si>
+  <si>
+    <t>i2_1o</t>
   </si>
 </sst>
 </file>
@@ -2283,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H208"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6592,10 +6610,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>454</v>
-      </c>
-      <c r="B166" s="15" t="s">
-        <v>128</v>
+        <v>613</v>
+      </c>
+      <c r="B166" s="14" t="s">
+        <v>614</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6610,18 +6628,18 @@
         <v>1</v>
       </c>
       <c r="G166" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>293</v>
+        <v>615</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
-        <v>455</v>
-      </c>
-      <c r="B167" s="15" t="s">
-        <v>129</v>
+        <v>616</v>
+      </c>
+      <c r="B167" s="14" t="s">
+        <v>617</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6636,18 +6654,18 @@
         <v>1</v>
       </c>
       <c r="G167" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>294</v>
+        <v>618</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B168" s="14" t="s">
-        <v>130</v>
+        <v>454</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6665,15 +6683,15 @@
         <v>0</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="B169" s="14" t="s">
-        <v>131</v>
+        <v>455</v>
+      </c>
+      <c r="B169" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6684,22 +6702,22 @@
       <c r="E169" s="20">
         <v>1</v>
       </c>
-      <c r="F169" s="20">
+      <c r="F169" s="22">
         <v>1</v>
       </c>
       <c r="G169" s="3">
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6717,15 +6735,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6736,22 +6754,22 @@
       <c r="E171" s="20">
         <v>1</v>
       </c>
-      <c r="F171" s="22">
+      <c r="F171" s="20">
         <v>1</v>
       </c>
       <c r="G171" s="3">
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6766,18 +6784,18 @@
         <v>1</v>
       </c>
       <c r="G172" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6792,18 +6810,18 @@
         <v>1</v>
       </c>
       <c r="G173" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6818,18 +6836,18 @@
         <v>1</v>
       </c>
       <c r="G174" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6844,18 +6862,18 @@
         <v>1</v>
       </c>
       <c r="G175" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6873,15 +6891,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6899,15 +6917,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6925,15 +6943,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6951,15 +6969,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -6977,15 +6995,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7003,15 +7021,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7029,15 +7047,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7055,15 +7073,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7081,15 +7099,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7107,15 +7125,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7133,15 +7151,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7159,15 +7177,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7185,15 +7203,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7211,15 +7229,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7237,15 +7255,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7256,22 +7274,22 @@
       <c r="E191" s="20">
         <v>1</v>
       </c>
-      <c r="F191" s="20">
+      <c r="F191" s="22">
         <v>1</v>
       </c>
       <c r="G191" s="3">
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7289,15 +7307,15 @@
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7308,22 +7326,22 @@
       <c r="E193" s="20">
         <v>1</v>
       </c>
-      <c r="F193" s="22">
+      <c r="F193" s="20">
         <v>1</v>
       </c>
       <c r="G193" s="3">
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7341,15 +7359,15 @@
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7367,15 +7385,15 @@
         <v>0</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7393,15 +7411,15 @@
         <v>0</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7419,15 +7437,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7445,15 +7463,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7471,93 +7489,93 @@
         <v>0</v>
       </c>
       <c r="H199" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C200" s="2">
+        <v>0</v>
+      </c>
+      <c r="D200" s="2">
+        <v>0</v>
+      </c>
+      <c r="E200" s="20">
+        <v>1</v>
+      </c>
+      <c r="F200" s="22">
+        <v>1</v>
+      </c>
+      <c r="G200" s="3">
+        <v>0</v>
+      </c>
+      <c r="H200" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C201" s="2">
+        <v>0</v>
+      </c>
+      <c r="D201" s="2">
+        <v>0</v>
+      </c>
+      <c r="E201" s="20">
+        <v>1</v>
+      </c>
+      <c r="F201" s="22">
+        <v>1</v>
+      </c>
+      <c r="G201" s="3">
+        <v>0</v>
+      </c>
+      <c r="H201" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="17" t="s">
         <v>488</v>
       </c>
-      <c r="B200" s="14" t="s">
+      <c r="B202" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C200" s="2">
-        <v>0</v>
-      </c>
-      <c r="D200" s="2">
-        <v>0</v>
-      </c>
-      <c r="E200" s="20">
-        <v>1</v>
-      </c>
-      <c r="F200" s="22">
-        <v>1</v>
-      </c>
-      <c r="G200" s="3">
-        <v>0</v>
-      </c>
-      <c r="H200" s="17" t="s">
+      <c r="C202" s="2">
+        <v>0</v>
+      </c>
+      <c r="D202" s="2">
+        <v>0</v>
+      </c>
+      <c r="E202" s="20">
+        <v>1</v>
+      </c>
+      <c r="F202" s="22">
+        <v>1</v>
+      </c>
+      <c r="G202" s="3">
+        <v>0</v>
+      </c>
+      <c r="H202" s="17" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A201" s="18" t="s">
-        <v>489</v>
-      </c>
-      <c r="B201" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C201" s="2">
-        <v>0</v>
-      </c>
-      <c r="D201" s="2">
-        <v>0</v>
-      </c>
-      <c r="E201" s="20">
-        <v>1</v>
-      </c>
-      <c r="F201" s="22">
-        <v>1</v>
-      </c>
-      <c r="G201" s="3">
-        <v>0</v>
-      </c>
-      <c r="H201" s="18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A202" s="18" t="s">
-        <v>490</v>
-      </c>
-      <c r="B202" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C202" s="2">
-        <v>0</v>
-      </c>
-      <c r="D202" s="2">
-        <v>0</v>
-      </c>
-      <c r="E202" s="20">
-        <v>1</v>
-      </c>
-      <c r="F202" s="22">
-        <v>1</v>
-      </c>
-      <c r="G202" s="3">
-        <v>0</v>
-      </c>
-      <c r="H202" s="18" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B203" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C203" s="2">
         <v>0</v>
@@ -7575,15 +7593,15 @@
         <v>0</v>
       </c>
       <c r="H203" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7601,15 +7619,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7627,15 +7645,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7653,15 +7671,15 @@
         <v>0</v>
       </c>
       <c r="H206" s="18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C207" s="2">
         <v>0</v>
@@ -7679,32 +7697,84 @@
         <v>0</v>
       </c>
       <c r="H207" s="18" t="s">
-        <v>214</v>
+        <v>332</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="B208" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C208" s="2">
+        <v>0</v>
+      </c>
+      <c r="D208" s="2">
+        <v>0</v>
+      </c>
+      <c r="E208" s="20">
+        <v>1</v>
+      </c>
+      <c r="F208" s="22">
+        <v>1</v>
+      </c>
+      <c r="G208" s="3">
+        <v>0</v>
+      </c>
+      <c r="H208" s="18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="B209" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C209" s="2">
+        <v>0</v>
+      </c>
+      <c r="D209" s="2">
+        <v>0</v>
+      </c>
+      <c r="E209" s="20">
+        <v>1</v>
+      </c>
+      <c r="F209" s="22">
+        <v>1</v>
+      </c>
+      <c r="G209" s="3">
+        <v>0</v>
+      </c>
+      <c r="H209" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="18" t="s">
         <v>496</v>
       </c>
-      <c r="B208" s="16" t="s">
+      <c r="B210" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C208" s="2">
-        <v>0</v>
-      </c>
-      <c r="D208" s="2">
-        <v>0</v>
-      </c>
-      <c r="E208" s="20">
-        <v>1</v>
-      </c>
-      <c r="F208" s="20">
-        <v>1</v>
-      </c>
-      <c r="G208" s="3">
-        <v>0</v>
-      </c>
-      <c r="H208" s="18" t="s">
+      <c r="C210" s="2">
+        <v>0</v>
+      </c>
+      <c r="D210" s="2">
+        <v>0</v>
+      </c>
+      <c r="E210" s="20">
+        <v>1</v>
+      </c>
+      <c r="F210" s="20">
+        <v>1</v>
+      </c>
+      <c r="G210" s="3">
+        <v>0</v>
+      </c>
+      <c r="H210" s="18" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update export / quality checks
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="622">
   <si>
     <t>old</t>
   </si>
@@ -872,9 +872,6 @@
     <t>fu</t>
   </si>
   <si>
-    <t>injection</t>
-  </si>
-  <si>
     <t>injection_types</t>
   </si>
   <si>
@@ -1358,9 +1355,6 @@
     <t>crfs-t09a1-fu</t>
   </si>
   <si>
-    <t>crfs-t09a1-injection</t>
-  </si>
-  <si>
     <t>crfs-t09a1-injection_types</t>
   </si>
   <si>
@@ -1376,9 +1370,6 @@
     <t>crfs-t09a1-h2_2o</t>
   </si>
   <si>
-    <t>crfs-t09a2-b1_9</t>
-  </si>
-  <si>
     <t>crfs-t09a2-g3_1</t>
   </si>
   <si>
@@ -1715,114 +1706,6 @@
     <t>dx_mlist</t>
   </si>
   <si>
-    <t>paracetamol_route</t>
-  </si>
-  <si>
-    <t>artesunate_route</t>
-  </si>
-  <si>
-    <t>ciprofloxacin_route</t>
-  </si>
-  <si>
-    <t>metronidazol_route</t>
-  </si>
-  <si>
-    <t>quinine_route</t>
-  </si>
-  <si>
-    <t>salbutamol_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxsevere</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxpneumonia</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxpneumoniaseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxdiarrhoea</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxdiarrhoeaseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxdiarrhoeaduration</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxdehydration</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxdehydrationseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxmalaria</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxmalariaseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxearinfection</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxearinfectionduration</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxmalnutrition</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxmalnuseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxanaemia</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxanaemiaseverity</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxothermain</t>
-  </si>
-  <si>
-    <t>crfs-t09a2-rxother</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-paracetamol_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-artesunate_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-ciprofloxacin_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-metronidazol_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-quinine_route</t>
-  </si>
-  <si>
-    <t>crfs-t09a1-salbutamol_route</t>
-  </si>
-  <si>
-    <t>rx_paracetamol_route</t>
-  </si>
-  <si>
-    <t>rx_artesunate_route</t>
-  </si>
-  <si>
-    <t>rx_ciprofloxacin_route</t>
-  </si>
-  <si>
-    <t>rx_metronidazol_route</t>
-  </si>
-  <si>
-    <t>rx_quinine_route</t>
-  </si>
-  <si>
-    <t>rx_salbutamol_route</t>
-  </si>
-  <si>
     <t>crfs-t09a2-g3_1o</t>
   </si>
   <si>
@@ -1881,6 +1764,132 @@
   </si>
   <si>
     <t>i2_1o</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxsevere</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxpneumonia</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxpneumoniaseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxdiarrhoea</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxdiarrhoeaseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxdiarrhoeaduration</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxdehydration</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxdehydrationseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxmalaria</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxmalariaseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxearinfection</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxearinfectionduration</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxmalnutrition</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxmalnuseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxanaemia</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxanaemiaseverity</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxothermain</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t09a2-rxother</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-paracetamol_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-artesunate_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-ciprofloxacin_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-metronidazol_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-quinine_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-salbutamol_route_hf</t>
+  </si>
+  <si>
+    <t>rx_paracetamol_route_hf</t>
+  </si>
+  <si>
+    <t>rx_artesunate_route_hf</t>
+  </si>
+  <si>
+    <t>rx_ciprofloxacin_route_hf</t>
+  </si>
+  <si>
+    <t>rx_metronidazol_route_hf</t>
+  </si>
+  <si>
+    <t>rx_quinine_route_hf</t>
+  </si>
+  <si>
+    <t>rx_salbutamol_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-medication_injection</t>
+  </si>
+  <si>
+    <t>inj_vacc</t>
+  </si>
+  <si>
+    <t>vaccination_injection</t>
+  </si>
+  <si>
+    <t>medication_injection</t>
+  </si>
+  <si>
+    <t>paracetamol_route_hf</t>
+  </si>
+  <si>
+    <t>artesunate_route_hf</t>
+  </si>
+  <si>
+    <t>ciprofloxacin_route_hf</t>
+  </si>
+  <si>
+    <t>metronidazol_route_hf</t>
+  </si>
+  <si>
+    <t>quinine_route_hf</t>
+  </si>
+  <si>
+    <t>salbutamol_route_hf</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-b1_9</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-vaccine_injection</t>
   </si>
 </sst>
 </file>
@@ -2301,15 +2310,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
@@ -2338,7 +2347,7 @@
         <v>172</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>194</v>
@@ -2424,7 +2433,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>173</v>
@@ -2445,15 +2454,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>600</v>
+        <v>561</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>600</v>
+        <v>561</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2471,12 +2480,12 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>600</v>
+        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>21</v>
@@ -2502,7 +2511,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>35</v>
@@ -2528,10 +2537,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2549,12 +2558,12 @@
         <v>0</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>36</v>
@@ -2580,7 +2589,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>37</v>
@@ -2606,7 +2615,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>9</v>
@@ -2632,10 +2641,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -2653,12 +2662,12 @@
         <v>0</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>29</v>
@@ -2684,7 +2693,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>2</v>
@@ -2710,7 +2719,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>14</v>
@@ -2736,10 +2745,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -2757,12 +2766,12 @@
         <v>0</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>11</v>
@@ -2788,7 +2797,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>12</v>
@@ -2814,7 +2823,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>10</v>
@@ -2840,7 +2849,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>23</v>
@@ -2866,7 +2875,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>24</v>
@@ -2892,7 +2901,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>8</v>
@@ -2918,7 +2927,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>38</v>
@@ -2944,7 +2953,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>22</v>
@@ -2970,7 +2979,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>13</v>
@@ -2996,7 +3005,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>15</v>
@@ -3022,7 +3031,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>4</v>
@@ -3048,7 +3057,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>6</v>
@@ -3074,7 +3083,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>16</v>
@@ -3100,7 +3109,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>5</v>
@@ -3126,10 +3135,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -3147,15 +3156,15 @@
         <v>1</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -3173,12 +3182,12 @@
         <v>0</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>17</v>
@@ -3204,7 +3213,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>46</v>
@@ -3230,7 +3239,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>47</v>
@@ -3256,7 +3265,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>48</v>
@@ -3282,7 +3291,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>49</v>
@@ -3308,7 +3317,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>50</v>
@@ -3334,7 +3343,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>18</v>
@@ -3360,7 +3369,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>19</v>
@@ -3386,7 +3395,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>20</v>
@@ -3412,7 +3421,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>3</v>
@@ -3438,7 +3447,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>30</v>
@@ -3464,7 +3473,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>32</v>
@@ -3490,10 +3499,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -3511,12 +3520,12 @@
         <v>1</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>33</v>
@@ -3542,7 +3551,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>34</v>
@@ -3568,7 +3577,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>43</v>
@@ -3594,10 +3603,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>612</v>
+        <v>573</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>610</v>
+        <v>571</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -3615,12 +3624,12 @@
         <v>1</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>611</v>
+        <v>572</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>39</v>
@@ -3646,7 +3655,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>40</v>
@@ -3672,10 +3681,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -3693,15 +3702,15 @@
         <v>0</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -3719,15 +3728,15 @@
         <v>0</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
@@ -3745,12 +3754,12 @@
         <v>0</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>41</v>
@@ -3776,7 +3785,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>42</v>
@@ -3802,7 +3811,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>44</v>
@@ -3828,7 +3837,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>45</v>
@@ -3854,10 +3863,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C60" s="2">
         <v>1</v>
@@ -3875,15 +3884,15 @@
         <v>1</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C61" s="2">
         <v>1</v>
@@ -3901,15 +3910,15 @@
         <v>1</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C62" s="2">
         <v>1</v>
@@ -3927,15 +3936,15 @@
         <v>1</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>601</v>
+        <v>562</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>602</v>
+        <v>563</v>
       </c>
       <c r="C63" s="2">
         <v>1</v>
@@ -3953,15 +3962,15 @@
         <v>1</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>603</v>
+        <v>564</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>604</v>
+        <v>565</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>606</v>
+        <v>567</v>
       </c>
       <c r="C64" s="2">
         <v>1</v>
@@ -3979,15 +3988,15 @@
         <v>1</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>608</v>
+        <v>569</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>605</v>
+        <v>566</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>607</v>
+        <v>568</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -4005,12 +4014,12 @@
         <v>1</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>609</v>
+        <v>570</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>52</v>
@@ -4036,7 +4045,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>53</v>
@@ -4062,7 +4071,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>54</v>
@@ -4088,7 +4097,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>55</v>
@@ -4114,7 +4123,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>56</v>
@@ -4140,7 +4149,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>57</v>
@@ -4166,7 +4175,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>58</v>
@@ -4192,7 +4201,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>59</v>
@@ -4218,7 +4227,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>60</v>
@@ -4244,7 +4253,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>61</v>
@@ -4270,7 +4279,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>62</v>
@@ -4296,7 +4305,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>63</v>
@@ -4322,7 +4331,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>64</v>
@@ -4348,7 +4357,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>65</v>
@@ -4374,7 +4383,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>66</v>
@@ -4400,7 +4409,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>67</v>
@@ -4426,7 +4435,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>68</v>
@@ -4452,7 +4461,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>69</v>
@@ -4478,7 +4487,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>70</v>
@@ -4504,7 +4513,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>71</v>
@@ -4530,7 +4539,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>72</v>
@@ -4556,7 +4565,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>73</v>
@@ -4582,7 +4591,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>74</v>
@@ -4608,7 +4617,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>75</v>
@@ -4634,7 +4643,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>76</v>
@@ -4660,7 +4669,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>77</v>
@@ -4686,7 +4695,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>78</v>
@@ -4712,7 +4721,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>79</v>
@@ -4738,7 +4747,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>80</v>
@@ -4764,7 +4773,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>81</v>
@@ -4790,7 +4799,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>82</v>
@@ -4816,7 +4825,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>83</v>
@@ -4842,7 +4851,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>84</v>
@@ -4868,7 +4877,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>85</v>
@@ -4894,7 +4903,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>86</v>
@@ -4920,7 +4929,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>87</v>
@@ -4946,7 +4955,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>88</v>
@@ -4972,7 +4981,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B103" s="14" t="s">
         <v>89</v>
@@ -4998,7 +5007,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B104" s="14" t="s">
         <v>90</v>
@@ -5024,7 +5033,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>91</v>
@@ -5050,7 +5059,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>92</v>
@@ -5076,7 +5085,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>93</v>
@@ -5102,7 +5111,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B108" s="14" t="s">
         <v>94</v>
@@ -5128,7 +5137,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>95</v>
@@ -5154,7 +5163,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B110" s="14" t="s">
         <v>96</v>
@@ -5180,7 +5189,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B111" s="14" t="s">
         <v>97</v>
@@ -5206,7 +5215,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>98</v>
@@ -5232,7 +5241,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>99</v>
@@ -5258,7 +5267,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>100</v>
@@ -5284,7 +5293,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>101</v>
@@ -5310,7 +5319,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>102</v>
@@ -5336,7 +5345,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>103</v>
@@ -5362,7 +5371,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>104</v>
@@ -5388,7 +5397,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>105</v>
@@ -5414,7 +5423,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>106</v>
@@ -5440,7 +5449,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>107</v>
@@ -5466,7 +5475,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B122" s="15" t="s">
         <v>108</v>
@@ -5492,7 +5501,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>109</v>
@@ -5518,7 +5527,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>110</v>
@@ -5544,7 +5553,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>111</v>
@@ -5570,7 +5579,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>112</v>
@@ -5596,7 +5605,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>113</v>
@@ -5622,7 +5631,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B128" s="14" t="s">
         <v>114</v>
@@ -5648,7 +5657,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>115</v>
@@ -5674,7 +5683,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B130" s="14" t="s">
         <v>116</v>
@@ -5700,7 +5709,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
-        <v>444</v>
+        <v>610</v>
       </c>
       <c r="B131" s="14" t="s">
         <v>117</v>
@@ -5721,12 +5730,12 @@
         <v>0</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>282</v>
+        <v>613</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B132" s="14" t="s">
         <v>118</v>
@@ -5747,12 +5756,12 @@
         <v>0</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B133" s="14" t="s">
         <v>119</v>
@@ -5773,15 +5782,15 @@
         <v>0</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
-        <v>447</v>
+        <v>621</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>120</v>
+        <v>611</v>
       </c>
       <c r="C134" s="2">
         <v>0</v>
@@ -5799,15 +5808,15 @@
         <v>0</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>285</v>
+        <v>612</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -5825,42 +5834,42 @@
         <v>0</v>
       </c>
       <c r="H135" s="17" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B136" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C136" s="2">
+        <v>0</v>
+      </c>
+      <c r="D136" s="2">
+        <v>0</v>
+      </c>
+      <c r="E136" s="20">
+        <v>1</v>
+      </c>
+      <c r="F136" s="22">
+        <v>1</v>
+      </c>
+      <c r="G136" s="3">
+        <v>0</v>
+      </c>
+      <c r="H136" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B137" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C136" s="2">
-        <v>0</v>
-      </c>
-      <c r="D136" s="2">
-        <v>0</v>
-      </c>
-      <c r="E136" s="20">
-        <v>1</v>
-      </c>
-      <c r="F136" s="22">
-        <v>1</v>
-      </c>
-      <c r="G136" s="3">
-        <v>0</v>
-      </c>
-      <c r="H136" s="17" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="18" t="s">
-        <v>587</v>
-      </c>
-      <c r="B137" s="16" t="s">
-        <v>593</v>
-      </c>
       <c r="C137" s="2">
         <v>0</v>
       </c>
@@ -5870,22 +5879,22 @@
       <c r="E137" s="20">
         <v>1</v>
       </c>
-      <c r="F137" s="20">
+      <c r="F137" s="22">
         <v>1</v>
       </c>
       <c r="G137" s="3">
         <v>0</v>
       </c>
-      <c r="H137" s="18" t="s">
-        <v>563</v>
+      <c r="H137" s="17" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5903,15 +5912,15 @@
         <v>0</v>
       </c>
       <c r="H138" s="18" t="s">
-        <v>564</v>
+        <v>614</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -5929,15 +5938,15 @@
         <v>0</v>
       </c>
       <c r="H139" s="18" t="s">
-        <v>565</v>
+        <v>615</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="18" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="C140" s="2">
         <v>0</v>
@@ -5955,15 +5964,15 @@
         <v>0</v>
       </c>
       <c r="H140" s="18" t="s">
-        <v>566</v>
+        <v>616</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="18" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>597</v>
+        <v>607</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -5981,15 +5990,15 @@
         <v>0</v>
       </c>
       <c r="H141" s="18" t="s">
-        <v>567</v>
+        <v>617</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
-        <v>592</v>
+        <v>602</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -6007,15 +6016,15 @@
         <v>0</v>
       </c>
       <c r="H142" s="18" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="17" t="s">
-        <v>450</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>123</v>
+      <c r="A143" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>609</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -6026,22 +6035,22 @@
       <c r="E143" s="20">
         <v>1</v>
       </c>
-      <c r="F143" s="22">
+      <c r="F143" s="20">
         <v>1</v>
       </c>
       <c r="G143" s="3">
         <v>0</v>
       </c>
-      <c r="H143" s="17" t="s">
-        <v>288</v>
+      <c r="H143" s="18" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>569</v>
-      </c>
-      <c r="B144" s="23" t="s">
-        <v>545</v>
+        <v>620</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6049,7 +6058,7 @@
       <c r="D144" s="2">
         <v>0</v>
       </c>
-      <c r="E144" s="4">
+      <c r="E144" s="20">
         <v>1</v>
       </c>
       <c r="F144" s="22">
@@ -6059,15 +6068,15 @@
         <v>0</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>527</v>
+        <v>287</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6085,15 +6094,15 @@
         <v>0</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6111,15 +6120,15 @@
         <v>0</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6137,15 +6146,15 @@
         <v>0</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6163,15 +6172,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6189,15 +6198,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6215,15 +6224,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6241,15 +6250,15 @@
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>577</v>
+        <v>587</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6267,15 +6276,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6293,15 +6302,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6319,15 +6328,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6345,15 +6354,15 @@
         <v>0</v>
       </c>
       <c r="H155" s="17" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -6371,15 +6380,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="17" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6397,15 +6406,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="17" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6423,15 +6432,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6449,15 +6458,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6475,15 +6484,15 @@
         <v>0</v>
       </c>
       <c r="H160" s="17" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6501,15 +6510,15 @@
         <v>0</v>
       </c>
       <c r="H161" s="17" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="B162" s="14" t="s">
-        <v>124</v>
+        <v>597</v>
+      </c>
+      <c r="B162" s="23" t="s">
+        <v>558</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6517,7 +6526,7 @@
       <c r="D162" s="2">
         <v>0</v>
       </c>
-      <c r="E162" s="20">
+      <c r="E162" s="4">
         <v>1</v>
       </c>
       <c r="F162" s="22">
@@ -6527,15 +6536,15 @@
         <v>0</v>
       </c>
       <c r="H162" s="17" t="s">
-        <v>289</v>
+        <v>541</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>599</v>
+        <v>448</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6553,15 +6562,15 @@
         <v>0</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>452</v>
+        <v>560</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6576,18 +6585,18 @@
         <v>1</v>
       </c>
       <c r="G164" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H164" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6605,15 +6614,15 @@
         <v>1</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>613</v>
+        <v>450</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>614</v>
+        <v>127</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6631,15 +6640,15 @@
         <v>1</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>615</v>
+        <v>291</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
-        <v>616</v>
+        <v>574</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>617</v>
+        <v>575</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6657,15 +6666,15 @@
         <v>1</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>618</v>
+        <v>576</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
-        <v>454</v>
-      </c>
-      <c r="B168" s="15" t="s">
-        <v>128</v>
+        <v>577</v>
+      </c>
+      <c r="B168" s="14" t="s">
+        <v>578</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6680,18 +6689,18 @@
         <v>1</v>
       </c>
       <c r="G168" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>293</v>
+        <v>579</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6709,15 +6718,15 @@
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B170" s="14" t="s">
-        <v>130</v>
+        <v>452</v>
+      </c>
+      <c r="B170" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6735,15 +6744,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6754,22 +6763,22 @@
       <c r="E171" s="20">
         <v>1</v>
       </c>
-      <c r="F171" s="20">
+      <c r="F171" s="22">
         <v>1</v>
       </c>
       <c r="G171" s="3">
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6780,22 +6789,22 @@
       <c r="E172" s="20">
         <v>1</v>
       </c>
-      <c r="F172" s="22">
+      <c r="F172" s="20">
         <v>1</v>
       </c>
       <c r="G172" s="3">
         <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6813,15 +6822,15 @@
         <v>0</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6836,18 +6845,18 @@
         <v>1</v>
       </c>
       <c r="G174" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6865,15 +6874,15 @@
         <v>1</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6888,18 +6897,18 @@
         <v>1</v>
       </c>
       <c r="G176" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6917,15 +6926,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6943,15 +6952,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6969,15 +6978,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -6995,15 +7004,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7021,15 +7030,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7047,15 +7056,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7073,15 +7082,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7099,15 +7108,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7125,15 +7134,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7151,15 +7160,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7177,15 +7186,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7203,15 +7212,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7229,15 +7238,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7255,15 +7264,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7281,15 +7290,15 @@
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7307,15 +7316,15 @@
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7326,22 +7335,22 @@
       <c r="E193" s="20">
         <v>1</v>
       </c>
-      <c r="F193" s="20">
+      <c r="F193" s="22">
         <v>1</v>
       </c>
       <c r="G193" s="3">
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7352,22 +7361,22 @@
       <c r="E194" s="20">
         <v>1</v>
       </c>
-      <c r="F194" s="22">
+      <c r="F194" s="20">
         <v>1</v>
       </c>
       <c r="G194" s="3">
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7385,15 +7394,15 @@
         <v>0</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7411,15 +7420,15 @@
         <v>0</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7437,15 +7446,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7463,15 +7472,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7489,15 +7498,15 @@
         <v>0</v>
       </c>
       <c r="H199" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="17" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C200" s="2">
         <v>0</v>
@@ -7515,15 +7524,15 @@
         <v>0</v>
       </c>
       <c r="H200" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="17" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B201" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C201" s="2">
         <v>0</v>
@@ -7541,42 +7550,42 @@
         <v>0</v>
       </c>
       <c r="H201" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="17" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B202" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C202" s="2">
+        <v>0</v>
+      </c>
+      <c r="D202" s="2">
+        <v>0</v>
+      </c>
+      <c r="E202" s="20">
+        <v>1</v>
+      </c>
+      <c r="F202" s="22">
+        <v>1</v>
+      </c>
+      <c r="G202" s="3">
+        <v>0</v>
+      </c>
+      <c r="H202" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="B203" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C202" s="2">
-        <v>0</v>
-      </c>
-      <c r="D202" s="2">
-        <v>0</v>
-      </c>
-      <c r="E202" s="20">
-        <v>1</v>
-      </c>
-      <c r="F202" s="22">
-        <v>1</v>
-      </c>
-      <c r="G202" s="3">
-        <v>0</v>
-      </c>
-      <c r="H202" s="17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A203" s="18" t="s">
-        <v>489</v>
-      </c>
-      <c r="B203" s="16" t="s">
-        <v>163</v>
-      </c>
       <c r="C203" s="2">
         <v>0</v>
       </c>
@@ -7592,16 +7601,16 @@
       <c r="G203" s="3">
         <v>0</v>
       </c>
-      <c r="H203" s="18" t="s">
-        <v>328</v>
+      <c r="H203" s="17" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7619,15 +7628,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7645,15 +7654,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7671,15 +7680,15 @@
         <v>0</v>
       </c>
       <c r="H206" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C207" s="2">
         <v>0</v>
@@ -7697,15 +7706,15 @@
         <v>0</v>
       </c>
       <c r="H207" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="18" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B208" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C208" s="2">
         <v>0</v>
@@ -7723,15 +7732,15 @@
         <v>0</v>
       </c>
       <c r="H208" s="18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="18" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B209" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C209" s="2">
         <v>0</v>
@@ -7749,32 +7758,58 @@
         <v>0</v>
       </c>
       <c r="H209" s="18" t="s">
-        <v>214</v>
+        <v>332</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B210" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C210" s="2">
+        <v>0</v>
+      </c>
+      <c r="D210" s="2">
+        <v>0</v>
+      </c>
+      <c r="E210" s="20">
+        <v>1</v>
+      </c>
+      <c r="F210" s="22">
+        <v>1</v>
+      </c>
+      <c r="G210" s="3">
+        <v>0</v>
+      </c>
+      <c r="H210" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="B211" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C210" s="2">
-        <v>0</v>
-      </c>
-      <c r="D210" s="2">
-        <v>0</v>
-      </c>
-      <c r="E210" s="20">
-        <v>1</v>
-      </c>
-      <c r="F210" s="20">
-        <v>1</v>
-      </c>
-      <c r="G210" s="3">
-        <v>0</v>
-      </c>
-      <c r="H210" s="18" t="s">
+      <c r="C211" s="2">
+        <v>0</v>
+      </c>
+      <c r="D211" s="2">
+        <v>0</v>
+      </c>
+      <c r="E211" s="20">
+        <v>1</v>
+      </c>
+      <c r="F211" s="20">
+        <v>1</v>
+      </c>
+      <c r="G211" s="3">
+        <v>0</v>
+      </c>
+      <c r="H211" s="18" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data quality checks and reports
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -68,9 +68,6 @@
     <t>cg_age_yr</t>
   </si>
   <si>
-    <t>yg_age_ctg</t>
-  </si>
-  <si>
     <t>cg_age_ctg</t>
   </si>
   <si>
@@ -1890,6 +1887,9 @@
   </si>
   <si>
     <t>crfs-t09a1-vaccine_injection</t>
+  </si>
+  <si>
+    <t>yg_infant_ctg</t>
   </si>
 </sst>
 </file>
@@ -2312,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2335,22 +2335,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2358,7 +2358,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -2381,10 +2381,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -2402,16 +2402,16 @@
         <v>0</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -2428,15 +2428,15 @@
         <v>0</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -2454,15 +2454,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2480,15 +2480,15 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2506,15 +2506,15 @@
         <v>0</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -2532,15 +2532,15 @@
         <v>0</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2558,15 +2558,15 @@
         <v>0</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2584,15 +2584,15 @@
         <v>0</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2610,15 +2610,15 @@
         <v>0</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>338</v>
+        <v>502</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>504</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -2633,18 +2633,18 @@
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>177</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>503</v>
+        <v>337</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>505</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -2659,18 +2659,18 @@
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>504</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -2688,12 +2688,12 @@
         <v>0</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>2</v>
@@ -2714,15 +2714,15 @@
         <v>1</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>341</v>
+        <v>501</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>14</v>
+        <v>500</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -2737,18 +2737,18 @@
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>180</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>502</v>
+        <v>341</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>501</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>501</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2774,7 +2774,7 @@
         <v>342</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -2800,13 +2800,13 @@
         <v>343</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>182</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>10</v>
+        <v>621</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -2844,15 +2844,15 @@
         <v>1</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="20">
         <v>1</v>
@@ -2870,15 +2870,15 @@
         <v>1</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="20">
         <v>1</v>
@@ -2896,12 +2896,12 @@
         <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>8</v>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -2948,15 +2948,15 @@
         <v>1</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -2974,12 +2974,12 @@
         <v>0</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>13</v>
@@ -3000,15 +3000,15 @@
         <v>1</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -3026,12 +3026,12 @@
         <v>1</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>4</v>
@@ -3052,12 +3052,12 @@
         <v>1</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>6</v>
@@ -3078,15 +3078,15 @@
         <v>0</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3104,12 +3104,12 @@
         <v>0</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>5</v>
@@ -3130,42 +3130,42 @@
         <v>0</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>518</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>522</v>
-      </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
@@ -3182,15 +3182,15 @@
         <v>0</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -3208,15 +3208,15 @@
         <v>1</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -3234,15 +3234,15 @@
         <v>1</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -3260,15 +3260,15 @@
         <v>1</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -3286,15 +3286,15 @@
         <v>1</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -3312,15 +3312,15 @@
         <v>1</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
@@ -3338,15 +3338,15 @@
         <v>0</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
@@ -3364,15 +3364,15 @@
         <v>0</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
@@ -3390,15 +3390,15 @@
         <v>0</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
@@ -3416,12 +3416,12 @@
         <v>0</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>3</v>
@@ -3442,15 +3442,15 @@
         <v>0</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -3468,15 +3468,15 @@
         <v>0</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -3494,15 +3494,15 @@
         <v>1</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -3520,15 +3520,15 @@
         <v>1</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -3546,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48" s="2">
         <v>0</v>
@@ -3572,15 +3572,15 @@
         <v>0</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -3598,41 +3598,41 @@
         <v>1</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B50" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+      <c r="H50" s="11" t="s">
         <v>571</v>
-      </c>
-      <c r="C50" s="2">
-        <v>0</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0</v>
-      </c>
-      <c r="G50" s="3">
-        <v>1</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -3650,15 +3650,15 @@
         <v>0</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
@@ -3676,15 +3676,15 @@
         <v>0</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -3702,15 +3702,15 @@
         <v>0</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -3728,41 +3728,41 @@
         <v>0</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="C55" s="2">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>508</v>
-      </c>
-      <c r="C55" s="2">
-        <v>0</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4">
-        <v>0</v>
-      </c>
-      <c r="F55" s="4">
-        <v>0</v>
-      </c>
-      <c r="G55" s="3">
-        <v>0</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
@@ -3780,15 +3780,15 @@
         <v>0</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -3806,15 +3806,15 @@
         <v>0</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
@@ -3832,15 +3832,15 @@
         <v>0</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -3858,16 +3858,16 @@
         <v>0</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="B60" s="19" t="s">
-        <v>514</v>
-      </c>
       <c r="C60" s="2">
         <v>1</v>
       </c>
@@ -3884,16 +3884,16 @@
         <v>1</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="B61" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="B61" s="19" t="s">
-        <v>516</v>
-      </c>
       <c r="C61" s="2">
         <v>1</v>
       </c>
@@ -3910,67 +3910,67 @@
         <v>1</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="4">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+      <c r="H62" s="11" t="s">
         <v>510</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="C62" s="2">
-        <v>1</v>
-      </c>
-      <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="4">
-        <v>1</v>
-      </c>
-      <c r="F62" s="4">
-        <v>0</v>
-      </c>
-      <c r="G62" s="3">
-        <v>1</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>562</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1</v>
+      </c>
+      <c r="E63" s="4">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0</v>
+      </c>
+      <c r="G63" s="3">
+        <v>1</v>
+      </c>
+      <c r="H63" s="11" t="s">
         <v>563</v>
-      </c>
-      <c r="C63" s="2">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2">
-        <v>1</v>
-      </c>
-      <c r="E63" s="4">
-        <v>1</v>
-      </c>
-      <c r="F63" s="4">
-        <v>0</v>
-      </c>
-      <c r="G63" s="3">
-        <v>1</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C64" s="2">
         <v>1</v>
@@ -3988,15 +3988,15 @@
         <v>1</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -4014,15 +4014,15 @@
         <v>1</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
@@ -4040,15 +4040,15 @@
         <v>1</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="20">
         <v>0</v>
@@ -4066,15 +4066,15 @@
         <v>1</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="20">
         <v>0</v>
@@ -4092,15 +4092,15 @@
         <v>1</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" s="20">
         <v>0</v>
@@ -4118,15 +4118,15 @@
         <v>1</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C70" s="20">
         <v>0</v>
@@ -4144,15 +4144,15 @@
         <v>1</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C71" s="2">
         <v>0</v>
@@ -4170,15 +4170,15 @@
         <v>1</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C72" s="2">
         <v>0</v>
@@ -4196,15 +4196,15 @@
         <v>1</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -4222,15 +4222,15 @@
         <v>1</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -4248,15 +4248,15 @@
         <v>1</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -4274,15 +4274,15 @@
         <v>1</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -4300,15 +4300,15 @@
         <v>1</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -4326,15 +4326,15 @@
         <v>1</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -4352,15 +4352,15 @@
         <v>1</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -4378,15 +4378,15 @@
         <v>1</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -4404,15 +4404,15 @@
         <v>1</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
@@ -4430,15 +4430,15 @@
         <v>1</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C82" s="2">
         <v>0</v>
@@ -4456,15 +4456,15 @@
         <v>1</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -4482,15 +4482,15 @@
         <v>1</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C84" s="2">
         <v>0</v>
@@ -4508,15 +4508,15 @@
         <v>1</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C85" s="2">
         <v>0</v>
@@ -4534,15 +4534,15 @@
         <v>1</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C86" s="20">
         <v>0</v>
@@ -4560,15 +4560,15 @@
         <v>1</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C87" s="20">
         <v>0</v>
@@ -4586,15 +4586,15 @@
         <v>1</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C88" s="20">
         <v>0</v>
@@ -4612,15 +4612,15 @@
         <v>1</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C89" s="20">
         <v>0</v>
@@ -4638,15 +4638,15 @@
         <v>1</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C90" s="20">
         <v>0</v>
@@ -4664,15 +4664,15 @@
         <v>1</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C91" s="20">
         <v>0</v>
@@ -4690,15 +4690,15 @@
         <v>1</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C92" s="20">
         <v>0</v>
@@ -4716,15 +4716,15 @@
         <v>1</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -4742,15 +4742,15 @@
         <v>1</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -4768,15 +4768,15 @@
         <v>1</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C95" s="2">
         <v>0</v>
@@ -4794,15 +4794,15 @@
         <v>1</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C96" s="2">
         <v>0</v>
@@ -4820,15 +4820,15 @@
         <v>0</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -4846,15 +4846,15 @@
         <v>0</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -4872,15 +4872,15 @@
         <v>0</v>
       </c>
       <c r="H98" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -4898,15 +4898,15 @@
         <v>0</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -4924,15 +4924,15 @@
         <v>0</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -4950,15 +4950,15 @@
         <v>0</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
@@ -4976,15 +4976,15 @@
         <v>0</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -5002,15 +5002,15 @@
         <v>0</v>
       </c>
       <c r="H103" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -5028,15 +5028,15 @@
         <v>0</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
@@ -5054,15 +5054,15 @@
         <v>0</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -5080,15 +5080,15 @@
         <v>0</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
@@ -5106,15 +5106,15 @@
         <v>0</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
@@ -5132,15 +5132,15 @@
         <v>0</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -5158,15 +5158,15 @@
         <v>0</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -5184,15 +5184,15 @@
         <v>0</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -5210,15 +5210,15 @@
         <v>0</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
@@ -5236,15 +5236,15 @@
         <v>1</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113" s="2">
         <v>0</v>
@@ -5262,15 +5262,15 @@
         <v>1</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -5288,15 +5288,15 @@
         <v>1</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -5314,15 +5314,15 @@
         <v>1</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -5340,15 +5340,15 @@
         <v>1</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
@@ -5366,15 +5366,15 @@
         <v>1</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C118" s="2">
         <v>0</v>
@@ -5392,15 +5392,15 @@
         <v>1</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C119" s="2">
         <v>0</v>
@@ -5418,15 +5418,15 @@
         <v>1</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
@@ -5444,15 +5444,15 @@
         <v>1</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C121" s="2">
         <v>0</v>
@@ -5470,15 +5470,15 @@
         <v>1</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C122" s="2">
         <v>0</v>
@@ -5496,15 +5496,15 @@
         <v>1</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -5522,15 +5522,15 @@
         <v>1</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -5548,15 +5548,15 @@
         <v>1</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -5574,15 +5574,15 @@
         <v>1</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -5600,15 +5600,15 @@
         <v>1</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -5626,15 +5626,15 @@
         <v>1</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -5652,15 +5652,15 @@
         <v>1</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -5678,15 +5678,15 @@
         <v>0</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -5704,15 +5704,15 @@
         <v>0</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C131" s="2">
         <v>0</v>
@@ -5730,15 +5730,15 @@
         <v>0</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C132" s="2">
         <v>0</v>
@@ -5756,15 +5756,15 @@
         <v>0</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
@@ -5782,41 +5782,41 @@
         <v>0</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B134" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0</v>
+      </c>
+      <c r="E134" s="20">
+        <v>1</v>
+      </c>
+      <c r="F134" s="22">
+        <v>1</v>
+      </c>
+      <c r="G134" s="3">
+        <v>0</v>
+      </c>
+      <c r="H134" s="17" t="s">
         <v>611</v>
-      </c>
-      <c r="C134" s="2">
-        <v>0</v>
-      </c>
-      <c r="D134" s="2">
-        <v>0</v>
-      </c>
-      <c r="E134" s="20">
-        <v>1</v>
-      </c>
-      <c r="F134" s="22">
-        <v>1</v>
-      </c>
-      <c r="G134" s="3">
-        <v>0</v>
-      </c>
-      <c r="H134" s="17" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -5834,15 +5834,15 @@
         <v>0</v>
       </c>
       <c r="H135" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -5860,15 +5860,15 @@
         <v>0</v>
       </c>
       <c r="H136" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -5886,15 +5886,15 @@
         <v>0</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5912,15 +5912,15 @@
         <v>0</v>
       </c>
       <c r="H138" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -5938,15 +5938,15 @@
         <v>0</v>
       </c>
       <c r="H139" s="18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="18" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C140" s="2">
         <v>0</v>
@@ -5964,15 +5964,15 @@
         <v>0</v>
       </c>
       <c r="H140" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -5990,15 +5990,15 @@
         <v>0</v>
       </c>
       <c r="H141" s="18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -6016,15 +6016,15 @@
         <v>0</v>
       </c>
       <c r="H142" s="18" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -6042,15 +6042,15 @@
         <v>0</v>
       </c>
       <c r="H143" s="18" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6068,15 +6068,15 @@
         <v>0</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6094,15 +6094,15 @@
         <v>0</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6120,15 +6120,15 @@
         <v>0</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6146,15 +6146,15 @@
         <v>0</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6172,15 +6172,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6198,15 +6198,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6224,15 +6224,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6250,15 +6250,15 @@
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6276,15 +6276,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6302,15 +6302,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6328,15 +6328,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6354,15 +6354,15 @@
         <v>0</v>
       </c>
       <c r="H155" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -6380,15 +6380,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6406,15 +6406,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6432,15 +6432,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6458,15 +6458,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6484,15 +6484,15 @@
         <v>0</v>
       </c>
       <c r="H160" s="17" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6510,15 +6510,15 @@
         <v>0</v>
       </c>
       <c r="H161" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6536,15 +6536,15 @@
         <v>0</v>
       </c>
       <c r="H162" s="17" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6562,15 +6562,15 @@
         <v>0</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6588,15 +6588,15 @@
         <v>0</v>
       </c>
       <c r="H164" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6614,15 +6614,15 @@
         <v>1</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6640,67 +6640,67 @@
         <v>1</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="B167" s="14" t="s">
         <v>574</v>
       </c>
-      <c r="B167" s="14" t="s">
+      <c r="C167" s="2">
+        <v>0</v>
+      </c>
+      <c r="D167" s="2">
+        <v>0</v>
+      </c>
+      <c r="E167" s="20">
+        <v>1</v>
+      </c>
+      <c r="F167" s="22">
+        <v>1</v>
+      </c>
+      <c r="G167" s="3">
+        <v>1</v>
+      </c>
+      <c r="H167" s="17" t="s">
         <v>575</v>
-      </c>
-      <c r="C167" s="2">
-        <v>0</v>
-      </c>
-      <c r="D167" s="2">
-        <v>0</v>
-      </c>
-      <c r="E167" s="20">
-        <v>1</v>
-      </c>
-      <c r="F167" s="22">
-        <v>1</v>
-      </c>
-      <c r="G167" s="3">
-        <v>1</v>
-      </c>
-      <c r="H167" s="17" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="B168" s="14" t="s">
         <v>577</v>
       </c>
-      <c r="B168" s="14" t="s">
+      <c r="C168" s="2">
+        <v>0</v>
+      </c>
+      <c r="D168" s="2">
+        <v>0</v>
+      </c>
+      <c r="E168" s="20">
+        <v>1</v>
+      </c>
+      <c r="F168" s="22">
+        <v>1</v>
+      </c>
+      <c r="G168" s="3">
+        <v>1</v>
+      </c>
+      <c r="H168" s="17" t="s">
         <v>578</v>
-      </c>
-      <c r="C168" s="2">
-        <v>0</v>
-      </c>
-      <c r="D168" s="2">
-        <v>0</v>
-      </c>
-      <c r="E168" s="20">
-        <v>1</v>
-      </c>
-      <c r="F168" s="22">
-        <v>1</v>
-      </c>
-      <c r="G168" s="3">
-        <v>1</v>
-      </c>
-      <c r="H168" s="17" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6718,15 +6718,15 @@
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6744,15 +6744,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6770,15 +6770,15 @@
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6796,15 +6796,15 @@
         <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6822,15 +6822,15 @@
         <v>0</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6848,15 +6848,15 @@
         <v>0</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6874,15 +6874,15 @@
         <v>1</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6900,15 +6900,15 @@
         <v>1</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6926,15 +6926,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6952,15 +6952,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6978,15 +6978,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -7004,15 +7004,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7030,15 +7030,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7056,15 +7056,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7082,15 +7082,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7108,15 +7108,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7134,15 +7134,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7160,15 +7160,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7186,15 +7186,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7212,15 +7212,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7238,15 +7238,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7264,15 +7264,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7290,15 +7290,15 @@
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7316,15 +7316,15 @@
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7342,15 +7342,15 @@
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7368,15 +7368,15 @@
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7394,15 +7394,15 @@
         <v>0</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7420,15 +7420,15 @@
         <v>0</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7446,15 +7446,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7472,15 +7472,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7498,15 +7498,15 @@
         <v>0</v>
       </c>
       <c r="H199" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C200" s="2">
         <v>0</v>
@@ -7524,15 +7524,15 @@
         <v>0</v>
       </c>
       <c r="H200" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B201" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C201" s="2">
         <v>0</v>
@@ -7550,15 +7550,15 @@
         <v>0</v>
       </c>
       <c r="H201" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C202" s="2">
         <v>0</v>
@@ -7576,15 +7576,15 @@
         <v>0</v>
       </c>
       <c r="H202" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B203" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C203" s="2">
         <v>0</v>
@@ -7602,15 +7602,15 @@
         <v>0</v>
       </c>
       <c r="H203" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7628,15 +7628,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7654,15 +7654,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7680,15 +7680,15 @@
         <v>0</v>
       </c>
       <c r="H206" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C207" s="2">
         <v>0</v>
@@ -7706,15 +7706,15 @@
         <v>0</v>
       </c>
       <c r="H207" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B208" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C208" s="2">
         <v>0</v>
@@ -7732,15 +7732,15 @@
         <v>0</v>
       </c>
       <c r="H208" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B209" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C209" s="2">
         <v>0</v>
@@ -7758,15 +7758,15 @@
         <v>0</v>
       </c>
       <c r="H209" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B210" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C210" s="2">
         <v>0</v>
@@ -7784,15 +7784,15 @@
         <v>0</v>
       </c>
       <c r="H210" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B211" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C211" s="2">
         <v>0</v>
@@ -7810,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="H211" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update RCT, SPA and PM/TF reports
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="641">
   <si>
     <t>old</t>
   </si>
@@ -1938,6 +1938,15 @@
   </si>
   <si>
     <t>submission_date</t>
+  </si>
+  <si>
+    <t>meta-instanceID</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>instanceID</t>
   </si>
 </sst>
 </file>
@@ -2361,24 +2370,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221:XFD221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
     <col min="5" max="5" width="9.25" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="3"/>
-    <col min="8" max="8" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>493</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>636</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>560</v>
       </c>
@@ -2560,7 +2569,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>634</v>
       </c>
@@ -2586,7 +2595,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>622</v>
       </c>
@@ -2612,7 +2621,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>635</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>623</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>625</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>627</v>
       </c>
@@ -2716,7 +2725,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>629</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>631</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>333</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>334</v>
       </c>
@@ -2820,7 +2829,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>494</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>335</v>
       </c>
@@ -2872,7 +2881,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>336</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>502</v>
       </c>
@@ -2924,7 +2933,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>337</v>
       </c>
@@ -2950,7 +2959,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>338</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>339</v>
       </c>
@@ -3002,7 +3011,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>501</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>341</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>342</v>
       </c>
@@ -3080,7 +3089,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>343</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>340</v>
       </c>
@@ -3132,7 +3141,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>344</v>
       </c>
@@ -3158,7 +3167,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>345</v>
       </c>
@@ -3184,7 +3193,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>346</v>
       </c>
@@ -3210,7 +3219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>347</v>
       </c>
@@ -3236,7 +3245,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>348</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>349</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>350</v>
       </c>
@@ -3314,7 +3323,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>351</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>352</v>
       </c>
@@ -3366,7 +3375,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>353</v>
       </c>
@@ -3392,7 +3401,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>354</v>
       </c>
@@ -3418,7 +3427,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>516</v>
       </c>
@@ -3444,7 +3453,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>520</v>
       </c>
@@ -3470,7 +3479,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>355</v>
       </c>
@@ -3496,7 +3505,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>356</v>
       </c>
@@ -3522,7 +3531,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>357</v>
       </c>
@@ -3548,7 +3557,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>358</v>
       </c>
@@ -3574,7 +3583,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>359</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>360</v>
       </c>
@@ -3626,7 +3635,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>361</v>
       </c>
@@ -3652,7 +3661,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>362</v>
       </c>
@@ -3678,7 +3687,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>363</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>364</v>
       </c>
@@ -3730,7 +3739,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>365</v>
       </c>
@@ -3756,7 +3765,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>366</v>
       </c>
@@ -3782,7 +3791,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>367</v>
       </c>
@@ -3808,7 +3817,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>368</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>369</v>
       </c>
@@ -3860,7 +3869,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>370</v>
       </c>
@@ -3886,7 +3895,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>572</v>
       </c>
@@ -3912,7 +3921,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>371</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>372</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>495</v>
       </c>
@@ -3990,7 +3999,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>496</v>
       </c>
@@ -4016,7 +4025,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>506</v>
       </c>
@@ -4042,7 +4051,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>373</v>
       </c>
@@ -4068,7 +4077,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>374</v>
       </c>
@@ -4094,7 +4103,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>375</v>
       </c>
@@ -4120,7 +4129,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>376</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>512</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>514</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>509</v>
       </c>
@@ -4224,7 +4233,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>561</v>
       </c>
@@ -4250,7 +4259,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>564</v>
       </c>
@@ -4276,7 +4285,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>565</v>
       </c>
@@ -4302,7 +4311,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
         <v>377</v>
       </c>
@@ -4328,7 +4337,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
         <v>378</v>
       </c>
@@ -4354,7 +4363,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
         <v>379</v>
       </c>
@@ -4380,7 +4389,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
         <v>380</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
         <v>381</v>
       </c>
@@ -4432,7 +4441,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
         <v>382</v>
       </c>
@@ -4458,7 +4467,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
         <v>383</v>
       </c>
@@ -4484,7 +4493,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
         <v>384</v>
       </c>
@@ -4510,7 +4519,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
         <v>385</v>
       </c>
@@ -4536,7 +4545,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
         <v>386</v>
       </c>
@@ -4562,7 +4571,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
         <v>387</v>
       </c>
@@ -4588,7 +4597,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
         <v>388</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
         <v>389</v>
       </c>
@@ -4640,7 +4649,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
         <v>390</v>
       </c>
@@ -4666,7 +4675,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>391</v>
       </c>
@@ -4692,7 +4701,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
         <v>392</v>
       </c>
@@ -4718,7 +4727,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
         <v>393</v>
       </c>
@@ -4744,7 +4753,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
         <v>394</v>
       </c>
@@ -4770,7 +4779,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
         <v>395</v>
       </c>
@@ -4796,7 +4805,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>396</v>
       </c>
@@ -4822,7 +4831,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
         <v>397</v>
       </c>
@@ -4848,7 +4857,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
         <v>398</v>
       </c>
@@ -4874,7 +4883,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>399</v>
       </c>
@@ -4900,7 +4909,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>400</v>
       </c>
@@ -4926,7 +4935,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>401</v>
       </c>
@@ -4952,7 +4961,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
         <v>402</v>
       </c>
@@ -4978,7 +4987,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
         <v>403</v>
       </c>
@@ -5004,7 +5013,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
         <v>404</v>
       </c>
@@ -5030,7 +5039,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
         <v>405</v>
       </c>
@@ -5056,7 +5065,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
         <v>406</v>
       </c>
@@ -5082,7 +5091,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="17" t="s">
         <v>407</v>
       </c>
@@ -5108,7 +5117,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="17" t="s">
         <v>408</v>
       </c>
@@ -5134,7 +5143,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="17" t="s">
         <v>409</v>
       </c>
@@ -5160,7 +5169,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="17" t="s">
         <v>410</v>
       </c>
@@ -5186,7 +5195,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="17" t="s">
         <v>411</v>
       </c>
@@ -5212,7 +5221,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
         <v>412</v>
       </c>
@@ -5238,7 +5247,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="17" t="s">
         <v>413</v>
       </c>
@@ -5264,7 +5273,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="17" t="s">
         <v>414</v>
       </c>
@@ -5290,7 +5299,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="17" t="s">
         <v>415</v>
       </c>
@@ -5316,7 +5325,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="17" t="s">
         <v>416</v>
       </c>
@@ -5342,7 +5351,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="17" t="s">
         <v>417</v>
       </c>
@@ -5368,7 +5377,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="17" t="s">
         <v>418</v>
       </c>
@@ -5394,7 +5403,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="17" t="s">
         <v>419</v>
       </c>
@@ -5420,7 +5429,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="17" t="s">
         <v>420</v>
       </c>
@@ -5446,7 +5455,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="17" t="s">
         <v>421</v>
       </c>
@@ -5472,7 +5481,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="s">
         <v>422</v>
       </c>
@@ -5498,7 +5507,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="17" t="s">
         <v>423</v>
       </c>
@@ -5524,7 +5533,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="17" t="s">
         <v>424</v>
       </c>
@@ -5550,7 +5559,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="17" t="s">
         <v>425</v>
       </c>
@@ -5576,7 +5585,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="17" t="s">
         <v>426</v>
       </c>
@@ -5602,7 +5611,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="s">
         <v>427</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="17" t="s">
         <v>428</v>
       </c>
@@ -5654,7 +5663,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="17" t="s">
         <v>429</v>
       </c>
@@ -5680,7 +5689,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="17" t="s">
         <v>430</v>
       </c>
@@ -5706,7 +5715,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="17" t="s">
         <v>431</v>
       </c>
@@ -5732,7 +5741,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="17" t="s">
         <v>432</v>
       </c>
@@ -5758,7 +5767,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
         <v>433</v>
       </c>
@@ -5784,7 +5793,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="17" t="s">
         <v>434</v>
       </c>
@@ -5810,7 +5819,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="17" t="s">
         <v>435</v>
       </c>
@@ -5836,7 +5845,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="17" t="s">
         <v>436</v>
       </c>
@@ -5862,7 +5871,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="17" t="s">
         <v>437</v>
       </c>
@@ -5888,7 +5897,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="17" t="s">
         <v>438</v>
       </c>
@@ -5914,7 +5923,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="17" t="s">
         <v>439</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="17" t="s">
         <v>440</v>
       </c>
@@ -5966,7 +5975,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="17" t="s">
         <v>441</v>
       </c>
@@ -5992,7 +6001,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="17" t="s">
         <v>609</v>
       </c>
@@ -6018,7 +6027,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="17" t="s">
         <v>442</v>
       </c>
@@ -6044,7 +6053,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="17" t="s">
         <v>443</v>
       </c>
@@ -6070,7 +6079,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="17" t="s">
         <v>620</v>
       </c>
@@ -6096,7 +6105,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="17" t="s">
         <v>444</v>
       </c>
@@ -6122,7 +6131,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="17" t="s">
         <v>445</v>
       </c>
@@ -6148,7 +6157,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="17" t="s">
         <v>446</v>
       </c>
@@ -6174,7 +6183,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="18" t="s">
         <v>597</v>
       </c>
@@ -6200,7 +6209,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="18" t="s">
         <v>598</v>
       </c>
@@ -6226,7 +6235,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="18" t="s">
         <v>599</v>
       </c>
@@ -6252,7 +6261,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="18" t="s">
         <v>600</v>
       </c>
@@ -6278,7 +6287,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="18" t="s">
         <v>601</v>
       </c>
@@ -6304,7 +6313,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="18" t="s">
         <v>602</v>
       </c>
@@ -6330,7 +6339,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="17" t="s">
         <v>619</v>
       </c>
@@ -6356,7 +6365,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="17" t="s">
         <v>579</v>
       </c>
@@ -6382,7 +6391,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="17" t="s">
         <v>580</v>
       </c>
@@ -6408,7 +6417,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="17" t="s">
         <v>581</v>
       </c>
@@ -6434,7 +6443,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="17" t="s">
         <v>582</v>
       </c>
@@ -6460,7 +6469,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="17" t="s">
         <v>583</v>
       </c>
@@ -6486,7 +6495,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="17" t="s">
         <v>584</v>
       </c>
@@ -6512,7 +6521,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="17" t="s">
         <v>585</v>
       </c>
@@ -6538,7 +6547,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="17" t="s">
         <v>586</v>
       </c>
@@ -6564,7 +6573,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="17" t="s">
         <v>587</v>
       </c>
@@ -6590,7 +6599,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="17" t="s">
         <v>588</v>
       </c>
@@ -6616,7 +6625,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="17" t="s">
         <v>589</v>
       </c>
@@ -6642,7 +6651,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="17" t="s">
         <v>590</v>
       </c>
@@ -6668,7 +6677,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="17" t="s">
         <v>591</v>
       </c>
@@ -6694,7 +6703,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="17" t="s">
         <v>592</v>
       </c>
@@ -6720,7 +6729,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="17" t="s">
         <v>593</v>
       </c>
@@ -6746,7 +6755,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="17" t="s">
         <v>594</v>
       </c>
@@ -6772,7 +6781,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="17" t="s">
         <v>595</v>
       </c>
@@ -6798,7 +6807,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="17" t="s">
         <v>596</v>
       </c>
@@ -6824,7 +6833,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="17" t="s">
         <v>447</v>
       </c>
@@ -6850,7 +6859,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="17" t="s">
         <v>559</v>
       </c>
@@ -6876,7 +6885,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="17" t="s">
         <v>448</v>
       </c>
@@ -6902,7 +6911,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="17" t="s">
         <v>449</v>
       </c>
@@ -6928,7 +6937,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="17" t="s">
         <v>573</v>
       </c>
@@ -6954,7 +6963,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="17" t="s">
         <v>576</v>
       </c>
@@ -6980,7 +6989,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="17" t="s">
         <v>450</v>
       </c>
@@ -7006,7 +7015,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="17" t="s">
         <v>451</v>
       </c>
@@ -7032,7 +7041,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="17" t="s">
         <v>452</v>
       </c>
@@ -7058,7 +7067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="17" t="s">
         <v>453</v>
       </c>
@@ -7084,7 +7093,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="17" t="s">
         <v>454</v>
       </c>
@@ -7110,7 +7119,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="17" t="s">
         <v>455</v>
       </c>
@@ -7136,7 +7145,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="17" t="s">
         <v>456</v>
       </c>
@@ -7162,7 +7171,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="17" t="s">
         <v>457</v>
       </c>
@@ -7188,7 +7197,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="17" t="s">
         <v>458</v>
       </c>
@@ -7214,7 +7223,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="17" t="s">
         <v>459</v>
       </c>
@@ -7240,7 +7249,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="17" t="s">
         <v>460</v>
       </c>
@@ -7266,7 +7275,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="17" t="s">
         <v>461</v>
       </c>
@@ -7292,7 +7301,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="17" t="s">
         <v>462</v>
       </c>
@@ -7318,7 +7327,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="17" t="s">
         <v>463</v>
       </c>
@@ -7344,7 +7353,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="17" t="s">
         <v>464</v>
       </c>
@@ -7370,7 +7379,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="17" t="s">
         <v>465</v>
       </c>
@@ -7396,7 +7405,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="17" t="s">
         <v>466</v>
       </c>
@@ -7422,7 +7431,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="17" t="s">
         <v>467</v>
       </c>
@@ -7448,7 +7457,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="17" t="s">
         <v>468</v>
       </c>
@@ -7474,7 +7483,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="17" t="s">
         <v>469</v>
       </c>
@@ -7500,7 +7509,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="17" t="s">
         <v>470</v>
       </c>
@@ -7526,7 +7535,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="17" t="s">
         <v>471</v>
       </c>
@@ -7552,7 +7561,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="17" t="s">
         <v>472</v>
       </c>
@@ -7578,7 +7587,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="17" t="s">
         <v>473</v>
       </c>
@@ -7604,7 +7613,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="17" t="s">
         <v>474</v>
       </c>
@@ -7630,7 +7639,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="17" t="s">
         <v>475</v>
       </c>
@@ -7656,7 +7665,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="17" t="s">
         <v>476</v>
       </c>
@@ -7682,7 +7691,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="17" t="s">
         <v>477</v>
       </c>
@@ -7708,7 +7717,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="17" t="s">
         <v>478</v>
       </c>
@@ -7734,7 +7743,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="17" t="s">
         <v>479</v>
       </c>
@@ -7760,7 +7769,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="17" t="s">
         <v>480</v>
       </c>
@@ -7786,7 +7795,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="17" t="s">
         <v>481</v>
       </c>
@@ -7812,7 +7821,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="17" t="s">
         <v>482</v>
       </c>
@@ -7838,7 +7847,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="17" t="s">
         <v>483</v>
       </c>
@@ -7864,7 +7873,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" s="17" t="s">
         <v>484</v>
       </c>
@@ -7890,7 +7899,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="18" t="s">
         <v>485</v>
       </c>
@@ -7916,7 +7925,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="18" t="s">
         <v>486</v>
       </c>
@@ -7942,7 +7951,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="18" t="s">
         <v>487</v>
       </c>
@@ -7968,7 +7977,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="18" t="s">
         <v>488</v>
       </c>
@@ -7994,7 +8003,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="18" t="s">
         <v>489</v>
       </c>
@@ -8020,7 +8029,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" s="18" t="s">
         <v>490</v>
       </c>
@@ -8046,7 +8055,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="18" t="s">
         <v>491</v>
       </c>
@@ -8072,7 +8081,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" s="18" t="s">
         <v>492</v>
       </c>
@@ -8096,6 +8105,32 @@
       </c>
       <c r="H220" s="18" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="C221" s="2">
+        <v>1</v>
+      </c>
+      <c r="D221" s="2">
+        <v>1</v>
+      </c>
+      <c r="E221" s="4">
+        <v>1</v>
+      </c>
+      <c r="F221" s="3">
+        <v>1</v>
+      </c>
+      <c r="G221" s="3">
+        <v>0</v>
+      </c>
+      <c r="H221" s="5" t="s">
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates necessary for Tanzania RCT launch
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="690">
   <si>
     <t>old</t>
   </si>
@@ -431,18 +431,6 @@
     <t>spo2_meas1</t>
   </si>
   <si>
-    <t>spo2_rpt2</t>
-  </si>
-  <si>
-    <t>spo2_meas2</t>
-  </si>
-  <si>
-    <t>spo2_rept3</t>
-  </si>
-  <si>
-    <t>spo2_meas3</t>
-  </si>
-  <si>
     <t>temp</t>
   </si>
   <si>
@@ -923,18 +911,6 @@
     <t>e2_2a</t>
   </si>
   <si>
-    <t>e2_3</t>
-  </si>
-  <si>
-    <t>e2_3a</t>
-  </si>
-  <si>
-    <t>e2_4</t>
-  </si>
-  <si>
-    <t>e2_4a</t>
-  </si>
-  <si>
     <t>d2_6</t>
   </si>
   <si>
@@ -1388,123 +1364,6 @@
     <t>crfs-t09a2-h2_2ao</t>
   </si>
   <si>
-    <t>crfs-t07a-tt07a-e2_1</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_1a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_2</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_2a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_3</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_3a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_4</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt07a-e2_4a</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_6</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_6b</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_1</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_1a</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_4</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_4a</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_5</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_5a</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_2</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_2b</t>
-  </si>
-  <si>
-    <t>crfs-t06a-tt06a-d2_3</t>
-  </si>
-  <si>
-    <t>crfs-t06a-d2_3b</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_1</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_1o</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_2</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_3</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_4</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_5</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_10a</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_6</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_7</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_8</t>
-  </si>
-  <si>
-    <t>crfs-t08a-f2_9</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_1</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_2</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_3</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_3a</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_4</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_6a</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_6</t>
-  </si>
-  <si>
-    <t>crfs-t05b-c3_6o</t>
-  </si>
-  <si>
     <t>SubmitterID</t>
   </si>
   <si>
@@ -2130,6 +1989,111 @@
   </si>
   <si>
     <t>ra_name</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t07a-e2_2a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t07a-e2_2</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t07a-e2_1</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t07a-e2_1a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_6</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_6b</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_1</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_1a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_4</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_4a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_5</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_5a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_2</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_2b</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_3</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t06a-d2_3b</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_1</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_1o</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_2</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_3</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_4</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_5</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_6</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_7</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_8</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_9</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t08a-f2_10a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_1</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_2</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_3</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_3a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_4</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_6a</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_6</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-t05b-c3_6o</t>
   </si>
 </sst>
 </file>
@@ -2553,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H242"/>
+  <dimension ref="A1:H238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2584,16 +2548,16 @@
         <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>522</v>
+        <v>475</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2676,10 +2640,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>493</v>
+        <v>446</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -2697,15 +2661,15 @@
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>493</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>700</v>
+        <v>653</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>701</v>
+        <v>654</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -2723,15 +2687,15 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>700</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>636</v>
+        <v>589</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>637</v>
+        <v>590</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2749,15 +2713,15 @@
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>636</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>560</v>
+        <v>513</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>560</v>
+        <v>513</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -2775,15 +2739,15 @@
         <v>0</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>560</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>634</v>
+        <v>587</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2801,15 +2765,15 @@
         <v>0</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>560</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>622</v>
+        <v>575</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>622</v>
+        <v>575</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -2827,15 +2791,15 @@
         <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>622</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>635</v>
+        <v>588</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>635</v>
+        <v>588</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2853,15 +2817,15 @@
         <v>0</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>622</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>623</v>
+        <v>576</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>624</v>
+        <v>577</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -2879,15 +2843,15 @@
         <v>1</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>623</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>625</v>
+        <v>578</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>626</v>
+        <v>579</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -2905,15 +2869,15 @@
         <v>1</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>625</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>627</v>
+        <v>580</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>628</v>
+        <v>581</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -2931,15 +2895,15 @@
         <v>1</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>627</v>
+        <v>580</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>629</v>
+        <v>582</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>630</v>
+        <v>583</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -2957,15 +2921,15 @@
         <v>1</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>629</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>631</v>
+        <v>584</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>633</v>
+        <v>586</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -2983,12 +2947,12 @@
         <v>0</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>632</v>
+        <v>585</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>20</v>
@@ -3009,12 +2973,12 @@
         <v>0</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>34</v>
@@ -3035,15 +2999,15 @@
         <v>0</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>494</v>
+        <v>447</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>494</v>
+        <v>447</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -3061,12 +3025,12 @@
         <v>0</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>494</v>
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>35</v>
@@ -3087,12 +3051,12 @@
         <v>0</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>36</v>
@@ -3118,10 +3082,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>502</v>
+        <v>455</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>504</v>
+        <v>457</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -3139,12 +3103,12 @@
         <v>0</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>503</v>
+        <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>9</v>
@@ -3165,12 +3129,12 @@
         <v>1</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>28</v>
@@ -3191,12 +3155,12 @@
         <v>0</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>2</v>
@@ -3217,15 +3181,15 @@
         <v>1</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>501</v>
+        <v>454</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>500</v>
+        <v>453</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
@@ -3243,12 +3207,12 @@
         <v>0</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>500</v>
+        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>11</v>
@@ -3269,12 +3233,12 @@
         <v>0</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>12</v>
@@ -3295,12 +3259,12 @@
         <v>0</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>10</v>
@@ -3321,15 +3285,15 @@
         <v>1</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>621</v>
+        <v>574</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -3347,12 +3311,12 @@
         <v>1</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>22</v>
@@ -3373,12 +3337,12 @@
         <v>1</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>23</v>
@@ -3399,12 +3363,12 @@
         <v>1</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>8</v>
@@ -3430,7 +3394,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>37</v>
@@ -3451,12 +3415,12 @@
         <v>1</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>21</v>
@@ -3477,12 +3441,12 @@
         <v>0</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>13</v>
@@ -3503,12 +3467,12 @@
         <v>1</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>14</v>
@@ -3529,12 +3493,12 @@
         <v>1</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>4</v>
@@ -3555,12 +3519,12 @@
         <v>1</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>6</v>
@@ -3581,12 +3545,12 @@
         <v>0</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>15</v>
@@ -3607,12 +3571,12 @@
         <v>0</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>5</v>
@@ -3633,15 +3597,15 @@
         <v>0</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>516</v>
+        <v>469</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>517</v>
+        <v>470</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
@@ -3659,15 +3623,15 @@
         <v>1</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>520</v>
+        <v>473</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>521</v>
+        <v>474</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -3685,12 +3649,12 @@
         <v>0</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>519</v>
+        <v>472</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>16</v>
@@ -3711,12 +3675,12 @@
         <v>1</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>45</v>
@@ -3737,12 +3701,12 @@
         <v>1</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>46</v>
@@ -3763,12 +3727,12 @@
         <v>1</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>47</v>
@@ -3789,12 +3753,12 @@
         <v>1</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>48</v>
@@ -3815,12 +3779,12 @@
         <v>1</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>49</v>
@@ -3841,12 +3805,12 @@
         <v>0</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>17</v>
@@ -3867,12 +3831,12 @@
         <v>0</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>18</v>
@@ -3893,12 +3857,12 @@
         <v>0</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>19</v>
@@ -3919,12 +3883,12 @@
         <v>0</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>3</v>
@@ -3945,12 +3909,12 @@
         <v>0</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>29</v>
@@ -3971,15 +3935,15 @@
         <v>0</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>641</v>
+        <v>594</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>643</v>
+        <v>596</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
@@ -3997,15 +3961,15 @@
         <v>1</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>644</v>
+        <v>597</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>642</v>
+        <v>595</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>646</v>
+        <v>599</v>
       </c>
       <c r="C56" s="2">
         <v>1</v>
@@ -4023,12 +3987,12 @@
         <v>1</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>645</v>
+        <v>598</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>31</v>
@@ -4049,15 +4013,15 @@
         <v>1</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C58" s="2">
         <v>1</v>
@@ -4075,12 +4039,12 @@
         <v>1</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>32</v>
@@ -4101,12 +4065,12 @@
         <v>0</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>33</v>
@@ -4127,12 +4091,12 @@
         <v>0</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>42</v>
@@ -4153,15 +4117,15 @@
         <v>1</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>572</v>
+        <v>525</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>570</v>
+        <v>523</v>
       </c>
       <c r="C62" s="2">
         <v>0</v>
@@ -4179,12 +4143,12 @@
         <v>1</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>571</v>
+        <v>524</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>38</v>
@@ -4205,12 +4169,12 @@
         <v>0</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>39</v>
@@ -4231,15 +4195,15 @@
         <v>0</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>495</v>
+        <v>448</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>499</v>
+        <v>452</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -4257,15 +4221,15 @@
         <v>0</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>497</v>
+        <v>450</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>496</v>
+        <v>449</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>505</v>
+        <v>458</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
@@ -4283,15 +4247,15 @@
         <v>0</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>498</v>
+        <v>451</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>506</v>
+        <v>459</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>507</v>
+        <v>460</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
@@ -4309,12 +4273,12 @@
         <v>0</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>508</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>40</v>
@@ -4335,15 +4299,15 @@
         <v>0</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
-        <v>654</v>
+        <v>607</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>652</v>
+        <v>605</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -4361,12 +4325,12 @@
         <v>0</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>653</v>
+        <v>606</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>41</v>
@@ -4387,12 +4351,12 @@
         <v>0</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>43</v>
@@ -4413,12 +4377,12 @@
         <v>0</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>44</v>
@@ -4439,15 +4403,15 @@
         <v>0</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
-        <v>512</v>
+        <v>465</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>513</v>
+        <v>466</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
@@ -4465,15 +4429,15 @@
         <v>1</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>513</v>
+        <v>466</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>514</v>
+        <v>467</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>515</v>
+        <v>468</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -4491,15 +4455,15 @@
         <v>1</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>515</v>
+        <v>468</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>509</v>
+        <v>462</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -4517,15 +4481,15 @@
         <v>1</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>561</v>
+        <v>514</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>562</v>
+        <v>515</v>
       </c>
       <c r="C76" s="2">
         <v>1</v>
@@ -4543,15 +4507,15 @@
         <v>1</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>563</v>
+        <v>516</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>564</v>
+        <v>517</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>566</v>
+        <v>519</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -4569,15 +4533,15 @@
         <v>1</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>568</v>
+        <v>521</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>565</v>
+        <v>518</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>567</v>
+        <v>520</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -4595,15 +4559,15 @@
         <v>1</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>569</v>
+        <v>522</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>647</v>
+        <v>600</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>648</v>
+        <v>601</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -4621,15 +4585,15 @@
         <v>1</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>648</v>
+        <v>601</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>649</v>
+        <v>602</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>650</v>
+        <v>603</v>
       </c>
       <c r="C80" s="2">
         <v>1</v>
@@ -4647,12 +4611,12 @@
         <v>0</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>651</v>
+        <v>604</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>51</v>
@@ -4673,12 +4637,12 @@
         <v>1</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>52</v>
@@ -4699,12 +4663,12 @@
         <v>1</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>53</v>
@@ -4725,12 +4689,12 @@
         <v>1</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>54</v>
@@ -4751,12 +4715,12 @@
         <v>1</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>55</v>
@@ -4777,12 +4741,12 @@
         <v>1</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>56</v>
@@ -4803,12 +4767,12 @@
         <v>1</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>57</v>
@@ -4829,12 +4793,12 @@
         <v>1</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>58</v>
@@ -4855,12 +4819,12 @@
         <v>1</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>59</v>
@@ -4881,12 +4845,12 @@
         <v>1</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>60</v>
@@ -4907,12 +4871,12 @@
         <v>1</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>61</v>
@@ -4933,12 +4897,12 @@
         <v>1</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>62</v>
@@ -4959,12 +4923,12 @@
         <v>1</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>63</v>
@@ -4985,12 +4949,12 @@
         <v>1</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>64</v>
@@ -5011,12 +4975,12 @@
         <v>1</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>65</v>
@@ -5037,12 +5001,12 @@
         <v>1</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>66</v>
@@ -5063,12 +5027,12 @@
         <v>1</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>67</v>
@@ -5089,12 +5053,12 @@
         <v>1</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B98" s="13" t="s">
         <v>68</v>
@@ -5115,12 +5079,12 @@
         <v>1</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B99" s="13" t="s">
         <v>69</v>
@@ -5141,12 +5105,12 @@
         <v>1</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="13" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>70</v>
@@ -5167,12 +5131,12 @@
         <v>1</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="13" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>71</v>
@@ -5193,12 +5157,12 @@
         <v>1</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>72</v>
@@ -5219,12 +5183,12 @@
         <v>1</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>73</v>
@@ -5245,12 +5209,12 @@
         <v>1</v>
       </c>
       <c r="H103" s="13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B104" s="13" t="s">
         <v>74</v>
@@ -5271,12 +5235,12 @@
         <v>1</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B105" s="13" t="s">
         <v>75</v>
@@ -5297,12 +5261,12 @@
         <v>1</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>76</v>
@@ -5323,12 +5287,12 @@
         <v>1</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="13" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B107" s="13" t="s">
         <v>77</v>
@@ -5349,12 +5313,12 @@
         <v>1</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B108" s="13" t="s">
         <v>78</v>
@@ -5375,12 +5339,12 @@
         <v>1</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B109" s="13" t="s">
         <v>79</v>
@@ -5401,15 +5365,15 @@
         <v>1</v>
       </c>
       <c r="H109" s="13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="21" t="s">
-        <v>658</v>
+        <v>611</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>659</v>
+        <v>612</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -5427,15 +5391,15 @@
         <v>0</v>
       </c>
       <c r="H110" s="22" t="s">
-        <v>660</v>
+        <v>613</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="21" t="s">
-        <v>656</v>
+        <v>609</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>657</v>
+        <v>610</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -5453,12 +5417,12 @@
         <v>0</v>
       </c>
       <c r="H111" s="22" t="s">
-        <v>655</v>
+        <v>608</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>80</v>
@@ -5479,12 +5443,12 @@
         <v>1</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B113" s="14" t="s">
         <v>81</v>
@@ -5505,12 +5469,12 @@
         <v>0</v>
       </c>
       <c r="H113" s="14" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>82</v>
@@ -5531,12 +5495,12 @@
         <v>0</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B115" s="14" t="s">
         <v>83</v>
@@ -5557,12 +5521,12 @@
         <v>0</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="14" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B116" s="14" t="s">
         <v>84</v>
@@ -5583,12 +5547,12 @@
         <v>0</v>
       </c>
       <c r="H116" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="14" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B117" s="14" t="s">
         <v>85</v>
@@ -5609,12 +5573,12 @@
         <v>0</v>
       </c>
       <c r="H117" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B118" s="14" t="s">
         <v>86</v>
@@ -5635,12 +5599,12 @@
         <v>0</v>
       </c>
       <c r="H118" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="14" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B119" s="14" t="s">
         <v>87</v>
@@ -5661,12 +5625,12 @@
         <v>0</v>
       </c>
       <c r="H119" s="14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="14" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B120" s="14" t="s">
         <v>88</v>
@@ -5687,12 +5651,12 @@
         <v>0</v>
       </c>
       <c r="H120" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="14" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B121" s="14" t="s">
         <v>89</v>
@@ -5713,12 +5677,12 @@
         <v>0</v>
       </c>
       <c r="H121" s="14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="14" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B122" s="14" t="s">
         <v>90</v>
@@ -5739,12 +5703,12 @@
         <v>0</v>
       </c>
       <c r="H122" s="14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="14" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B123" s="14" t="s">
         <v>91</v>
@@ -5765,12 +5729,12 @@
         <v>0</v>
       </c>
       <c r="H123" s="14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="14" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B124" s="14" t="s">
         <v>92</v>
@@ -5791,12 +5755,12 @@
         <v>0</v>
       </c>
       <c r="H124" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="14" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B125" s="14" t="s">
         <v>93</v>
@@ -5817,12 +5781,12 @@
         <v>0</v>
       </c>
       <c r="H125" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="14" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B126" s="14" t="s">
         <v>94</v>
@@ -5843,12 +5807,12 @@
         <v>0</v>
       </c>
       <c r="H126" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="14" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B127" s="14" t="s">
         <v>95</v>
@@ -5869,12 +5833,12 @@
         <v>0</v>
       </c>
       <c r="H127" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="14" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B128" s="14" t="s">
         <v>96</v>
@@ -5895,12 +5859,12 @@
         <v>0</v>
       </c>
       <c r="H128" s="14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="14" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>97</v>
@@ -5921,12 +5885,12 @@
         <v>1</v>
       </c>
       <c r="H129" s="14" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="14" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B130" s="22" t="s">
         <v>98</v>
@@ -5947,12 +5911,12 @@
         <v>1</v>
       </c>
       <c r="H130" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B131" s="22" t="s">
         <v>99</v>
@@ -5973,12 +5937,12 @@
         <v>1</v>
       </c>
       <c r="H131" s="14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B132" s="22" t="s">
         <v>100</v>
@@ -5999,12 +5963,12 @@
         <v>1</v>
       </c>
       <c r="H132" s="14" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B133" s="22" t="s">
         <v>101</v>
@@ -6025,12 +5989,12 @@
         <v>1</v>
       </c>
       <c r="H133" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B134" s="22" t="s">
         <v>102</v>
@@ -6051,12 +6015,12 @@
         <v>1</v>
       </c>
       <c r="H134" s="14" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B135" s="22" t="s">
         <v>103</v>
@@ -6077,12 +6041,12 @@
         <v>1</v>
       </c>
       <c r="H135" s="14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B136" s="22" t="s">
         <v>104</v>
@@ -6103,12 +6067,12 @@
         <v>1</v>
       </c>
       <c r="H136" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="B137" s="22" t="s">
         <v>105</v>
@@ -6129,12 +6093,12 @@
         <v>1</v>
       </c>
       <c r="H137" s="14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B138" s="22" t="s">
         <v>106</v>
@@ -6155,12 +6119,12 @@
         <v>1</v>
       </c>
       <c r="H138" s="14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="B139" s="22" t="s">
         <v>107</v>
@@ -6181,12 +6145,12 @@
         <v>1</v>
       </c>
       <c r="H139" s="14" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B140" s="22" t="s">
         <v>108</v>
@@ -6207,12 +6171,12 @@
         <v>1</v>
       </c>
       <c r="H140" s="14" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="B141" s="22" t="s">
         <v>109</v>
@@ -6233,12 +6197,12 @@
         <v>1</v>
       </c>
       <c r="H141" s="14" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B142" s="22" t="s">
         <v>110</v>
@@ -6259,12 +6223,12 @@
         <v>1</v>
       </c>
       <c r="H142" s="14" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="B143" s="22" t="s">
         <v>111</v>
@@ -6285,12 +6249,12 @@
         <v>1</v>
       </c>
       <c r="H143" s="14" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B144" s="22" t="s">
         <v>112</v>
@@ -6311,12 +6275,12 @@
         <v>1</v>
       </c>
       <c r="H144" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B145" s="14" t="s">
         <v>113</v>
@@ -6337,12 +6301,12 @@
         <v>1</v>
       </c>
       <c r="H145" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>114</v>
@@ -6368,7 +6332,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B147" s="14" t="s">
         <v>115</v>
@@ -6389,12 +6353,12 @@
         <v>0</v>
       </c>
       <c r="H147" s="14" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
-        <v>609</v>
+        <v>562</v>
       </c>
       <c r="B148" s="14" t="s">
         <v>116</v>
@@ -6415,12 +6379,12 @@
         <v>0</v>
       </c>
       <c r="H148" s="14" t="s">
-        <v>612</v>
+        <v>565</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B149" s="14" t="s">
         <v>117</v>
@@ -6441,12 +6405,12 @@
         <v>0</v>
       </c>
       <c r="H149" s="14" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B150" s="14" t="s">
         <v>118</v>
@@ -6467,15 +6431,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
-        <v>620</v>
+        <v>573</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>610</v>
+        <v>563</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6493,12 +6457,12 @@
         <v>0</v>
       </c>
       <c r="H151" s="14" t="s">
-        <v>611</v>
+        <v>564</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B152" s="14" t="s">
         <v>119</v>
@@ -6519,15 +6483,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="14" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="15" t="s">
-        <v>661</v>
+        <v>614</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>662</v>
+        <v>615</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6545,15 +6509,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="15" t="s">
-        <v>663</v>
+        <v>616</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="15" t="s">
-        <v>664</v>
+        <v>617</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>665</v>
+        <v>618</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6571,15 +6535,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="15" t="s">
-        <v>666</v>
+        <v>619</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="15" t="s">
-        <v>667</v>
+        <v>620</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>668</v>
+        <v>621</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6597,15 +6561,15 @@
         <v>0</v>
       </c>
       <c r="H155" s="15" t="s">
-        <v>669</v>
+        <v>622</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="15" t="s">
-        <v>670</v>
+        <v>623</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>671</v>
+        <v>624</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -6623,15 +6587,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="15" t="s">
-        <v>672</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="15" t="s">
-        <v>673</v>
+        <v>626</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>674</v>
+        <v>627</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6649,15 +6613,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="15" t="s">
-        <v>675</v>
+        <v>628</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="15" t="s">
-        <v>676</v>
+        <v>629</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>677</v>
+        <v>630</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6675,15 +6639,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="15" t="s">
-        <v>678</v>
+        <v>631</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="15" t="s">
-        <v>679</v>
+        <v>632</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>680</v>
+        <v>633</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6701,15 +6665,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="15" t="s">
-        <v>681</v>
+        <v>634</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="15" t="s">
-        <v>682</v>
+        <v>635</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>683</v>
+        <v>636</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6727,15 +6691,15 @@
         <v>0</v>
       </c>
       <c r="H160" s="15" t="s">
-        <v>684</v>
+        <v>637</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="15" t="s">
-        <v>685</v>
+        <v>638</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>686</v>
+        <v>639</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6753,15 +6717,15 @@
         <v>0</v>
       </c>
       <c r="H161" s="15" t="s">
-        <v>687</v>
+        <v>640</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="15" t="s">
-        <v>688</v>
+        <v>641</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>689</v>
+        <v>642</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6779,15 +6743,15 @@
         <v>0</v>
       </c>
       <c r="H162" s="15" t="s">
-        <v>690</v>
+        <v>643</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="15" t="s">
-        <v>691</v>
+        <v>644</v>
       </c>
       <c r="B163" s="15" t="s">
-        <v>692</v>
+        <v>645</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6805,15 +6769,15 @@
         <v>0</v>
       </c>
       <c r="H163" s="15" t="s">
-        <v>693</v>
+        <v>646</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="15" t="s">
-        <v>694</v>
+        <v>647</v>
       </c>
       <c r="B164" s="15" t="s">
-        <v>695</v>
+        <v>648</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6831,15 +6795,15 @@
         <v>0</v>
       </c>
       <c r="H164" s="15" t="s">
-        <v>696</v>
+        <v>649</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="15" t="s">
-        <v>697</v>
+        <v>650</v>
       </c>
       <c r="B165" s="15" t="s">
-        <v>698</v>
+        <v>651</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6857,12 +6821,12 @@
         <v>0</v>
       </c>
       <c r="H165" s="15" t="s">
-        <v>699</v>
+        <v>652</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="14" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B166" s="14" t="s">
         <v>120</v>
@@ -6883,12 +6847,12 @@
         <v>0</v>
       </c>
       <c r="H166" s="14" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="14" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B167" s="14" t="s">
         <v>121</v>
@@ -6909,15 +6873,15 @@
         <v>0</v>
       </c>
       <c r="H167" s="14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="15" t="s">
-        <v>597</v>
+        <v>550</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>603</v>
+        <v>556</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6935,15 +6899,15 @@
         <v>0</v>
       </c>
       <c r="H168" s="15" t="s">
-        <v>613</v>
+        <v>566</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="15" t="s">
-        <v>598</v>
+        <v>551</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>604</v>
+        <v>557</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6961,15 +6925,15 @@
         <v>0</v>
       </c>
       <c r="H169" s="15" t="s">
-        <v>614</v>
+        <v>567</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="15" t="s">
-        <v>599</v>
+        <v>552</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>605</v>
+        <v>558</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6987,15 +6951,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="15" t="s">
-        <v>615</v>
+        <v>568</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="15" t="s">
-        <v>600</v>
+        <v>553</v>
       </c>
       <c r="B171" s="15" t="s">
-        <v>606</v>
+        <v>559</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -7013,15 +6977,15 @@
         <v>0</v>
       </c>
       <c r="H171" s="15" t="s">
-        <v>616</v>
+        <v>569</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="15" t="s">
-        <v>601</v>
+        <v>554</v>
       </c>
       <c r="B172" s="15" t="s">
-        <v>607</v>
+        <v>560</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -7039,15 +7003,15 @@
         <v>0</v>
       </c>
       <c r="H172" s="15" t="s">
-        <v>617</v>
+        <v>570</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="15" t="s">
-        <v>602</v>
+        <v>555</v>
       </c>
       <c r="B173" s="15" t="s">
-        <v>608</v>
+        <v>561</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -7065,12 +7029,12 @@
         <v>0</v>
       </c>
       <c r="H173" s="15" t="s">
-        <v>618</v>
+        <v>571</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="14" t="s">
-        <v>619</v>
+        <v>572</v>
       </c>
       <c r="B174" s="14" t="s">
         <v>122</v>
@@ -7091,15 +7055,15 @@
         <v>0</v>
       </c>
       <c r="H174" s="14" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="14" t="s">
-        <v>579</v>
+        <v>532</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>541</v>
+        <v>494</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -7117,15 +7081,15 @@
         <v>0</v>
       </c>
       <c r="H175" s="14" t="s">
-        <v>523</v>
+        <v>476</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="14" t="s">
-        <v>580</v>
+        <v>533</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>542</v>
+        <v>495</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -7143,15 +7107,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="14" t="s">
-        <v>524</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="14" t="s">
-        <v>581</v>
+        <v>534</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>548</v>
+        <v>501</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -7169,15 +7133,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="14" t="s">
-        <v>525</v>
+        <v>478</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="14" t="s">
-        <v>582</v>
+        <v>535</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>543</v>
+        <v>496</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -7195,15 +7159,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="14" t="s">
-        <v>526</v>
+        <v>479</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="14" t="s">
-        <v>583</v>
+        <v>536</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>549</v>
+        <v>502</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -7221,15 +7185,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="14" t="s">
-        <v>527</v>
+        <v>480</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="14" t="s">
-        <v>584</v>
+        <v>537</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>550</v>
+        <v>503</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -7247,15 +7211,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="14" t="s">
-        <v>528</v>
+        <v>481</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="14" t="s">
-        <v>585</v>
+        <v>538</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>544</v>
+        <v>497</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7273,15 +7237,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="14" t="s">
-        <v>529</v>
+        <v>482</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="14" t="s">
-        <v>586</v>
+        <v>539</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>551</v>
+        <v>504</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7299,15 +7263,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="14" t="s">
-        <v>530</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
-        <v>587</v>
+        <v>540</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>545</v>
+        <v>498</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7325,15 +7289,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="14" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="14" t="s">
-        <v>588</v>
+        <v>541</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>552</v>
+        <v>505</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7351,15 +7315,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="14" t="s">
-        <v>532</v>
+        <v>485</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="14" t="s">
-        <v>589</v>
+        <v>542</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>553</v>
+        <v>506</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7377,15 +7341,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="14" t="s">
-        <v>533</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="14" t="s">
-        <v>590</v>
+        <v>543</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>554</v>
+        <v>507</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7403,15 +7367,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="14" t="s">
-        <v>534</v>
+        <v>487</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="14" t="s">
-        <v>591</v>
+        <v>544</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>546</v>
+        <v>499</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7429,15 +7393,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="14" t="s">
-        <v>535</v>
+        <v>488</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="14" t="s">
-        <v>592</v>
+        <v>545</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>555</v>
+        <v>508</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7455,15 +7419,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="14" t="s">
-        <v>536</v>
+        <v>489</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="14" t="s">
-        <v>593</v>
+        <v>546</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>547</v>
+        <v>500</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7481,15 +7445,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="14" t="s">
-        <v>537</v>
+        <v>490</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="14" t="s">
-        <v>594</v>
+        <v>547</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>556</v>
+        <v>509</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7507,15 +7471,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="14" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="14" t="s">
-        <v>595</v>
+        <v>548</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>558</v>
+        <v>511</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7533,15 +7497,15 @@
         <v>0</v>
       </c>
       <c r="H191" s="14" t="s">
-        <v>539</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="14" t="s">
-        <v>596</v>
+        <v>549</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>557</v>
+        <v>510</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7559,12 +7523,12 @@
         <v>0</v>
       </c>
       <c r="H192" s="14" t="s">
-        <v>540</v>
+        <v>493</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="14" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B193" s="14" t="s">
         <v>123</v>
@@ -7585,12 +7549,12 @@
         <v>0</v>
       </c>
       <c r="H193" s="14" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
-        <v>559</v>
+        <v>512</v>
       </c>
       <c r="B194" s="14" t="s">
         <v>124</v>
@@ -7611,12 +7575,12 @@
         <v>0</v>
       </c>
       <c r="H194" s="14" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B195" s="14" t="s">
         <v>125</v>
@@ -7637,12 +7601,12 @@
         <v>1</v>
       </c>
       <c r="H195" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="14" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B196" s="14" t="s">
         <v>126</v>
@@ -7663,15 +7627,15 @@
         <v>1</v>
       </c>
       <c r="H196" s="14" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="14" t="s">
-        <v>573</v>
+        <v>526</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>574</v>
+        <v>527</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7689,15 +7653,15 @@
         <v>1</v>
       </c>
       <c r="H197" s="14" t="s">
-        <v>575</v>
+        <v>528</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="14" t="s">
-        <v>576</v>
+        <v>529</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>577</v>
+        <v>530</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7715,12 +7679,12 @@
         <v>1</v>
       </c>
       <c r="H198" s="14" t="s">
-        <v>578</v>
+        <v>531</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B199" s="22" t="s">
         <v>127</v>
@@ -7741,12 +7705,12 @@
         <v>0</v>
       </c>
       <c r="H199" s="14" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="14" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B200" s="22" t="s">
         <v>128</v>
@@ -7767,12 +7731,12 @@
         <v>0</v>
       </c>
       <c r="H200" s="14" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B201" s="14" t="s">
         <v>129</v>
@@ -7793,12 +7757,12 @@
         <v>0</v>
       </c>
       <c r="H201" s="14" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="B202" s="14" t="s">
         <v>130</v>
@@ -7819,12 +7783,12 @@
         <v>0</v>
       </c>
       <c r="H202" s="14" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
-        <v>454</v>
+        <v>657</v>
       </c>
       <c r="B203" s="14" t="s">
         <v>131</v>
@@ -7845,12 +7809,12 @@
         <v>0</v>
       </c>
       <c r="H203" s="14" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
-        <v>455</v>
+        <v>658</v>
       </c>
       <c r="B204" s="14" t="s">
         <v>132</v>
@@ -7871,12 +7835,12 @@
         <v>0</v>
       </c>
       <c r="H204" s="14" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="14" t="s">
-        <v>456</v>
+        <v>656</v>
       </c>
       <c r="B205" s="14" t="s">
         <v>133</v>
@@ -7897,12 +7861,12 @@
         <v>1</v>
       </c>
       <c r="H205" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
-        <v>457</v>
+        <v>655</v>
       </c>
       <c r="B206" s="14" t="s">
         <v>134</v>
@@ -7923,12 +7887,12 @@
         <v>1</v>
       </c>
       <c r="H206" s="14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
-        <v>458</v>
+        <v>659</v>
       </c>
       <c r="B207" s="14" t="s">
         <v>135</v>
@@ -7949,12 +7913,12 @@
         <v>0</v>
       </c>
       <c r="H207" s="14" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="14" t="s">
-        <v>459</v>
+        <v>660</v>
       </c>
       <c r="B208" s="14" t="s">
         <v>136</v>
@@ -7975,12 +7939,12 @@
         <v>0</v>
       </c>
       <c r="H208" s="14" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="14" t="s">
-        <v>460</v>
+        <v>661</v>
       </c>
       <c r="B209" s="14" t="s">
         <v>137</v>
@@ -8001,12 +7965,12 @@
         <v>0</v>
       </c>
       <c r="H209" s="14" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="14" t="s">
-        <v>461</v>
+        <v>662</v>
       </c>
       <c r="B210" s="14" t="s">
         <v>138</v>
@@ -8027,12 +7991,12 @@
         <v>0</v>
       </c>
       <c r="H210" s="14" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="14" t="s">
-        <v>462</v>
+        <v>663</v>
       </c>
       <c r="B211" s="14" t="s">
         <v>139</v>
@@ -8053,12 +8017,12 @@
         <v>0</v>
       </c>
       <c r="H211" s="14" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" s="14" t="s">
-        <v>463</v>
+        <v>664</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>140</v>
@@ -8079,12 +8043,12 @@
         <v>0</v>
       </c>
       <c r="H212" s="14" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="14" t="s">
-        <v>464</v>
+        <v>665</v>
       </c>
       <c r="B213" s="14" t="s">
         <v>141</v>
@@ -8105,12 +8069,12 @@
         <v>0</v>
       </c>
       <c r="H213" s="14" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="14" t="s">
-        <v>465</v>
+        <v>666</v>
       </c>
       <c r="B214" s="14" t="s">
         <v>142</v>
@@ -8131,12 +8095,12 @@
         <v>0</v>
       </c>
       <c r="H214" s="14" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="14" t="s">
-        <v>466</v>
+        <v>667</v>
       </c>
       <c r="B215" s="14" t="s">
         <v>143</v>
@@ -8157,12 +8121,12 @@
         <v>0</v>
       </c>
       <c r="H215" s="14" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="14" t="s">
-        <v>467</v>
+        <v>668</v>
       </c>
       <c r="B216" s="14" t="s">
         <v>144</v>
@@ -8183,12 +8147,12 @@
         <v>0</v>
       </c>
       <c r="H216" s="14" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="14" t="s">
-        <v>468</v>
+        <v>669</v>
       </c>
       <c r="B217" s="14" t="s">
         <v>145</v>
@@ -8209,12 +8173,12 @@
         <v>0</v>
       </c>
       <c r="H217" s="14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" s="14" t="s">
-        <v>469</v>
+        <v>670</v>
       </c>
       <c r="B218" s="14" t="s">
         <v>146</v>
@@ -8235,12 +8199,12 @@
         <v>0</v>
       </c>
       <c r="H218" s="14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="14" t="s">
-        <v>470</v>
+        <v>671</v>
       </c>
       <c r="B219" s="14" t="s">
         <v>147</v>
@@ -8261,12 +8225,12 @@
         <v>0</v>
       </c>
       <c r="H219" s="14" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" s="14" t="s">
-        <v>471</v>
+        <v>672</v>
       </c>
       <c r="B220" s="14" t="s">
         <v>148</v>
@@ -8280,19 +8244,19 @@
       <c r="E220" s="17">
         <v>1</v>
       </c>
-      <c r="F220" s="19">
+      <c r="F220" s="17">
         <v>1</v>
       </c>
       <c r="G220" s="3">
         <v>0</v>
       </c>
       <c r="H220" s="14" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" s="14" t="s">
-        <v>472</v>
+        <v>673</v>
       </c>
       <c r="B221" s="14" t="s">
         <v>149</v>
@@ -8313,12 +8277,12 @@
         <v>0</v>
       </c>
       <c r="H221" s="14" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" s="14" t="s">
-        <v>473</v>
+        <v>674</v>
       </c>
       <c r="B222" s="14" t="s">
         <v>150</v>
@@ -8339,12 +8303,12 @@
         <v>0</v>
       </c>
       <c r="H222" s="14" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="14" t="s">
-        <v>474</v>
+        <v>675</v>
       </c>
       <c r="B223" s="14" t="s">
         <v>151</v>
@@ -8365,12 +8329,12 @@
         <v>0</v>
       </c>
       <c r="H223" s="14" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" s="14" t="s">
-        <v>475</v>
+        <v>676</v>
       </c>
       <c r="B224" s="14" t="s">
         <v>152</v>
@@ -8384,19 +8348,19 @@
       <c r="E224" s="17">
         <v>1</v>
       </c>
-      <c r="F224" s="17">
+      <c r="F224" s="19">
         <v>1</v>
       </c>
       <c r="G224" s="3">
         <v>0</v>
       </c>
       <c r="H224" s="14" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" s="14" t="s">
-        <v>476</v>
+        <v>681</v>
       </c>
       <c r="B225" s="14" t="s">
         <v>153</v>
@@ -8417,12 +8381,12 @@
         <v>0</v>
       </c>
       <c r="H225" s="14" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="14" t="s">
-        <v>477</v>
+        <v>677</v>
       </c>
       <c r="B226" s="14" t="s">
         <v>154</v>
@@ -8443,12 +8407,12 @@
         <v>0</v>
       </c>
       <c r="H226" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" s="14" t="s">
-        <v>478</v>
+        <v>678</v>
       </c>
       <c r="B227" s="14" t="s">
         <v>155</v>
@@ -8469,12 +8433,12 @@
         <v>0</v>
       </c>
       <c r="H227" s="14" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" s="14" t="s">
-        <v>479</v>
+        <v>679</v>
       </c>
       <c r="B228" s="14" t="s">
         <v>156</v>
@@ -8495,12 +8459,12 @@
         <v>0</v>
       </c>
       <c r="H228" s="14" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" s="14" t="s">
-        <v>480</v>
+        <v>680</v>
       </c>
       <c r="B229" s="14" t="s">
         <v>157</v>
@@ -8521,116 +8485,116 @@
         <v>0</v>
       </c>
       <c r="H229" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A230" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="B230" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C230" s="2">
+        <v>0</v>
+      </c>
+      <c r="D230" s="2">
+        <v>0</v>
+      </c>
+      <c r="E230" s="17">
+        <v>1</v>
+      </c>
+      <c r="F230" s="19">
+        <v>1</v>
+      </c>
+      <c r="G230" s="3">
+        <v>0</v>
+      </c>
+      <c r="H230" s="15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A231" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="B231" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C231" s="2">
+        <v>0</v>
+      </c>
+      <c r="D231" s="2">
+        <v>0</v>
+      </c>
+      <c r="E231" s="17">
+        <v>1</v>
+      </c>
+      <c r="F231" s="19">
+        <v>1</v>
+      </c>
+      <c r="G231" s="3">
+        <v>0</v>
+      </c>
+      <c r="H231" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A232" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="B232" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C232" s="2">
+        <v>0</v>
+      </c>
+      <c r="D232" s="2">
+        <v>0</v>
+      </c>
+      <c r="E232" s="17">
+        <v>1</v>
+      </c>
+      <c r="F232" s="19">
+        <v>1</v>
+      </c>
+      <c r="G232" s="3">
+        <v>0</v>
+      </c>
+      <c r="H232" s="15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A233" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="B233" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C233" s="2">
+        <v>0</v>
+      </c>
+      <c r="D233" s="2">
+        <v>0</v>
+      </c>
+      <c r="E233" s="17">
+        <v>1</v>
+      </c>
+      <c r="F233" s="19">
+        <v>1</v>
+      </c>
+      <c r="G233" s="3">
+        <v>0</v>
+      </c>
+      <c r="H233" s="15" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A230" s="14" t="s">
-        <v>481</v>
-      </c>
-      <c r="B230" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C230" s="2">
-        <v>0</v>
-      </c>
-      <c r="D230" s="2">
-        <v>0</v>
-      </c>
-      <c r="E230" s="17">
-        <v>1</v>
-      </c>
-      <c r="F230" s="19">
-        <v>1</v>
-      </c>
-      <c r="G230" s="3">
-        <v>0</v>
-      </c>
-      <c r="H230" s="14" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A231" s="14" t="s">
-        <v>482</v>
-      </c>
-      <c r="B231" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C231" s="2">
-        <v>0</v>
-      </c>
-      <c r="D231" s="2">
-        <v>0</v>
-      </c>
-      <c r="E231" s="17">
-        <v>1</v>
-      </c>
-      <c r="F231" s="19">
-        <v>1</v>
-      </c>
-      <c r="G231" s="3">
-        <v>0</v>
-      </c>
-      <c r="H231" s="14" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A232" s="14" t="s">
-        <v>483</v>
-      </c>
-      <c r="B232" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C232" s="2">
-        <v>0</v>
-      </c>
-      <c r="D232" s="2">
-        <v>0</v>
-      </c>
-      <c r="E232" s="17">
-        <v>1</v>
-      </c>
-      <c r="F232" s="19">
-        <v>1</v>
-      </c>
-      <c r="G232" s="3">
-        <v>0</v>
-      </c>
-      <c r="H232" s="14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A233" s="14" t="s">
-        <v>484</v>
-      </c>
-      <c r="B233" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C233" s="2">
-        <v>0</v>
-      </c>
-      <c r="D233" s="2">
-        <v>0</v>
-      </c>
-      <c r="E233" s="17">
-        <v>1</v>
-      </c>
-      <c r="F233" s="19">
-        <v>1</v>
-      </c>
-      <c r="G233" s="3">
-        <v>0</v>
-      </c>
-      <c r="H233" s="14" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" s="15" t="s">
-        <v>485</v>
+        <v>686</v>
       </c>
       <c r="B234" s="15" t="s">
         <v>162</v>
@@ -8651,12 +8615,12 @@
         <v>0</v>
       </c>
       <c r="H234" s="15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" s="15" t="s">
-        <v>486</v>
+        <v>687</v>
       </c>
       <c r="B235" s="15" t="s">
         <v>163</v>
@@ -8677,12 +8641,12 @@
         <v>0</v>
       </c>
       <c r="H235" s="15" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" s="15" t="s">
-        <v>487</v>
+        <v>688</v>
       </c>
       <c r="B236" s="15" t="s">
         <v>164</v>
@@ -8703,12 +8667,12 @@
         <v>0</v>
       </c>
       <c r="H236" s="15" t="s">
-        <v>328</v>
+        <v>209</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" s="15" t="s">
-        <v>488</v>
+        <v>689</v>
       </c>
       <c r="B237" s="15" t="s">
         <v>165</v>
@@ -8722,144 +8686,40 @@
       <c r="E237" s="17">
         <v>1</v>
       </c>
-      <c r="F237" s="19">
+      <c r="F237" s="17">
         <v>1</v>
       </c>
       <c r="G237" s="3">
         <v>0</v>
       </c>
       <c r="H237" s="15" t="s">
-        <v>329</v>
+        <v>208</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A238" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="B238" s="15" t="s">
-        <v>166</v>
+      <c r="A238" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>592</v>
       </c>
       <c r="C238" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D238" s="2">
-        <v>0</v>
-      </c>
-      <c r="E238" s="17">
-        <v>1</v>
-      </c>
-      <c r="F238" s="19">
+        <v>1</v>
+      </c>
+      <c r="E238" s="4">
+        <v>1</v>
+      </c>
+      <c r="F238" s="3">
         <v>1</v>
       </c>
       <c r="G238" s="3">
         <v>0</v>
       </c>
-      <c r="H238" s="15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A239" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="B239" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C239" s="2">
-        <v>0</v>
-      </c>
-      <c r="D239" s="2">
-        <v>0</v>
-      </c>
-      <c r="E239" s="17">
-        <v>1</v>
-      </c>
-      <c r="F239" s="19">
-        <v>1</v>
-      </c>
-      <c r="G239" s="3">
-        <v>0</v>
-      </c>
-      <c r="H239" s="15" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A240" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="B240" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C240" s="2">
-        <v>0</v>
-      </c>
-      <c r="D240" s="2">
-        <v>0</v>
-      </c>
-      <c r="E240" s="17">
-        <v>1</v>
-      </c>
-      <c r="F240" s="19">
-        <v>1</v>
-      </c>
-      <c r="G240" s="3">
-        <v>0</v>
-      </c>
-      <c r="H240" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A241" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="B241" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C241" s="2">
-        <v>0</v>
-      </c>
-      <c r="D241" s="2">
-        <v>0</v>
-      </c>
-      <c r="E241" s="17">
-        <v>1</v>
-      </c>
-      <c r="F241" s="17">
-        <v>1</v>
-      </c>
-      <c r="G241" s="3">
-        <v>0</v>
-      </c>
-      <c r="H241" s="15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A242" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="B242" s="5" t="s">
-        <v>639</v>
-      </c>
-      <c r="C242" s="2">
-        <v>1</v>
-      </c>
-      <c r="D242" s="2">
-        <v>1</v>
-      </c>
-      <c r="E242" s="4">
-        <v>1</v>
-      </c>
-      <c r="F242" s="3">
-        <v>1</v>
-      </c>
-      <c r="G242" s="3">
-        <v>0</v>
-      </c>
-      <c r="H242" s="5" t="s">
-        <v>640</v>
+      <c r="H238" s="5" t="s">
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data export for Kenya lock
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -6161,7 +6161,7 @@
   <dimension ref="A1:P406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6975,7 +6975,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="2">
         <v>0</v>
@@ -7075,7 +7075,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Update Kenya soft lock
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -6837,7 +6837,7 @@
   <dimension ref="A1:Q410"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8250,7 +8250,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -8303,7 +8303,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -8356,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -8459,22 +8459,22 @@
         <v>435</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="2">
         <v>0</v>
@@ -8515,7 +8515,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
@@ -8568,7 +8568,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Updates for Kenya soft lock
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -3018,9 +3018,6 @@
     <t>fs_name_check</t>
   </si>
   <si>
-    <t>crfs-t02c-a4_a_5_2</t>
-  </si>
-  <si>
     <t>ls_name_check</t>
   </si>
   <si>
@@ -3034,6 +3031,9 @@
   </si>
   <si>
     <t>sd_start</t>
+  </si>
+  <si>
+    <t>crfs-t02c-a4_a_5_3</t>
   </si>
 </sst>
 </file>
@@ -6836,8 +6836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q410"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7393,11 +7393,11 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
+        <v>997</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>998</v>
       </c>
-      <c r="B11" s="35" t="s">
-        <v>999</v>
-      </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
@@ -7446,11 +7446,11 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
+        <v>999</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>1000</v>
       </c>
-      <c r="B12" s="35" t="s">
-        <v>1001</v>
-      </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
@@ -11324,7 +11324,7 @@
         <v>0</v>
       </c>
       <c r="D85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" s="2">
         <v>0</v>
@@ -11352,16 +11352,16 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>996</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>997</v>
-      </c>
       <c r="C86" s="1">
         <v>0</v>
       </c>
       <c r="D86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Update fonts to see if it fixes JA's issue
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="1001">
   <si>
     <t>old</t>
   </si>
@@ -3028,6 +3028,9 @@
   </si>
   <si>
     <t>rx_misc_oth_hf</t>
+  </si>
+  <si>
+    <t>antibiotics_hf</t>
   </si>
 </sst>
 </file>
@@ -6830,8 +6833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J248" sqref="J248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -19943,7 +19946,7 @@
         <v>0</v>
       </c>
       <c r="J248" s="31" t="s">
-        <v>953</v>
+        <v>1000</v>
       </c>
       <c r="K248" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Update repeat visit check + hospitalisation log
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -6833,8 +6833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="R191" sqref="R191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -15191,7 +15191,7 @@
         <v>1</v>
       </c>
       <c r="O158" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P158" s="2">
         <v>1</v>
@@ -15244,7 +15244,7 @@
         <v>1</v>
       </c>
       <c r="O159" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P159" s="2">
         <v>1</v>
@@ -15297,7 +15297,7 @@
         <v>1</v>
       </c>
       <c r="O160" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P160" s="2">
         <v>1</v>
@@ -15350,7 +15350,7 @@
         <v>1</v>
       </c>
       <c r="O161" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P161" s="2">
         <v>1</v>
@@ -15403,7 +15403,7 @@
         <v>1</v>
       </c>
       <c r="O162" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P162" s="2">
         <v>1</v>
@@ -15456,7 +15456,7 @@
         <v>1</v>
       </c>
       <c r="O163" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P163" s="2">
         <v>1</v>
@@ -15509,7 +15509,7 @@
         <v>1</v>
       </c>
       <c r="O164" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P164" s="2">
         <v>1</v>
@@ -15562,7 +15562,7 @@
         <v>1</v>
       </c>
       <c r="O165" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P165" s="2">
         <v>1</v>
@@ -15615,7 +15615,7 @@
         <v>1</v>
       </c>
       <c r="O166" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P166" s="2">
         <v>1</v>
@@ -15668,7 +15668,7 @@
         <v>1</v>
       </c>
       <c r="O167" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P167" s="2">
         <v>1</v>
@@ -28452,7 +28452,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q414"/>
-  <conditionalFormatting sqref="C302:D302 C64:D64 C69:D69 M69 C66:D67 M72 C105:D133 K304 K307 C137:D172 M199 C189:D190 C178:D187 K179:K187 C174:D176 K174:K176 P21:P35 M66:M67 P105:P111 K105:K172 K189:K190 K192:K193 K195 K197 P198:P199 P173:P187 K309:K314 C329:D329 K329 K357:K358 C357:D358 K336 C336:D336 C343:D343 K343 K350 C350:D350 K333:K334 C333:D334 C354:D355 K354:K355 K347:K348 C347:D348 C360:D361 K360:K361 K363:K366 C363:D366 K368:K371 K373:K376 C378:D395 K378:K395 K397:K403 C340:D341 K340:K341 C326:D327 K326:K327 C318:D323 K318:K323 M74 C71:D74 C76:D78 M76:M78 M80:M85 C80:D84 M95 P89:P93 O80:O85 O76:O78 O74 O318:O319 O326:O327 O340:O341 O397:O402 O378:O395 O373:O376 O368:O371 O363:O366 O360:O361 O347:O348 O354:O355 O333:O334 O350 O343 O336 O357:O358 O329 O309:O314 O321:O323 O263 O197:P197 O195:P195 O192:P193 O189:P190 O137:P172 O66:P69 O174:O176 O297:O304 O199 O178:O187 O307 O105:O133 O72 O403:P405 O289 O291 O287 O285 O283 O281 O279 O277 O275 O273 O271 O269 O267 O293 O295 O265 O261:P261 C397:D405 C373:D376 C368:D371 K36:K69 O95:P95 O97:P97 M97 Q95:Q97 C100:D101 C95:D97 K100:K101 K96 M96:P96 M100:P100 M36:P64 M261:N302 M318:M319 M326:M327 M340:M341 M397:M405 M378:M395 M373:M376 M368:M371 M363:M366 M360:M361 M347:M348 M354:M355 M333:M334 M350 M343 M336 M357:M358 M329 M309:M314 M321:M323 M197 M195 M192:M193 M189:M190 M137:M172 M174:M176 M178:M187 M307 M304 M105:M133 M316 Q316:Q323 I316:I323 C316:D316 O316 K316 I325:I329 Q325:Q329 Q331:Q336 I331:I336 M331 O331 K331 C331:D331 I338:I343 Q338:Q343 M338 O338 C338:D338 K338 Q345:Q350 I345:I350 M345 O345 K345 C345:D345 Q352:Q405 M352 O352 C352:D352 K352 C304:D314 Q261:Q314 K261:K302 C261:D300 I261:I300 I304:I314 I95:I97 I100:I101 I352:I405 I80:I84 I76:I78 I71:I74 I174:I176 I178:I187 I189:I190 I137:I172 I105:I133 I66:I67 I69 I64 I302 E17:F84 C17:D62 M9:P9 K17:O35 K6:Q6 K9:L10 K5:L5 O10:P10 O5:Q5 K13:P16 K7:P8 K2:Q4 K406:Q408 C406:F408 H406:I408 Q87:Q93 I87:I88 O87:O88 C87:D88 M87:M88 H2:I10 C2:F10 Q7:Q10 Q13:Q85 C13:F16 H13:I62 Q100:Q240 K201:P240 E260:F405 C192:D244 G192:I244 K241:Q244 C246:D247 G246:I247 K246:Q259 E87:F247 C248:I259">
+  <conditionalFormatting sqref="C302:D302 C64:D64 C69:D69 M69 C66:D67 M72 C105:D133 K304 K307 C137:D172 M199 C189:D190 C178:D187 K179:K187 C174:D176 K174:K176 P21:P35 M66:M67 P105:P111 K105:K172 K189:K190 K192:K193 K195 K197 P198:P199 P173:P187 K309:K314 C329:D329 K329 K357:K358 C357:D358 K336 C336:D336 C343:D343 K343 K350 C350:D350 K333:K334 C333:D334 C354:D355 K354:K355 K347:K348 C347:D348 C360:D361 K360:K361 K363:K366 C363:D366 K368:K371 K373:K376 C378:D395 K378:K395 K397:K403 C340:D341 K340:K341 C326:D327 K326:K327 C318:D323 K318:K323 M74 C71:D74 C76:D78 M76:M78 M80:M85 C80:D84 M95 P89:P93 O80:O85 O76:O78 O74 O318:O319 O326:O327 O340:O341 O397:O402 O378:O395 O373:O376 O368:O371 O363:O366 O360:O361 O347:O348 O354:O355 O333:O334 O350 O343 O336 O357:O358 O329 O309:O314 O321:O323 O263 O197:P197 O195:P195 O192:P193 O189:P190 O66:P69 O174:O176 O297:O304 O199 O178:O187 O307 O105:O133 O72 O403:P405 O289 O291 O287 O285 O283 O281 O279 O277 O275 O273 O271 O269 O267 O293 O295 O265 O261:P261 C397:D405 C373:D376 C368:D371 K36:K69 O95:P95 O97:P97 M97 Q95:Q97 C100:D101 C95:D97 K100:K101 K96 M96:P96 M100:P100 M36:P64 M261:N302 M318:M319 M326:M327 M340:M341 M397:M405 M378:M395 M373:M376 M368:M371 M363:M366 M360:M361 M347:M348 M354:M355 M333:M334 M350 M343 M336 M357:M358 M329 M309:M314 M321:M323 M197 M195 M192:M193 M189:M190 M137:M172 M174:M176 M178:M187 M307 M304 M105:M133 M316 Q316:Q323 I316:I323 C316:D316 O316 K316 I325:I329 Q325:Q329 Q331:Q336 I331:I336 M331 O331 K331 C331:D331 I338:I343 Q338:Q343 M338 O338 C338:D338 K338 Q345:Q350 I345:I350 M345 O345 K345 C345:D345 Q352:Q405 M352 O352 C352:D352 K352 C304:D314 Q261:Q314 K261:K302 C261:D300 I261:I300 I304:I314 I95:I97 I100:I101 I352:I405 I80:I84 I76:I78 I71:I74 I174:I176 I178:I187 I189:I190 I137:I172 I105:I133 I66:I67 I69 I64 I302 E17:F84 C17:D62 M9:P9 K17:O35 K6:Q6 K9:L10 K5:L5 O10:P10 O5:Q5 K13:P16 K7:P8 K2:Q4 K406:Q408 C406:F408 H406:I408 Q87:Q93 I87:I88 O87:O88 C87:D88 M87:M88 H2:I10 C2:F10 Q7:Q10 Q13:Q85 C13:F16 H13:I62 Q100:Q240 K201:P240 E260:F405 C192:D244 G192:I244 K241:Q244 C246:D247 G246:I247 K246:Q259 E87:F247 C248:I259 O137:P172">
     <cfRule type="cellIs" dxfId="329" priority="352" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update time-flow data cleaning + minor aspects
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict.xlsx
+++ b/inst/extdata/main_dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6810,32 +6810,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.58203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.25" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.08203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.08203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>487</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>454</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
         <v>461</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>27</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>485</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>486</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>532</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>530</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>991</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
         <v>993</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>468</v>
       </c>
@@ -7479,22 +7479,22 @@
         <v>469</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -7524,7 +7524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>470</v>
       </c>
@@ -7532,22 +7532,22 @@
         <v>471</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -7577,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>472</v>
       </c>
@@ -7585,22 +7585,22 @@
         <v>473</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -7630,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>474</v>
       </c>
@@ -7638,22 +7638,22 @@
         <v>475</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -7683,7 +7683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>534</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>476</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>535</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>478</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>326</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>292</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>293</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>430</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>294</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>295</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>435</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>296</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>297</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>298</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>434</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>300</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>301</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>302</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>299</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>310</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>311</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>312</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>313</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
         <v>303</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>304</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>305</v>
       </c>
@@ -9061,7 +9061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="s">
         <v>306</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="s">
         <v>307</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="27" t="s">
         <v>308</v>
       </c>
@@ -9220,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
         <v>309</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
         <v>446</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
         <v>450</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>314</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>315</v>
       </c>
@@ -9485,7 +9485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>316</v>
       </c>
@@ -9538,7 +9538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>317</v>
       </c>
@@ -9591,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>318</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>319</v>
       </c>
@@ -9697,7 +9697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>320</v>
       </c>
@@ -9750,7 +9750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>321</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>322</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>323</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>324</v>
       </c>
@@ -9962,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>515</v>
       </c>
@@ -10015,7 +10015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>518</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>325</v>
       </c>
@@ -10121,7 +10121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>768</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>328</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>775</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>329</v>
       </c>
@@ -10333,7 +10333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>327</v>
       </c>
@@ -10386,7 +10386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>985</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>680</v>
       </c>
@@ -10492,7 +10492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>772</v>
       </c>
@@ -10545,7 +10545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>880</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
         <v>465</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>881</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>466</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>882</v>
       </c>
@@ -10810,7 +10810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
         <v>462</v>
       </c>
@@ -10863,7 +10863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>463</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>482</v>
       </c>
@@ -10969,7 +10969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>883</v>
       </c>
@@ -11022,7 +11022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
         <v>464</v>
       </c>
@@ -11075,7 +11075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
         <v>683</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>438</v>
       </c>
@@ -11181,7 +11181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>330</v>
       </c>
@@ -11234,7 +11234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>331</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>988</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
         <v>995</v>
       </c>
@@ -11393,7 +11393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
         <v>442</v>
       </c>
@@ -11446,7 +11446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>444</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>778</v>
       </c>
@@ -11552,7 +11552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
         <v>779</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
         <v>782</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
         <v>785</v>
       </c>
@@ -11711,7 +11711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>788</v>
       </c>
@@ -11764,7 +11764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
         <v>967</v>
       </c>
@@ -11817,7 +11817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>467</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
         <v>884</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
         <v>968</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
         <v>493</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>969</v>
       </c>
@@ -12082,7 +12082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
         <v>495</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
         <v>855</v>
       </c>
@@ -12188,7 +12188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>791</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>793</v>
       </c>
@@ -12294,7 +12294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>796</v>
       </c>
@@ -12347,7 +12347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>756</v>
       </c>
@@ -12400,7 +12400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
         <v>332</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
         <v>333</v>
       </c>
@@ -12506,7 +12506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
         <v>689</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
         <v>334</v>
       </c>
@@ -12612,7 +12612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="s">
         <v>335</v>
       </c>
@@ -12665,7 +12665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>511</v>
       </c>
@@ -12718,7 +12718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>336</v>
       </c>
@@ -12771,7 +12771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
         <v>692</v>
       </c>
@@ -12824,7 +12824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="s">
         <v>695</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="s">
         <v>698</v>
       </c>
@@ -12930,7 +12930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="s">
         <v>701</v>
       </c>
@@ -12983,7 +12983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
         <v>704</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
         <v>707</v>
       </c>
@@ -13089,7 +13089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
         <v>710</v>
       </c>
@@ -13142,7 +13142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>337</v>
       </c>
@@ -13195,7 +13195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
         <v>338</v>
       </c>
@@ -13248,7 +13248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
         <v>339</v>
       </c>
@@ -13301,7 +13301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
         <v>340</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
         <v>341</v>
       </c>
@@ -13407,7 +13407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
         <v>342</v>
       </c>
@@ -13460,7 +13460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
         <v>343</v>
       </c>
@@ -13513,7 +13513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="s">
         <v>344</v>
       </c>
@@ -13566,7 +13566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="s">
         <v>345</v>
       </c>
@@ -13619,7 +13619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="s">
         <v>346</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="s">
         <v>347</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="s">
         <v>348</v>
       </c>
@@ -13778,7 +13778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="12" t="s">
         <v>349</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="s">
         <v>350</v>
       </c>
@@ -13884,7 +13884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="28" t="s">
         <v>799</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" s="29" t="s">
         <v>800</v>
       </c>
@@ -13990,7 +13990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="29" t="s">
         <v>803</v>
       </c>
@@ -14043,7 +14043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
         <v>351</v>
       </c>
@@ -14096,7 +14096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>352</v>
       </c>
@@ -14149,7 +14149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>353</v>
       </c>
@@ -14202,7 +14202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
         <v>354</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
         <v>355</v>
       </c>
@@ -14308,7 +14308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>356</v>
       </c>
@@ -14361,7 +14361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>357</v>
       </c>
@@ -14414,7 +14414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>358</v>
       </c>
@@ -14467,7 +14467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>359</v>
       </c>
@@ -14520,7 +14520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>360</v>
       </c>
@@ -14573,7 +14573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>361</v>
       </c>
@@ -14626,7 +14626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>362</v>
       </c>
@@ -14679,7 +14679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>363</v>
       </c>
@@ -14732,7 +14732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
         <v>364</v>
       </c>
@@ -14785,7 +14785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
         <v>365</v>
       </c>
@@ -14838,7 +14838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
         <v>366</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>367</v>
       </c>
@@ -14944,7 +14944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
         <v>368</v>
       </c>
@@ -14997,7 +14997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
         <v>369</v>
       </c>
@@ -15050,7 +15050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
         <v>370</v>
       </c>
@@ -15103,7 +15103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
         <v>371</v>
       </c>
@@ -15156,7 +15156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
         <v>372</v>
       </c>
@@ -15209,7 +15209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" s="13" t="s">
         <v>373</v>
       </c>
@@ -15262,7 +15262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
         <v>374</v>
       </c>
@@ -15315,7 +15315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
         <v>375</v>
       </c>
@@ -15368,7 +15368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
         <v>376</v>
       </c>
@@ -15421,7 +15421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
         <v>377</v>
       </c>
@@ -15474,7 +15474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>378</v>
       </c>
@@ -15527,7 +15527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" s="13" t="s">
         <v>379</v>
       </c>
@@ -15580,7 +15580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" s="13" t="s">
         <v>380</v>
       </c>
@@ -15633,7 +15633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" s="13" t="s">
         <v>381</v>
       </c>
@@ -15686,7 +15686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" s="13" t="s">
         <v>748</v>
       </c>
@@ -15739,7 +15739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" s="13" t="s">
         <v>751</v>
       </c>
@@ -15792,7 +15792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" s="24" t="s">
         <v>857</v>
       </c>
@@ -15845,7 +15845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" s="24" t="s">
         <v>754</v>
       </c>
@@ -15898,7 +15898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" s="32" t="s">
         <v>382</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" s="32" t="s">
         <v>852</v>
       </c>
@@ -16004,7 +16004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" s="32" t="s">
         <v>713</v>
       </c>
@@ -16057,7 +16057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" s="32" t="s">
         <v>716</v>
       </c>
@@ -16110,7 +16110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="32" t="s">
         <v>383</v>
       </c>
@@ -16163,7 +16163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="24" t="s">
         <v>845</v>
       </c>
@@ -16216,7 +16216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" s="24" t="s">
         <v>719</v>
       </c>
@@ -16269,7 +16269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" s="13" t="s">
         <v>594</v>
       </c>
@@ -16322,7 +16322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" s="13" t="s">
         <v>499</v>
       </c>
@@ -16375,7 +16375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" s="13" t="s">
         <v>596</v>
       </c>
@@ -16428,7 +16428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" s="13" t="s">
         <v>599</v>
       </c>
@@ -16481,7 +16481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" s="13" t="s">
         <v>602</v>
       </c>
@@ -16534,7 +16534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" s="13" t="s">
         <v>384</v>
       </c>
@@ -16587,7 +16587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="13" t="s">
         <v>501</v>
       </c>
@@ -16640,7 +16640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" s="13" t="s">
         <v>503</v>
       </c>
@@ -16693,7 +16693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" s="13" t="s">
         <v>508</v>
       </c>
@@ -16746,7 +16746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" s="32" t="s">
         <v>848</v>
       </c>
@@ -16799,7 +16799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" s="32" t="s">
         <v>386</v>
       </c>
@@ -16852,7 +16852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" s="32" t="s">
         <v>387</v>
       </c>
@@ -16905,7 +16905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" s="32" t="s">
         <v>849</v>
       </c>
@@ -16958,7 +16958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" s="32" t="s">
         <v>759</v>
       </c>
@@ -17011,7 +17011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" s="32" t="s">
         <v>762</v>
       </c>
@@ -17064,7 +17064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" s="32" t="s">
         <v>850</v>
       </c>
@@ -17117,7 +17117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" s="32" t="s">
         <v>455</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" s="32" t="s">
         <v>851</v>
       </c>
@@ -17223,7 +17223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" s="32" t="s">
         <v>458</v>
       </c>
@@ -17276,7 +17276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" s="24" t="s">
         <v>846</v>
       </c>
@@ -17329,7 +17329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" s="24" t="s">
         <v>388</v>
       </c>
@@ -17382,7 +17382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" s="24" t="s">
         <v>847</v>
       </c>
@@ -17435,7 +17435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" s="24" t="s">
         <v>389</v>
       </c>
@@ -17488,7 +17488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" s="13" t="s">
         <v>605</v>
       </c>
@@ -17541,7 +17541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" s="14" t="s">
         <v>608</v>
       </c>
@@ -17594,7 +17594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" s="14" t="s">
         <v>611</v>
       </c>
@@ -17647,7 +17647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" s="14" t="s">
         <v>614</v>
       </c>
@@ -17700,7 +17700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" s="20" t="s">
         <v>960</v>
       </c>
@@ -17753,7 +17753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" s="14" t="s">
         <v>617</v>
       </c>
@@ -17806,7 +17806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" s="14" t="s">
         <v>623</v>
       </c>
@@ -17859,7 +17859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" s="14" t="s">
         <v>629</v>
       </c>
@@ -17912,7 +17912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" s="14" t="s">
         <v>635</v>
       </c>
@@ -17965,7 +17965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" s="14" t="s">
         <v>638</v>
       </c>
@@ -18018,7 +18018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" s="14" t="s">
         <v>641</v>
       </c>
@@ -18071,7 +18071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="14" t="s">
         <v>644</v>
       </c>
@@ -18124,7 +18124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" s="14" t="s">
         <v>647</v>
       </c>
@@ -18177,7 +18177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" s="14" t="s">
         <v>650</v>
       </c>
@@ -18230,7 +18230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" s="13" t="s">
         <v>653</v>
       </c>
@@ -18283,7 +18283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" s="13" t="s">
         <v>961</v>
       </c>
@@ -18336,7 +18336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" s="13" t="s">
         <v>656</v>
       </c>
@@ -18389,7 +18389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="13" t="s">
         <v>665</v>
       </c>
@@ -18442,7 +18442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
         <v>668</v>
       </c>
@@ -18495,7 +18495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A221" s="13" t="s">
         <v>671</v>
       </c>
@@ -18548,7 +18548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A222" s="13" t="s">
         <v>674</v>
       </c>
@@ -18601,7 +18601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A223" s="13" t="s">
         <v>677</v>
       </c>
@@ -18654,7 +18654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A224" s="14" t="s">
         <v>620</v>
       </c>
@@ -18707,7 +18707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" s="14" t="s">
         <v>626</v>
       </c>
@@ -18760,7 +18760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" s="14" t="s">
         <v>632</v>
       </c>
@@ -18813,7 +18813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" s="14" t="s">
         <v>659</v>
       </c>
@@ -18866,7 +18866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" s="14" t="s">
         <v>662</v>
       </c>
@@ -18919,7 +18919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" s="14" t="s">
         <v>722</v>
       </c>
@@ -18972,7 +18972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" s="14" t="s">
         <v>725</v>
       </c>
@@ -19025,7 +19025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A231" s="31" t="s">
         <v>885</v>
       </c>
@@ -19078,7 +19078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" s="31" t="s">
         <v>886</v>
       </c>
@@ -19131,7 +19131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" s="31" t="s">
         <v>926</v>
       </c>
@@ -19184,7 +19184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" s="31" t="s">
         <v>895</v>
       </c>
@@ -19237,7 +19237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" s="31" t="s">
         <v>887</v>
       </c>
@@ -19290,7 +19290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" s="31" t="s">
         <v>927</v>
       </c>
@@ -19343,7 +19343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" s="31" t="s">
         <v>928</v>
       </c>
@@ -19396,7 +19396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" s="31" t="s">
         <v>888</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" s="31" t="s">
         <v>929</v>
       </c>
@@ -19502,7 +19502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" s="31" t="s">
         <v>889</v>
       </c>
@@ -19555,7 +19555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" s="31" t="s">
         <v>891</v>
       </c>
@@ -19608,7 +19608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="31" t="s">
         <v>892</v>
       </c>
@@ -19661,7 +19661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" s="31" t="s">
         <v>930</v>
       </c>
@@ -19714,7 +19714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" s="31" t="s">
         <v>894</v>
       </c>
@@ -19767,7 +19767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245" s="31" t="s">
         <v>999</v>
       </c>
@@ -19820,7 +19820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246" s="31" t="s">
         <v>932</v>
       </c>
@@ -19873,7 +19873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" s="31" t="s">
         <v>933</v>
       </c>
@@ -19926,7 +19926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" s="31" t="s">
         <v>934</v>
       </c>
@@ -19979,7 +19979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A249" s="31" t="s">
         <v>935</v>
       </c>
@@ -20032,7 +20032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" s="31" t="s">
         <v>898</v>
       </c>
@@ -20085,7 +20085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" s="31" t="s">
         <v>390</v>
       </c>
@@ -20138,7 +20138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252" s="31" t="s">
         <v>391</v>
       </c>
@@ -20191,7 +20191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A253" s="31" t="s">
         <v>890</v>
       </c>
@@ -20244,7 +20244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A254" s="31" t="s">
         <v>893</v>
       </c>
@@ -20297,7 +20297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255" s="31" t="s">
         <v>931</v>
       </c>
@@ -20350,7 +20350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A256" s="31" t="s">
         <v>896</v>
       </c>
@@ -20403,7 +20403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" s="31" t="s">
         <v>897</v>
       </c>
@@ -20456,7 +20456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" s="31" t="s">
         <v>936</v>
       </c>
@@ -20509,7 +20509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" s="31" t="s">
         <v>937</v>
       </c>
@@ -20562,7 +20562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" s="23" t="s">
         <v>981</v>
       </c>
@@ -20615,7 +20615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" s="23" t="s">
         <v>536</v>
       </c>
@@ -20668,7 +20668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A262" s="23" t="s">
         <v>730</v>
       </c>
@@ -20721,7 +20721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" s="23" t="s">
         <v>539</v>
       </c>
@@ -20774,7 +20774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" s="23" t="s">
         <v>731</v>
       </c>
@@ -20827,7 +20827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A265" s="23" t="s">
         <v>542</v>
       </c>
@@ -20880,7 +20880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A266" s="23" t="s">
         <v>732</v>
       </c>
@@ -20933,7 +20933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" s="23" t="s">
         <v>545</v>
       </c>
@@ -20986,7 +20986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A268" s="23" t="s">
         <v>733</v>
       </c>
@@ -21039,7 +21039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A269" s="23" t="s">
         <v>548</v>
       </c>
@@ -21092,7 +21092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A270" s="23" t="s">
         <v>734</v>
       </c>
@@ -21145,7 +21145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A271" s="23" t="s">
         <v>551</v>
       </c>
@@ -21198,7 +21198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A272" s="23" t="s">
         <v>735</v>
       </c>
@@ -21251,7 +21251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A273" s="23" t="s">
         <v>554</v>
       </c>
@@ -21304,7 +21304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A274" s="23" t="s">
         <v>736</v>
       </c>
@@ -21357,7 +21357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A275" s="23" t="s">
         <v>557</v>
       </c>
@@ -21410,7 +21410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A276" s="23" t="s">
         <v>737</v>
       </c>
@@ -21463,7 +21463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A277" s="23" t="s">
         <v>560</v>
       </c>
@@ -21516,7 +21516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A278" s="23" t="s">
         <v>738</v>
       </c>
@@ -21569,7 +21569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A279" s="23" t="s">
         <v>563</v>
       </c>
@@ -21622,7 +21622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A280" s="23" t="s">
         <v>739</v>
       </c>
@@ -21675,7 +21675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A281" s="23" t="s">
         <v>566</v>
       </c>
@@ -21728,7 +21728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A282" s="23" t="s">
         <v>740</v>
       </c>
@@ -21781,7 +21781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A283" s="23" t="s">
         <v>569</v>
       </c>
@@ -21834,7 +21834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A284" s="23" t="s">
         <v>741</v>
       </c>
@@ -21887,7 +21887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A285" s="23" t="s">
         <v>572</v>
       </c>
@@ -21940,7 +21940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A286" s="23" t="s">
         <v>742</v>
       </c>
@@ -21993,7 +21993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" s="23" t="s">
         <v>575</v>
       </c>
@@ -22046,7 +22046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" s="23" t="s">
         <v>743</v>
       </c>
@@ -22099,7 +22099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" s="23" t="s">
         <v>578</v>
       </c>
@@ -22152,7 +22152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A290" s="23" t="s">
         <v>744</v>
       </c>
@@ -22205,7 +22205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" s="23" t="s">
         <v>581</v>
       </c>
@@ -22258,7 +22258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" s="23" t="s">
         <v>745</v>
       </c>
@@ -22311,7 +22311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" s="23" t="s">
         <v>584</v>
       </c>
@@ -22364,7 +22364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" s="23" t="s">
         <v>746</v>
       </c>
@@ -22417,7 +22417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" s="23" t="s">
         <v>587</v>
       </c>
@@ -22470,7 +22470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" s="23" t="s">
         <v>747</v>
       </c>
@@ -22523,7 +22523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A297" s="23" t="s">
         <v>590</v>
       </c>
@@ -22576,7 +22576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A298" s="23" t="s">
         <v>385</v>
       </c>
@@ -22629,7 +22629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A299" s="23" t="s">
         <v>591</v>
       </c>
@@ -22682,7 +22682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A300" s="23" t="s">
         <v>453</v>
       </c>
@@ -22735,7 +22735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A301" s="24" t="s">
         <v>592</v>
       </c>
@@ -22788,7 +22788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A302" s="25" t="s">
         <v>392</v>
       </c>
@@ -22841,7 +22841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A303" s="24" t="s">
         <v>593</v>
       </c>
@@ -22894,7 +22894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A304" s="25" t="s">
         <v>393</v>
       </c>
@@ -22947,7 +22947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" s="25" t="s">
         <v>979</v>
       </c>
@@ -23000,7 +23000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A306" s="24" t="s">
         <v>831</v>
       </c>
@@ -23053,7 +23053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A307" s="25" t="s">
         <v>394</v>
       </c>
@@ -23106,7 +23106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A308" s="24" t="s">
         <v>832</v>
       </c>
@@ -23159,7 +23159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A309" s="25" t="s">
         <v>395</v>
       </c>
@@ -23212,7 +23212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A310" s="25" t="s">
         <v>396</v>
       </c>
@@ -23265,7 +23265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A311" s="25" t="s">
         <v>397</v>
       </c>
@@ -23318,7 +23318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A312" s="25" t="s">
         <v>398</v>
       </c>
@@ -23371,7 +23371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A313" s="25" t="s">
         <v>399</v>
       </c>
@@ -23424,7 +23424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A314" s="24" t="s">
         <v>833</v>
       </c>
@@ -23477,7 +23477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A315" s="24" t="s">
         <v>971</v>
       </c>
@@ -23530,7 +23530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A316" s="24" t="s">
         <v>400</v>
       </c>
@@ -23583,7 +23583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A317" s="24" t="s">
         <v>879</v>
       </c>
@@ -23636,7 +23636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A318" s="24" t="s">
         <v>834</v>
       </c>
@@ -23689,7 +23689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A319" s="24" t="s">
         <v>498</v>
       </c>
@@ -23742,7 +23742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A320" s="24" t="s">
         <v>765</v>
       </c>
@@ -23795,7 +23795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A321" s="24" t="s">
         <v>863</v>
       </c>
@@ -23848,7 +23848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A322" s="24" t="s">
         <v>835</v>
       </c>
@@ -23901,7 +23901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A323" s="24" t="s">
         <v>972</v>
       </c>
@@ -23954,7 +23954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A324" s="24" t="s">
         <v>401</v>
       </c>
@@ -24007,7 +24007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A325" s="24" t="s">
         <v>878</v>
       </c>
@@ -24060,7 +24060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A326" s="24" t="s">
         <v>836</v>
       </c>
@@ -24113,7 +24113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A327" s="24" t="s">
         <v>402</v>
       </c>
@@ -24166,7 +24166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A328" s="24" t="s">
         <v>864</v>
       </c>
@@ -24219,7 +24219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A329" s="24" t="s">
         <v>837</v>
       </c>
@@ -24272,7 +24272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A330" s="24" t="s">
         <v>973</v>
       </c>
@@ -24325,7 +24325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A331" s="24" t="s">
         <v>403</v>
       </c>
@@ -24378,7 +24378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A332" s="24" t="s">
         <v>869</v>
       </c>
@@ -24431,7 +24431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A333" s="24" t="s">
         <v>838</v>
       </c>
@@ -24484,7 +24484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A334" s="24" t="s">
         <v>404</v>
       </c>
@@ -24537,7 +24537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A335" s="24" t="s">
         <v>866</v>
       </c>
@@ -24590,7 +24590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A336" s="24" t="s">
         <v>839</v>
       </c>
@@ -24643,7 +24643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A337" s="24" t="s">
         <v>974</v>
       </c>
@@ -24696,7 +24696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A338" s="24" t="s">
         <v>405</v>
       </c>
@@ -24749,7 +24749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A339" s="24" t="s">
         <v>877</v>
       </c>
@@ -24802,7 +24802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A340" s="24" t="s">
         <v>840</v>
       </c>
@@ -24855,7 +24855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A341" s="24" t="s">
         <v>406</v>
       </c>
@@ -24908,7 +24908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A342" s="24" t="s">
         <v>867</v>
       </c>
@@ -24961,7 +24961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A343" s="24" t="s">
         <v>841</v>
       </c>
@@ -25014,7 +25014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A344" s="24" t="s">
         <v>975</v>
       </c>
@@ -25067,7 +25067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A345" s="24" t="s">
         <v>407</v>
       </c>
@@ -25120,7 +25120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A346" s="24" t="s">
         <v>871</v>
       </c>
@@ -25173,7 +25173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A347" s="24" t="s">
         <v>842</v>
       </c>
@@ -25226,7 +25226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A348" s="24" t="s">
         <v>408</v>
       </c>
@@ -25279,7 +25279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A349" s="24" t="s">
         <v>868</v>
       </c>
@@ -25332,7 +25332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A350" s="24" t="s">
         <v>843</v>
       </c>
@@ -25385,7 +25385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A351" s="24" t="s">
         <v>976</v>
       </c>
@@ -25438,7 +25438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A352" s="24" t="s">
         <v>409</v>
       </c>
@@ -25491,7 +25491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A353" s="24" t="s">
         <v>870</v>
       </c>
@@ -25544,7 +25544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A354" s="24" t="s">
         <v>844</v>
       </c>
@@ -25597,7 +25597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A355" s="24" t="s">
         <v>410</v>
       </c>
@@ -25650,7 +25650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A356" s="24" t="s">
         <v>865</v>
       </c>
@@ -25703,7 +25703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A357" s="13" t="s">
         <v>806</v>
       </c>
@@ -25756,7 +25756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A358" s="13" t="s">
         <v>411</v>
       </c>
@@ -25809,7 +25809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A359" s="13" t="s">
         <v>872</v>
       </c>
@@ -25862,7 +25862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A360" s="13" t="s">
         <v>807</v>
       </c>
@@ -25915,7 +25915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A361" s="13" t="s">
         <v>412</v>
       </c>
@@ -25968,7 +25968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A362" s="13" t="s">
         <v>873</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A363" s="13" t="s">
         <v>808</v>
       </c>
@@ -26074,7 +26074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A364" s="13" t="s">
         <v>413</v>
       </c>
@@ -26127,7 +26127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A365" s="13" t="s">
         <v>809</v>
       </c>
@@ -26180,7 +26180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A366" s="13" t="s">
         <v>414</v>
       </c>
@@ -26233,7 +26233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A367" s="13" t="s">
         <v>874</v>
       </c>
@@ -26286,7 +26286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A368" s="13" t="s">
         <v>810</v>
       </c>
@@ -26339,7 +26339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A369" s="13" t="s">
         <v>415</v>
       </c>
@@ -26392,7 +26392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A370" s="13" t="s">
         <v>811</v>
       </c>
@@ -26445,7 +26445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A371" s="13" t="s">
         <v>492</v>
       </c>
@@ -26498,7 +26498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A372" s="13" t="s">
         <v>875</v>
       </c>
@@ -26551,7 +26551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A373" s="13" t="s">
         <v>813</v>
       </c>
@@ -26604,7 +26604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A374" s="13" t="s">
         <v>815</v>
       </c>
@@ -26657,7 +26657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A375" s="13" t="s">
         <v>817</v>
       </c>
@@ -26710,7 +26710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A376" s="13" t="s">
         <v>416</v>
       </c>
@@ -26763,7 +26763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A377" s="13" t="s">
         <v>977</v>
       </c>
@@ -26816,7 +26816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A378" s="13" t="s">
         <v>819</v>
       </c>
@@ -26869,7 +26869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A379" s="13" t="s">
         <v>417</v>
       </c>
@@ -26922,7 +26922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A380" s="13" t="s">
         <v>820</v>
       </c>
@@ -26975,7 +26975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A381" s="13" t="s">
         <v>418</v>
       </c>
@@ -27028,7 +27028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A382" s="13" t="s">
         <v>821</v>
       </c>
@@ -27081,7 +27081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A383" s="13" t="s">
         <v>419</v>
       </c>
@@ -27134,7 +27134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A384" s="13" t="s">
         <v>822</v>
       </c>
@@ -27187,7 +27187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A385" s="13" t="s">
         <v>420</v>
       </c>
@@ -27240,7 +27240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A386" s="14" t="s">
         <v>823</v>
       </c>
@@ -27293,7 +27293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A387" s="14" t="s">
         <v>421</v>
       </c>
@@ -27346,7 +27346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A388" s="14" t="s">
         <v>824</v>
       </c>
@@ -27399,7 +27399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A389" s="14" t="s">
         <v>422</v>
       </c>
@@ -27452,7 +27452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A390" s="14" t="s">
         <v>825</v>
       </c>
@@ -27505,7 +27505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A391" s="14" t="s">
         <v>423</v>
       </c>
@@ -27558,7 +27558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A392" s="14" t="s">
         <v>826</v>
       </c>
@@ -27611,7 +27611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A393" s="14" t="s">
         <v>424</v>
       </c>
@@ -27664,7 +27664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A394" s="14" t="s">
         <v>827</v>
       </c>
@@ -27717,7 +27717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A395" s="14" t="s">
         <v>425</v>
       </c>
@@ -27770,7 +27770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A396" s="14" t="s">
         <v>876</v>
       </c>
@@ -27823,7 +27823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A397" s="14" t="s">
         <v>828</v>
       </c>
@@ -27876,7 +27876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A398" s="14" t="s">
         <v>426</v>
       </c>
@@ -27929,7 +27929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A399" s="14" t="s">
         <v>829</v>
       </c>
@@ -27982,7 +27982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A400" s="14" t="s">
         <v>427</v>
       </c>
@@ -28035,7 +28035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A401" s="14" t="s">
         <v>830</v>
       </c>
@@ -28088,7 +28088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A402" s="14" t="s">
         <v>428</v>
       </c>
@@ -28141,7 +28141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A403" s="33" t="s">
         <v>860</v>
       </c>
@@ -28194,7 +28194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A404" s="4" t="s">
         <v>489</v>
       </c>
@@ -28247,7 +28247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A405" s="4" t="s">
         <v>522</v>
       </c>
@@ -28300,7 +28300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A406" s="4" t="s">
         <v>25</v>
       </c>
@@ -28353,7 +28353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A407" s="4" t="s">
         <v>429</v>
       </c>
@@ -28406,7 +28406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A408" s="4" t="s">
         <v>528</v>
       </c>
@@ -28461,7 +28461,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q414"/>
-  <conditionalFormatting sqref="C302 C64 C69 M69 C66:C67 M72 C105:C133 K304 K307 C137:C172 M199 C189:C190 C178:C187 K179:K187 C174:C176 K174:K176 P21:P35 M66:M67 P105:P111 K105:K172 K189:K190 K192:K193 K195 K197 P198:P199 P173:P187 K309:K314 C329 K329 K357:K358 C357:C358 K336 C336 C343 K343 K350 C350 K333:K334 C333:C334 C354:C355 K354:K355 K347:K348 C347:C348 C360:C361 K360:K361 K363:K366 C363:C366 K368:K371 K373:K376 C378:C395 K378:K395 K397:K403 C340:C341 K340:K341 C326:C327 K326:K327 C318:C323 K318:K323 M74 C72:D74 C76:D78 M76:M78 M95 P89:P93 O76:O78 O74 O318:O319 O326:O327 O340:O341 O397:O402 O378:O395 O373:O376 O368:O371 O363:O366 O360:O361 O347:O348 O354:O355 O333:O334 O350 O343 O336 O357:O358 O329 O309:O314 O321:O323 O263 O197:P197 O195:P195 O192:P193 O189:P190 O66:P69 O174:O176 O297:O304 O199 O178:O187 O307 O105:O133 O72 O403:P405 O289 O291 O287 O285 O283 O281 O279 O277 O275 O273 O271 O269 O267 O293 O295 O265 O261:P261 C403:D405 C373:C376 C368:C371 K36:K69 O95:P95 O97:P97 M97 Q95:Q97 C100:C101 C95:C97 K100:K101 K96 M96:P96 M100:P100 M36:P64 M261:N302 M318:M319 M326:M327 M340:M341 M397:M405 M378:M395 M373:M376 M368:M371 M363:M366 M360:M361 M347:M348 M354:M355 M333:M334 M350 M343 M336 M357:M358 M329 M309:M314 M321:M323 M197 M195 M192:M193 M189:M190 M137:M172 M174:M176 M178:M187 M307 M304 M105:M133 M316 Q316:Q323 I316:I323 C316 O316 K316 I325:I329 Q325:Q329 Q331:Q336 I331:I336 M331 O331 K331 C331 I338:I343 Q338:Q343 M338 O338 C338 K338 Q345:Q350 I345:I350 M345 O345 K345 C345 Q352:Q405 M352 O352 C352 K352 C304:C314 Q261:Q314 K261:K302 C261:C300 I261:I300 I304:I314 I95:I97 I100:I101 I352:I405 I76:I78 I71:I74 I174:I176 I178:I187 I189:I190 I137:I172 I105:I133 I66:I67 I69 I64 I302 M9:P9 K17:O35 K6:Q6 K9:L10 K5:L5 O10:P10 O5:Q5 K13:P16 K7:P8 K2:Q4 K406:Q408 C406:F408 H406:I408 H2:I2 Q7:Q10 Q100:Q240 K201:P240 E260:F402 C192:C244 G192:I244 K241:Q244 G246:I247 K246:Q259 C246:C259 O137:P172 Q13:Q84 M80:M84 C80:D83 O80:O84 I80:I84 I87:I88 O87:O88 C87:C88 M87:M88 Q87:Q93 E87:F169 H13:I50 E404:F405 E403:H403 E171:F247 E170:H170 C2:F2 C3:I3 C4:F8 H4:I10 C9:C10 E9:F10 D9:D20 C13:F50 H52:I52 C51:C52 E54:F84 H54:I62 C58:D58 C54:C57 E51:I51 E52:F52 D51:D57 C84 E248:I259 C397:C402 D84:D402 C59:C62 C71 D59:D71">
+  <conditionalFormatting sqref="C302 C64 C69 M69 C66:C67 M72 C105:C133 K304 K307 C137:C172 M199 C189:C190 C178:C187 K179:K187 C174:C176 K174:K176 P21:P35 M66:M67 P105:P111 K105:K172 K189:K190 K192:K193 K195 K197 P198:P199 P173:P187 K309:K314 C329 K329 K357:K358 C357:C358 K336 C336 C343 K343 K350 C350 K333:K334 C333:C334 C354:C355 K354:K355 K347:K348 C347:C348 C360:C361 K360:K361 K363:K366 C363:C366 K368:K371 K373:K376 C378:C395 K378:K395 K397:K403 C340:C341 K340:K341 C326:C327 K326:K327 C318:C323 K318:K323 M74 C72:D74 C76:D78 M76:M78 M95 P89:P93 O76:O78 O74 O318:O319 O326:O327 O340:O341 O397:O402 O378:O395 O373:O376 O368:O371 O363:O366 O360:O361 O347:O348 O354:O355 O333:O334 O350 O343 O336 O357:O358 O329 O309:O314 O321:O323 O263 O197:P197 O195:P195 O192:P193 O189:P190 O66:P69 O174:O176 O297:O304 O199 O178:O187 O307 O105:O133 O72 O403:P405 O289 O291 O287 O285 O283 O281 O279 O277 O275 O273 O271 O269 O267 O293 O295 O265 O261:P261 C403:D405 C373:C376 C368:C371 K36:K69 O95:P95 O97:P97 M97 Q95:Q97 C100:C101 C95:C97 K100:K101 K96 M96:P96 M100:P100 M36:P64 M261:N302 M318:M319 M326:M327 M340:M341 M397:M405 M378:M395 M373:M376 M368:M371 M363:M366 M360:M361 M347:M348 M354:M355 M333:M334 M350 M343 M336 M357:M358 M329 M309:M314 M321:M323 M197 M195 M192:M193 M189:M190 M137:M172 M174:M176 M178:M187 M307 M304 M105:M133 M316 Q316:Q323 I316:I323 C316 O316 K316 I325:I329 Q325:Q329 Q331:Q336 I331:I336 M331 O331 K331 C331 I338:I343 Q338:Q343 M338 O338 C338 K338 Q345:Q350 I345:I350 M345 O345 K345 C345 Q352:Q405 M352 O352 C352 K352 C304:C314 Q261:Q314 K261:K302 C261:C300 I261:I300 I304:I314 I95:I97 I100:I101 I352:I405 I76:I78 I71:I74 I174:I176 I178:I187 I189:I190 I137:I172 I105:I133 I66:I67 I69 I64 I302 M9:P9 K17:O35 K6:Q6 K9:L10 K5:L5 O10:P10 O5:Q5 K13:P16 K7:P8 K2:Q4 K406:Q408 C406:F408 H406:I408 H2:I2 Q7:Q10 Q100:Q240 K201:P240 E260:F402 C192:C244 G192:I244 K241:Q244 G246:I247 K246:Q259 C246:C259 O137:P172 Q13:Q84 M80:M84 C80:D83 O80:O84 I80:I84 I87:I88 O87:O88 C87:C88 M87:M88 Q87:Q93 E87:F169 E404:F405 E403:H403 E171:F247 E170:H170 C2:F2 C3:I3 C4:F8 H4:I10 C9:C10 E9:F10 D9:D20 H52:I52 C51:C52 E54:F84 H54:I62 C58:D58 C54:C57 E51:I51 E52:F52 D51:D57 C84 E248:I259 C397:C402 D84:D402 C59:C62 C71 D59:D71 C13:F50 H13:I50">
     <cfRule type="cellIs" dxfId="327" priority="394" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -30114,7 +30114,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>